<commit_message>
closed form Johnson put value
</commit_message>
<xml_diff>
--- a/xll_johnson/johnson.xlsx
+++ b/xll_johnson/johnson.xlsx
@@ -8,30 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\keithalewis\fms_johnson\xll_johnson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB2E446-E1A1-481E-B582-BAF27D3B1BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1429413-1496-455F-B121-CC976933529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{04679C06-6483-44F4-8D12-E76B362C6884}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{04679C06-6483-44F4-8D12-E76B362C6884}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="cdf">_xlfn.ANCHORARRAY(Sheet1!$J$3)</definedName>
-    <definedName name="delta">Sheet1!$C$3</definedName>
-    <definedName name="gamma">Sheet1!$C$2</definedName>
-    <definedName name="Johnson">Sheet1!$C$6</definedName>
-    <definedName name="lambda">Sheet1!$C$5</definedName>
-    <definedName name="mu">Sheet1!$C$12</definedName>
+    <definedName name="delta" localSheetId="1">Sheet2!$C$3</definedName>
+    <definedName name="delta">Sheet1!$C$4</definedName>
+    <definedName name="f">Sheet2!$C$9</definedName>
+    <definedName name="gamma" localSheetId="1">Sheet2!$C$2</definedName>
+    <definedName name="gamma">Sheet1!$C$3</definedName>
+    <definedName name="implied">Sheet2!$C$14</definedName>
+    <definedName name="Johnson" localSheetId="1">Sheet2!$C$6</definedName>
+    <definedName name="Johnson">Sheet1!$C$7</definedName>
+    <definedName name="k">Sheet2!$C$11</definedName>
+    <definedName name="lambda" localSheetId="1">Sheet2!$C$5</definedName>
+    <definedName name="lambda">Sheet1!$C$6</definedName>
+    <definedName name="mu">Sheet1!$C$13</definedName>
     <definedName name="ncdf">_xlfn.ANCHORARRAY(Sheet1!$L$3)</definedName>
-    <definedName name="Normal">Sheet1!$C$14</definedName>
+    <definedName name="Normal">Sheet1!$C$15</definedName>
     <definedName name="npdf">_xlfn.ANCHORARRAY(Sheet1!$K$3)</definedName>
     <definedName name="pdf">_xlfn.ANCHORARRAY(Sheet1!$I$3)</definedName>
-    <definedName name="sigma">Sheet1!$C$13</definedName>
+    <definedName name="s" localSheetId="1">Sheet2!$C$10</definedName>
+    <definedName name="s">Sheet1!$C$2</definedName>
+    <definedName name="sigma">Sheet1!$C$14</definedName>
+    <definedName name="value">Sheet2!$C$12</definedName>
     <definedName name="x">_xlfn.ANCHORARRAY(Sheet1!$H$3)</definedName>
-    <definedName name="xi">Sheet1!$C$4</definedName>
-    <definedName name="Z">Sheet1!$C$20</definedName>
+    <definedName name="xi" localSheetId="1">Sheet2!$C$4</definedName>
+    <definedName name="xi">Sheet1!$C$5</definedName>
+    <definedName name="Z">Sheet1!$C$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>xi</t>
   </si>
@@ -129,13 +142,41 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>put_value</t>
+  </si>
+  <si>
+    <t>put_delta</t>
+  </si>
+  <si>
+    <t>put_implied</t>
+  </si>
+  <si>
+    <t>johnson_put_value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -211,7 +252,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -223,6 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -730,307 +772,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.5399836433269091E-4</c:v>
+                  <c:v>2.7945408264877118E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1211821774760813E-4</c:v>
+                  <c:v>3.1839727400048375E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7852629168763541E-4</c:v>
+                  <c:v>3.632998017687571E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5452935795671087E-4</c:v>
+                  <c:v>4.1515869297340332E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4166034456623633E-4</c:v>
+                  <c:v>4.7515248884680305E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4172099301256791E-4</c:v>
+                  <c:v>5.4467702104806913E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5683322055249427E-4</c:v>
+                  <c:v>6.2538877917287341E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0895010941344631E-3</c:v>
+                  <c:v>7.1925759255649568E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2426857667214234E-3</c:v>
+                  <c:v>8.2863076445332726E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4198962794959649E-3</c:v>
+                  <c:v>9.5631131683989639E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.625299822335634E-3</c:v>
+                  <c:v>1.1056536568830638E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8638559044121114E-3</c:v>
+                  <c:v>1.2806807964020411E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1414799598519774E-3</c:v>
+                  <c:v>1.4862282874762718E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4652432537375711E-3</c:v>
+                  <c:v>1.7281213362173133E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.843617627810908E-3</c:v>
+                  <c:v>2.0133931923232711E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2867757148734374E-3</c:v>
+                  <c:v>2.3505549713937267E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.8069598556386285E-3</c:v>
+                  <c:v>2.7499296579260404E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.418936191114802E-3</c:v>
+                  <c:v>3.2240662915544159E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1405544175295729E-3</c:v>
+                  <c:v>3.7882544167237753E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9934386381301956E-3</c:v>
+                  <c:v>4.4611639641612428E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.0038407971688699E-3</c:v>
+                  <c:v>5.2656420440718964E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.2036955008012603E-3</c:v>
+                  <c:v>6.2297058931908567E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.6319237426882517E-3</c:v>
+                  <c:v>7.3877806466644868E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1336043180833468E-2</c:v>
+                  <c:v>8.7822418540801448E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3374153962431681E-2</c:v>
+                  <c:v>1.0465335719336001E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5817381060070058E-2</c:v>
+                  <c:v>1.2501564574641506E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.8752865321856195E-2</c:v>
+                  <c:v>1.4970640122302065E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2287403328615518E-2</c:v>
+                  <c:v>1.7971120372145401E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.6551835924275985E-2</c:v>
+                  <c:v>2.162485386135931E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1706268651791748E-2</c:v>
+                  <c:v>2.6082349222530603E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.7946160369435343E-2</c:v>
+                  <c:v>3.1529156554821171E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.5509216377232126E-2</c:v>
+                  <c:v>3.8193267748764997E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.4682833672723648E-2</c:v>
+                  <c:v>4.635338095207199E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.5811514016871256E-2</c:v>
+                  <c:v>5.6347575173483537E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.9303106330023757E-2</c:v>
+                  <c:v>6.8581423232842151E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.5631856999947168E-2</c:v>
+                  <c:v>8.3533721173020117E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.11533490846887444</c:v>
+                  <c:v>0.10175668714524692</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.13899698174264619</c:v>
+                  <c:v>0.12386553954620814</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.16721550635297847</c:v>
+                  <c:v>0.1505097457110279</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.20053573830560054</c:v>
+                  <c:v>0.18231516708719597</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.23934344697746879</c:v>
+                  <c:v>0.21978371233224786</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.28370383266135807</c:v>
+                  <c:v>0.26313711634201442</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.33314353279466052</c:v>
+                  <c:v>0.31209818271004786</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.38639348936483231</c:v>
+                  <c:v>0.36562223394466031</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.44114844502398848</c:v>
+                  <c:v>0.42162902038545386</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.49394968253813593</c:v>
+                  <c:v>0.47683859327233863</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.54033731014439135</c:v>
+                  <c:v>0.52686165134711072</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.57539832144528535</c:v>
+                  <c:v>0.56668689277319728</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.59470715122605933</c:v>
+                  <c:v>0.59158980722526067</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.59542882121551766</c:v>
+                  <c:v>0.59826048564870093</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.57715962684987532</c:v>
+                  <c:v>0.58573254518205409</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.54210271839214386</c:v>
+                  <c:v>0.55568406301801265</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.49447256967407777</c:v>
+                  <c:v>0.51195466625293107</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.43940566781679591</c:v>
+                  <c:v>0.45951310375493226</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.38184618915061219</c:v>
+                  <c:v>0.40333290231099084</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.32577559423885932</c:v>
+                  <c:v>0.34756551619886417</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.27390284321552266</c:v>
+                  <c:v>0.29516008101077751</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.22772309026885401</c:v>
+                  <c:v>0.24786265305354699</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.18777406465475951</c:v>
+                  <c:v>0.20643464151232535</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.15394269159729695</c:v>
+                  <c:v>0.17094208255481272</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.12573535723614146</c:v>
+                  <c:v>0.14102310732675341</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.10247924379988503</c:v>
+                  <c:v>0.11609451902596506</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.3454771452459969E-2</c:v>
+                  <c:v>9.5492644712746544E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.7973055423371204E-2</c:v>
+                  <c:v>7.8559459413378926E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.5414890241784878E-2</c:v>
+                  <c:v>6.4689101103908325E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.5245345804669039E-2</c:v>
+                  <c:v>5.3348411896260793E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.7014277081999572E-2</c:v>
+                  <c:v>4.4081848771799527E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.0349578854128156E-2</c:v>
+                  <c:v>3.6507840328979774E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.4947380161910032E-2</c:v>
+                  <c:v>3.0311076692013831E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.0561569352483568E-2</c:v>
+                  <c:v>2.5233391274780408E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.6993892996149909E-2</c:v>
+                  <c:v>2.1064695581679397E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.4085184456303192E-2</c:v>
+                  <c:v>1.7634688453057518E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.1707890250092369E-2</c:v>
+                  <c:v>1.4805628237730175E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.7598597336093773E-3</c:v>
+                  <c:v>1.2466218036361576E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>8.1592698982939811E-3</c:v>
+                  <c:v>1.0526533731672923E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.8405242152831357E-3</c:v>
+                  <c:v>8.9138724753217869E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.7509635581052959E-3</c:v>
+                  <c:v>7.5693849518498517E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.8482414581218526E-3</c:v>
+                  <c:v>6.4453597493496573E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.0982359455794416E-3</c:v>
+                  <c:v>5.5030419650537775E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3.4733910783840906E-3</c:v>
+                  <c:v>4.7108849258413223E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2.9514005876051532E-3</c:v>
+                  <c:v>4.043150573963262E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.5141629147183366E-3</c:v>
+                  <c:v>3.4787892306154138E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.1469510690586085E-3</c:v>
+                  <c:v>3.0005425676843875E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.8377523482641029E-3</c:v>
+                  <c:v>2.5942246219057556E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.5767423466555525E-3</c:v>
+                  <c:v>2.2481447322403158E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.3558651751259989E-3</c:v>
+                  <c:v>1.9526436183371142E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.1684977660526561E-3</c:v>
+                  <c:v>1.6997197136385473E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.0091808349999151E-3</c:v>
+                  <c:v>1.4827275743613338E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>8.7340276935282755E-4</c:v>
+                  <c:v>1.2961339288959828E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>7.574256199980884E-4</c:v>
+                  <c:v>1.1353199007592327E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6.5814465358202286E-4</c:v>
+                  <c:v>9.9642028890174761E-4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.7297471375401332E-4</c:v>
+                  <c:v>8.7619264935989358E-4</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.9975804626297467E-4</c:v>
+                  <c:v>7.7191039433856864E-4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.3668934832442088E-4</c:v>
+                  <c:v>6.8127529043126569E-4</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>3.8225467277555944E-4</c:v>
+                  <c:v>6.0234566151115142E-4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.3518150336470754E-4</c:v>
+                  <c:v>5.3347733494850847E-4</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.943978590340524E-4</c:v>
+                  <c:v>4.7327495247416327E-4</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.5899871342338073E-4</c:v>
+                  <c:v>4.2055173088343908E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.2821835536683484E-4</c:v>
+                  <c:v>3.7429612776366692E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0140758585771506E-4</c:v>
+                  <c:v>3.3364416311326613E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.7801486164813004E-4</c:v>
+                  <c:v>2.9785638450960893E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2044,307 +2086,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.0249846724529077E-8</c:v>
+                  <c:v>2.4129955889966093E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8027052671946424E-8</c:v>
+                  <c:v>4.7431684654640798E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4917468310943208E-7</c:v>
+                  <c:v>9.1949531688809475E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.812639004358628E-7</c:v>
+                  <c:v>1.7579213595838451E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2300015296346179E-7</c:v>
+                  <c:v>3.3145022194775128E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5908828542361814E-7</c:v>
+                  <c:v>6.1631982102863674E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7345399488046493E-6</c:v>
+                  <c:v>1.1302197849724961E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0937055515946621E-6</c:v>
+                  <c:v>2.0440364018191555E-6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4418002509752153E-6</c:v>
+                  <c:v>3.6457198742106871E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.4400689359710921E-6</c:v>
+                  <c:v>6.4127884815149315E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6150154630179564E-5</c:v>
+                  <c:v>1.1124473987528957E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.724878571889414E-5</c:v>
+                  <c:v>1.9031849904549581E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5340527891044492E-5</c:v>
+                  <c:v>3.2110825670618461E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.4403769813059637E-5</c:v>
+                  <c:v>5.3430703369420841E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2041268996905009E-4</c:v>
+                  <c:v>8.7679741268153059E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9218457433291009E-4</c:v>
+                  <c:v>1.4189809909383787E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0250582624115281E-4</c:v>
+                  <c:v>2.2647634381399296E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.6958899518251198E-4</c:v>
+                  <c:v>3.5648237506747424E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.189042109841952E-4</c:v>
+                  <c:v>5.5337843369258552E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0854081895048198E-3</c:v>
+                  <c:v>8.4717932134422715E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.6161590940232241E-3</c:v>
+                  <c:v>1.2790791308723813E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3732532063109467E-3</c:v>
+                  <c:v>1.9045326811821897E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.4369482416631019E-3</c:v>
+                  <c:v>2.7967161827415145E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.9087493569254593E-3</c:v>
+                  <c:v>4.0502078501963232E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.9141320948501372E-3</c:v>
+                  <c:v>5.7846245512400349E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.6044707297148531E-3</c:v>
+                  <c:v>8.1478306098394133E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.3157644610931496E-2</c:v>
+                  <c:v>1.1318210229330824E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.7776727540917244E-2</c:v>
+                  <c:v>1.5505382026789284E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3686147538921953E-2</c:v>
+                  <c:v>2.0948654554711729E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1124758746852912E-2</c:v>
+                  <c:v>2.7912500845991409E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.0335412919497708E-2</c:v>
+                  <c:v>3.667839412995362E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.1550866592650089E-2</c:v>
+                  <c:v>4.7532518548608807E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.4976211112027962E-2</c:v>
+                  <c:v>6.0749161720556701E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.0768449477460272E-2</c:v>
+                  <c:v>7.6570009734742317E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.9014331126980507E-2</c:v>
+                  <c:v>9.518007986163346E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.11970803997794603</c:v>
+                  <c:v>0.11668160036602157</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.14273074468823588</c:v>
+                  <c:v>0.14106771739328908</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.16783428900627631</c:v>
+                  <c:v>0.16819839635435682</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.1946313541389823</c:v>
+                  <c:v>0.19778120212145192</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.22259421080404848</c:v>
+                  <c:v>0.2293597060532393</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.25106367154362719</c:v>
+                  <c:v>0.26231201537401122</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.27926906815860497</c:v>
+                  <c:v>0.29586132286154604</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.30635907240424409</c:v>
+                  <c:v>0.32909944888366083</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.33144204934714083</c:v>
+                  <c:v>0.361023161474819</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.35363351273308435</c:v>
+                  <c:v>0.39058173000049884</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.37210728633127754</c:v>
+                  <c:v>0.41673284805446192</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.38614630456966198</c:v>
+                  <c:v>0.43850292359506593</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.39518872151042966</c:v>
+                  <c:v>0.45504694401087509</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.39886520272982412</c:v>
+                  <c:v>0.46570281238686317</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.39702395178508854</c:v>
+                  <c:v>0.47003529342785944</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.38974110802513773</c:v>
+                  <c:v>0.46786550543392069</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.37731552318190265</c:v>
+                  <c:v>0.45928317340728742</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.36024841612372832</c:v>
+                  <c:v>0.44464047362342363</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.33920983599314536</c:v>
+                  <c:v>0.42452805815285793</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.31499506041750763</c:v>
+                  <c:v>0.39973553396848466</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.28847487892577062</c:v>
+                  <c:v>0.37120008122633552</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.26054407761647447</c:v>
+                  <c:v>0.33994786568104446</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.23207232939372091</c:v>
+                  <c:v>0.30703333139918837</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.20386114863355567</c:v>
+                  <c:v>0.27348132826957205</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.17660968747111744</c:v>
+                  <c:v>0.2402363860289409</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.15089106605067718</c:v>
+                  <c:v>0.20812240753154615</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.1271397875585551</c:v>
+                  <c:v>0.17781477557172073</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.10564972858903163</c:v>
+                  <c:v>0.14982552236305358</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>8.6581327377994829E-2</c:v>
+                  <c:v>0.12450096132240532</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.9975988703070452E-2</c:v>
+                  <c:v>0.10203015791040425</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5.5775413262316602E-2</c:v>
+                  <c:v>8.2461904818584827E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.3843528634727978E-2</c:v>
+                  <c:v>6.5727500316870441E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.3988903389060465E-2</c:v>
+                  <c:v>5.16665923868425E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.5985899553835238E-2</c:v>
+                  <c:v>4.0053592212178295E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.9593287345387095E-2</c:v>
+                  <c:v>3.0622600914242487E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.4569538978236743E-2</c:v>
+                  <c:v>2.3089345732782745E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.0684476824571722E-2</c:v>
+                  <c:v>1.7169202732841192E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7.7273336186864392E-3</c:v>
+                  <c:v>1.2590923362052458E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5.5115660199926931E-3</c:v>
+                  <c:v>9.106132848932677E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3.8769420973590535E-3</c:v>
+                  <c:v>6.4950026568476515E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2.6895062966261762E-3</c:v>
+                  <c:v>4.568710441179645E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.8400294145894814E-3</c:v>
+                  <c:v>3.1693987659461372E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.241497689572178E-3</c:v>
+                  <c:v>2.168348504415149E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>8.2610645449592067E-4</c:v>
+                  <c:v>1.463019904504783E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.4211954457831233E-4</c:v>
+                  <c:v>9.7350981505563302E-4</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>3.5085127892498511E-4</c:v>
+                  <c:v>6.3885071313540126E-4</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.2393398716512202E-4</c:v>
+                  <c:v>4.1345417627405937E-4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.4095676091077988E-4</c:v>
+                  <c:v>2.6389084995445336E-4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>8.7502560127317714E-5</c:v>
+                  <c:v>1.6610787810491804E-4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.3570359110430774E-5</c:v>
+                  <c:v>1.0311576754162756E-4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>3.2344266403547226E-5</c:v>
+                  <c:v>6.3128995187286524E-5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.92592336877485E-5</c:v>
+                  <c:v>3.8115500288447229E-5</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.1309662629486974E-5</c:v>
+                  <c:v>2.2695686401474357E-5</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.5498182178739744E-6</c:v>
+                  <c:v>1.3327661967599159E-5</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>3.7409145954420133E-6</c:v>
+                  <c:v>7.7185116848182121E-6</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.1071492103023972E-6</c:v>
+                  <c:v>4.4084113568267356E-6</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.1705278083347855E-6</c:v>
+                  <c:v>2.4831308687302349E-6</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>6.4126440127278319E-7</c:v>
+                  <c:v>1.3793867654802345E-6</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>3.4646668191963948E-7</c:v>
+                  <c:v>7.5568612893329128E-7</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.8460980860359997E-7</c:v>
+                  <c:v>4.0828722933091742E-7</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>9.7010114438558822E-8</c:v>
+                  <c:v>2.1755000176195073E-7</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5.0274552257759479E-8</c:v>
+                  <c:v>1.1431976841681189E-7</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.5694984247864265E-8</c:v>
+                  <c:v>5.9245112786729675E-8</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.2951421863969333E-8</c:v>
+                  <c:v>3.0279777172615305E-8</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.4380670222978091E-9</c:v>
+                  <c:v>1.5262362659051862E-8</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>3.1561852577758855E-9</c:v>
+                  <c:v>7.5868205629954428E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2701,307 +2743,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
+                  <c:v>3.437040041465167E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.8888383886189786E-9</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.3621834660249021E-8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2.6574140887802855E-8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5.1147335033974173E-8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>9.7125529341379746E-8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.8196891743427202E-7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3.3637339674763567E-7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>6.1349960017720306E-7</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.1040358424141417E-6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1.9603643926502379E-6</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3.4346633864257292E-6</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>5.9379267369208399E-6</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1.0129753677645681E-5</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1.7052461216082726E-5</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2.8327666707850252E-5</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>4.6438932026160451E-5</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>7.5130149028268534E-5</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>1.199556345671815E-4</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1.8902363669015543E-4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2.9397900284716671E-4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>4.5127159502306169E-4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>6.837527541089794E-4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1.0226305623681764E-3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1.5097936510474752E-3</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2.200481002527066E-3</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>3.1662305551806158E-3</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>4.4979827366486425E-3</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>6.3091485395969649E-3</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>8.738379999018886E-3</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1.1951711127894171E-2</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>1.6143679195266492E-2</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>2.1537001230033159E-2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2.8380381049400383E-2</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>3.6944069202113072E-2</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>4.7512900186882034E-2</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>6.0376691115162584E-2</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>7.5818099411116724E-2</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>9.4098291512360543E-2</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>0.11544104856560938</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>0.1400162001061811</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>0.1679234992663976</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>0.19917819908999618</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>0.23369962916910997</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>0.27130398448337512</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>0.31170231708788843</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>0.35450437574156468</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>0.39922849533890892</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>0.4453172388022601</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>0.49215799108738634</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>0.5391072542633486</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>0.58551704670180216</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>0.6307616096276677</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>0.67426259492032903</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>0.71551105270225679</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>0.75408483827835626</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>0.78966047915550108</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
                   <c:v>0.82201903463938053</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>0.8510459871231203</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>0.87672567135600432</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>0.89913112989631394</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>0.91841054758371254</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="62">
                   <c:v>0.93477154988264299</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="63">
                   <c:v>0.9484646509808301</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="64">
                   <c:v>0.95976702402819636</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="65">
                   <c:v>0.96896756518996463</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="66">
                   <c:v>0.97635396851130229</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="67">
                   <c:v>0.98220225408289652</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="68">
                   <c:v>0.9867689282952028</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="69">
                   <c:v>0.9902857260411948</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="70">
                   <c:v>0.99295670616128739</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="71">
                   <c:v>0.99495735016618658</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="72">
                   <c:v>0.99643524956985763</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="73">
                   <c:v>0.99751195232230505</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="74">
                   <c:v>0.99828556336816709</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="75">
                   <c:v>0.9988337461459853</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="76">
                   <c:v>0.99921683895094049</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="77">
                   <c:v>0.99948087211676628</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="78">
                   <c:v>0.99966034087037814</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="79">
                   <c:v>0.9997806490298029</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="80">
                   <c:v>0.99986018749144967</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="81">
                   <c:v>0.99991204780711773</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="82">
                   <c:v>0.9999453957451081</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="83">
                   <c:v>0.99996654420133968</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="84">
                   <c:v>0.99997977128828142</c:v>
                 </c:pt>
-                <c:pt idx="84">
+                <c:pt idx="85">
                   <c:v>0.99998793007523878</c:v>
                 </c:pt>
-                <c:pt idx="85">
+                <c:pt idx="86">
                   <c:v>0.99999289328717444</c:v>
                 </c:pt>
-                <c:pt idx="86">
+                <c:pt idx="87">
                   <c:v>0.99999587095251719</c:v>
                 </c:pt>
-                <c:pt idx="87">
+                <c:pt idx="88">
                   <c:v>0.99999763278569898</c:v>
                 </c:pt>
-                <c:pt idx="88">
+                <c:pt idx="89">
                   <c:v>0.99999866087185763</c:v>
                 </c:pt>
-                <c:pt idx="89">
+                <c:pt idx="90">
                   <c:v>0.99999925252893296</c:v>
                 </c:pt>
-                <c:pt idx="90">
+                <c:pt idx="91">
                   <c:v>0.99999958833337033</c:v>
                 </c:pt>
-                <c:pt idx="91">
+                <c:pt idx="92">
                   <c:v>0.99999977629907244</c:v>
                 </c:pt>
-                <c:pt idx="92">
+                <c:pt idx="93">
                   <c:v>0.99999988006304719</c:v>
                 </c:pt>
-                <c:pt idx="93">
+                <c:pt idx="94">
                   <c:v>0.99999993655549446</c:v>
                 </c:pt>
-                <c:pt idx="94">
+                <c:pt idx="95">
                   <c:v>0.99999996688811787</c:v>
                 </c:pt>
-                <c:pt idx="95">
+                <c:pt idx="96">
                   <c:v>0.99999998295032966</c:v>
                 </c:pt>
-                <c:pt idx="96">
+                <c:pt idx="97">
                   <c:v>0.99999999133867901</c:v>
                 </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="98">
                   <c:v>0.99999999565907394</c:v>
                 </c:pt>
-                <c:pt idx="98">
+                <c:pt idx="99">
                   <c:v>0.99999999785362736</c:v>
                 </c:pt>
-                <c:pt idx="99">
+                <c:pt idx="100">
                   <c:v>0.99999999895299929</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.99999999949614815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4147,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F0A76B-08E5-40E0-BCFA-A9D795A3DB2C}">
   <dimension ref="B1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -4162,17 +4204,17 @@
   <sheetData>
     <row r="1" spans="2:12" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I1" s="3">
-        <f>1-SUM(pdf)*D16</f>
-        <v>5.4997005830159651E-4</v>
+        <f>1-SUM(pdf)*D17</f>
+        <v>5.0550260541992742E-4</v>
       </c>
       <c r="K1" s="3">
-        <f>1-SUM(npdf)*D16</f>
-        <v>0.1514143591668492</v>
+        <f>1-SUM(npdf)*D17</f>
+        <v>3.0788288585270607E-9</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>0.1</v>
@@ -4195,352 +4237,358 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="H3" cm="1">
-        <f t="array" ref="H3:H103">_xlfn.SEQUENCE(1+(C16-B16)/D16,1,B16,D16)</f>
+        <f t="array" ref="H3:H103">_xlfn.SEQUENCE(1+(C17-B17)/D17,1,B17,D17)</f>
         <v>-5</v>
       </c>
       <c r="I3" cm="1">
-        <f t="array" ref="I3:I103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Johnson,_xlpm.x)))</f>
-        <v>4.5399836433269091E-4</v>
+        <f t="array" ref="I3:I103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Johnson,_xlpm.x,s)))</f>
+        <v>2.7945408264877118E-4</v>
       </c>
       <c r="J3" cm="1">
-        <f t="array" ref="J3:J103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Johnson,_xlpm.x)))</f>
+        <f t="array" ref="J3:J103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Johnson,_xlpm.x,s)))</f>
         <v>4.2047300610986715E-4</v>
       </c>
       <c r="K3" cm="1">
-        <f t="array" ref="K3:K103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Normal,_xlpm.x)))</f>
-        <v>4.0249846724529077E-8</v>
+        <f t="array" ref="K3:K103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Normal,_xlpm.x,s)))</f>
+        <v>2.4129955889966093E-8</v>
       </c>
       <c r="L3" cm="1">
-        <f t="array" ref="L3:L103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Normal,_xlpm.x)))</f>
-        <v>6.8888383886189786E-9</v>
+        <f t="array" ref="L3:L103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Normal,_xlpm.x,s)))</f>
+        <v>3.437040041465167E-9</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>-0.1</v>
+        <v>1.5</v>
       </c>
       <c r="H4">
         <v>-4.9000000000000004</v>
       </c>
       <c r="I4">
-        <v>5.1211821774760813E-4</v>
+        <v>3.1839727400048375E-4</v>
       </c>
       <c r="J4">
         <v>4.6871468417442053E-4</v>
       </c>
       <c r="K4">
-        <v>7.8027052671946424E-8</v>
+        <v>4.7431684654640798E-8</v>
       </c>
       <c r="L4">
-        <v>1.3621834660249021E-8</v>
+        <v>6.8888383886189786E-9</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>-0.1</v>
       </c>
       <c r="H5">
         <v>-4.8000000000000007</v>
       </c>
       <c r="I5">
-        <v>5.7852629168763541E-4</v>
+        <v>3.632998017687571E-4</v>
       </c>
       <c r="J5">
         <v>5.2317271261348441E-4</v>
       </c>
       <c r="K5">
-        <v>1.4917468310943208E-7</v>
+        <v>9.1949531688809475E-8</v>
       </c>
       <c r="L5">
-        <v>2.6574140887802855E-8</v>
+        <v>1.3621834660249021E-8</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" cm="1">
-        <f t="array" ref="C6">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
-        <v>2600763039440</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
       <c r="H6">
         <v>-4.7000000000000011</v>
       </c>
       <c r="I6">
-        <v>6.5452935795671087E-4</v>
+        <v>4.1515869297340332E-4</v>
       </c>
       <c r="J6">
         <v>5.8473952524562556E-4</v>
       </c>
       <c r="K6">
-        <v>2.812639004358628E-7</v>
+        <v>1.7579213595838451E-7</v>
       </c>
       <c r="L6">
-        <v>5.1147335033974173E-8</v>
+        <v>2.6574140887802855E-8</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" cm="1">
+        <f t="array" ref="C7">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
+        <v>1815201892864</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="H7">
         <v>-4.6000000000000014</v>
       </c>
       <c r="I7">
-        <v>7.4166034456623633E-4</v>
+        <v>4.7515248884680305E-4</v>
       </c>
       <c r="J7">
         <v>6.5444921734547634E-4</v>
       </c>
       <c r="K7">
-        <v>5.2300015296346179E-7</v>
+        <v>3.3145022194775128E-7</v>
       </c>
       <c r="L7">
-        <v>9.7125529341379746E-8</v>
+        <v>5.1147335033974173E-8</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" cm="1">
-        <f t="array" ref="C8">_xll.JOHNSON.MOMENT(Johnson,B8)</f>
-        <v>-0.18331827652210433</v>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="H8">
         <v>-4.5000000000000018</v>
       </c>
       <c r="I8">
-        <v>8.4172099301256791E-4</v>
+        <v>5.4467702104806913E-4</v>
       </c>
       <c r="J8">
         <v>7.3350222853063585E-4</v>
       </c>
       <c r="K8">
-        <v>9.5908828542361814E-7</v>
+        <v>6.1631982102863674E-7</v>
       </c>
       <c r="L8">
-        <v>1.8196891743427202E-7</v>
+        <v>9.7125529341379746E-8</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" cm="1">
         <f t="array" ref="C9">_xll.JOHNSON.MOMENT(Johnson,B9)</f>
-        <v>0.753703187708885</v>
+        <v>-0.18331827652210433</v>
       </c>
       <c r="H9">
         <v>-4.4000000000000021</v>
       </c>
       <c r="I9">
-        <v>9.5683322055249427E-4</v>
+        <v>6.2538877917287341E-4</v>
       </c>
       <c r="J9">
         <v>8.2329471234382501E-4</v>
       </c>
       <c r="K9">
-        <v>1.7345399488046493E-6</v>
+        <v>1.1302197849724961E-6</v>
       </c>
       <c r="L9">
-        <v>3.3637339674763567E-7</v>
+        <v>1.8196891743427202E-7</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" cm="1">
         <f t="array" ref="C10">_xll.JOHNSON.MOMENT(Johnson,B10)</f>
-        <v>-0.53104345500307115</v>
+        <v>0.753703187708885</v>
       </c>
       <c r="H10">
         <v>-4.3000000000000025</v>
       </c>
       <c r="I10">
-        <v>1.0895010941344631E-3</v>
+        <v>7.1925759255649568E-4</v>
       </c>
       <c r="J10">
         <v>9.2545355505402327E-4</v>
       </c>
       <c r="K10">
-        <v>3.0937055515946621E-6</v>
+        <v>2.0440364018191555E-6</v>
       </c>
       <c r="L10">
-        <v>6.1349960017720306E-7</v>
+        <v>3.3637339674763567E-7</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" cm="1">
         <f t="array" ref="C11">_xll.JOHNSON.MOMENT(Johnson,B11)</f>
-        <v>3.8482088381788087</v>
+        <v>-0.53104345500307115</v>
       </c>
       <c r="H11">
         <v>-4.2000000000000028</v>
       </c>
       <c r="I11">
-        <v>1.2426857667214234E-3</v>
+        <v>8.2863076445332726E-4</v>
       </c>
       <c r="J11">
         <v>1.0418782182627373E-3</v>
       </c>
       <c r="K11">
-        <v>5.4418002509752153E-6</v>
+        <v>3.6457198742106871E-6</v>
       </c>
       <c r="L11">
-        <v>1.1040358424141417E-6</v>
+        <v>6.1349960017720306E-7</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <f>C8</f>
-        <v>-0.18331827652210433</v>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" cm="1">
+        <f t="array" ref="C12">_xll.JOHNSON.MOMENT(Johnson,B12)</f>
+        <v>3.8482088381788087</v>
       </c>
       <c r="H12">
         <v>-4.1000000000000032</v>
       </c>
       <c r="I12">
-        <v>1.4198962794959649E-3</v>
+        <v>9.5631131683989639E-4</v>
       </c>
       <c r="J12">
         <v>1.1747908416026576E-3</v>
       </c>
       <c r="K12">
-        <v>9.4400689359710921E-6</v>
+        <v>6.4127884815149315E-6</v>
       </c>
       <c r="L12">
-        <v>1.9603643926502379E-6</v>
+        <v>1.1040358424141417E-6</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <f>SQRT(C9-C8^2)</f>
-        <v>0.84858564517781598</v>
+        <f>C9</f>
+        <v>-0.18331827652210433</v>
       </c>
       <c r="H13">
         <v>-4.0000000000000036</v>
       </c>
       <c r="I13">
-        <v>1.625299822335634E-3</v>
+        <v>1.1056536568830638E-3</v>
       </c>
       <c r="J13">
         <v>1.3267963653426085E-3</v>
       </c>
       <c r="K13">
-        <v>1.6150154630179564E-5</v>
+        <v>1.1124473987528957E-5</v>
       </c>
       <c r="L13">
-        <v>3.4346633864257292E-6</v>
+        <v>1.9603643926502379E-6</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" cm="1">
-        <f t="array" ref="C14">_xll.\VARIATE.NORMAL(mu, sigma)</f>
-        <v>2601613569904</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f>SQRT(C10-C9^2)</f>
+        <v>0.84858564517781598</v>
+      </c>
       <c r="H14">
         <v>-3.9000000000000035</v>
       </c>
       <c r="I14">
-        <v>1.8638559044121114E-3</v>
+        <v>1.2806807964020411E-3</v>
       </c>
       <c r="J14">
         <v>1.5009548333401734E-3</v>
       </c>
       <c r="K14">
-        <v>2.724878571889414E-5</v>
+        <v>1.9031849904549581E-5</v>
       </c>
       <c r="L14">
-        <v>5.9379267369208399E-6</v>
+        <v>3.4346633864257292E-6</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" cm="1">
+        <f t="array" ref="C15">_xll.\VARIATE.NORMAL(mu, sigma)</f>
+        <v>1815687643184</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="H15">
         <v>-3.8000000000000034</v>
       </c>
       <c r="I15">
-        <v>2.1414799598519774E-3</v>
+        <v>1.4862282874762718E-3</v>
       </c>
       <c r="J15">
         <v>1.7008685336363238E-3</v>
       </c>
       <c r="K15">
-        <v>4.5340527891044492E-5</v>
+        <v>3.2110825670618461E-5</v>
       </c>
       <c r="L15">
-        <v>1.0129753677645681E-5</v>
+        <v>5.9379267369208399E-6</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>-5</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>0.1</v>
-      </c>
       <c r="H16">
         <v>-3.7000000000000033</v>
       </c>
       <c r="I16">
-        <v>2.4652432537375711E-3</v>
+        <v>1.7281213362173133E-3</v>
       </c>
       <c r="J16">
         <v>1.9307872510138657E-3</v>
       </c>
       <c r="K16">
-        <v>7.4403769813059637E-5</v>
+        <v>5.3430703369420841E-5</v>
       </c>
       <c r="L16">
-        <v>1.7052461216082726E-5</v>
+        <v>1.0129753677645681E-5</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>-5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
       <c r="H17">
         <v>-3.6000000000000032</v>
       </c>
       <c r="I17">
-        <v>2.843617627810908E-3</v>
+        <v>2.0133931923232711E-3</v>
       </c>
       <c r="J17">
         <v>2.1957356729779831E-3</v>
       </c>
       <c r="K17">
-        <v>1.2041268996905009E-4</v>
+        <v>8.7679741268153059E-5</v>
       </c>
       <c r="L17">
-        <v>2.8327666707850252E-5</v>
+        <v>1.7052461216082726E-5</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
@@ -4548,16 +4596,16 @@
         <v>-3.5000000000000031</v>
       </c>
       <c r="I18">
-        <v>3.2867757148734374E-3</v>
+        <v>2.3505549713937267E-3</v>
       </c>
       <c r="J18">
         <v>2.5016679451859702E-3</v>
       </c>
       <c r="K18">
-        <v>1.9218457433291009E-4</v>
+        <v>1.4189809909383787E-4</v>
       </c>
       <c r="L18">
-        <v>4.6438932026160451E-5</v>
+        <v>2.8327666707850252E-5</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
@@ -4565,346 +4613,346 @@
         <v>-3.400000000000003</v>
       </c>
       <c r="I19">
-        <v>3.8069598556386285E-3</v>
+        <v>2.7499296579260404E-3</v>
       </c>
       <c r="J19">
         <v>2.8556555607303635E-3</v>
       </c>
       <c r="K19">
-        <v>3.0250582624115281E-4</v>
+        <v>2.2647634381399296E-4</v>
       </c>
       <c r="L19">
-        <v>7.5130149028268534E-5</v>
+        <v>4.6438932026160451E-5</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <f ca="1">_xlfn.NORM.S.INV(RAND())</f>
-        <v>-0.13088058689728799</v>
-      </c>
-      <c r="E20">
-        <f t="array" aca="1" ref="E20:F20" ca="1">_xll.MONTE.STDEV(Z)</f>
-        <v>-1.7390495397351106E-2</v>
-      </c>
-      <c r="F20">
-        <f ca="1"/>
-        <v>0.9987308393807125</v>
-      </c>
       <c r="H20">
         <v>-3.3000000000000029</v>
       </c>
       <c r="I20">
-        <v>4.418936191114802E-3</v>
+        <v>3.2240662915544159E-3</v>
       </c>
       <c r="J20">
         <v>3.266116247183648E-3</v>
       </c>
       <c r="K20">
-        <v>4.6958899518251198E-4</v>
+        <v>3.5648237506747424E-4</v>
       </c>
       <c r="L20">
-        <v>1.199556345671815E-4</v>
+        <v>7.5130149028268534E-5</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <f ca="1">(Z-gamma)/delta</f>
-        <v>-0.15392039126485865</v>
+        <f ca="1">_xlfn.NORM.S.INV(RAND())</f>
+        <v>0.26850427979929986</v>
       </c>
       <c r="E21">
-        <f t="array" aca="1" ref="E21:F21" ca="1">_xll.MONTE.STDEV(C21)</f>
-        <v>-7.8260330264900979E-2</v>
+        <f t="array" aca="1" ref="E21:F21" ca="1">_xll.MONTE.STDEV(Z)</f>
+        <v>0</v>
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>0.66582055958714037</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>-3.2000000000000028</v>
       </c>
       <c r="I21">
-        <v>5.1405544175295729E-3</v>
+        <v>3.7882544167237753E-3</v>
       </c>
       <c r="J21">
         <v>3.7430933562233037E-3</v>
       </c>
       <c r="K21">
-        <v>7.189042109841952E-4</v>
+        <v>5.5337843369258552E-4</v>
       </c>
       <c r="L21">
-        <v>1.8902363669015543E-4</v>
+        <v>1.199556345671815E-4</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <f ca="1">SINH(C21)</f>
-        <v>-0.15452887877067095</v>
+        <f ca="1">(Z-gamma)/delta</f>
+        <v>0.11233618653286657</v>
       </c>
       <c r="E22">
         <f t="array" aca="1" ref="E22:F22" ca="1">_xll.MONTE.STDEV(C22)</f>
-        <v>-9.7344366815959288E-2</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>0.83969355162122594</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <v>-3.1000000000000028</v>
       </c>
       <c r="I22">
-        <v>5.9934386381301956E-3</v>
+        <v>4.4611639641612428E-3</v>
       </c>
       <c r="J22">
         <v>4.2985975482454086E-3</v>
       </c>
       <c r="K22">
-        <v>1.0854081895048198E-3</v>
+        <v>8.4717932134422715E-4</v>
       </c>
       <c r="L22">
-        <v>2.9397900284716671E-4</v>
+        <v>1.8902363669015543E-4</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23">
-        <v>1</v>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C23">
-        <f ca="1">POWER($C$22,B23)</f>
-        <v>-0.15452887877067095</v>
-      </c>
-      <c r="D23" cm="1">
-        <f t="array" ref="D23">_xll.JOHNSON.Esinh_k(Johnson,B23)</f>
-        <v>-8.3318276522104329E-2</v>
+        <f ca="1">SINH(C22)</f>
+        <v>0.11257260522102722</v>
       </c>
       <c r="E23">
         <f t="array" aca="1" ref="E23:F23" ca="1">_xll.MONTE.STDEV(C23)</f>
-        <v>-9.7344366815959288E-2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>0.83969355162122594</v>
-      </c>
-      <c r="G23">
-        <f ca="1">(D23-E23)/F23</f>
-        <v>1.6703820419692747E-2</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>-3.0000000000000027</v>
       </c>
       <c r="I23">
-        <v>7.0038407971688699E-3</v>
+        <v>5.2656420440718964E-3</v>
       </c>
       <c r="J23">
         <v>4.9470254004463921E-3</v>
       </c>
       <c r="K23">
-        <v>1.6161590940232241E-3</v>
+        <v>1.2790791308723813E-3</v>
       </c>
       <c r="L23">
-        <v>4.5127159502306169E-4</v>
+        <v>2.9397900284716671E-4</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <f ca="1">POWER($C$22,B24)</f>
-        <v>2.387917437412072E-2</v>
+        <f ca="1">POWER($C$23,B24)</f>
+        <v>0.11257260522102722</v>
       </c>
       <c r="D24" cm="1">
         <f t="array" ref="D24">_xll.JOHNSON.Esinh_k(Johnson,B24)</f>
-        <v>0.72703953240446417</v>
+        <v>-8.3318276522104329E-2</v>
       </c>
       <c r="E24">
         <f t="array" aca="1" ref="E24:F24" ca="1">_xll.MONTE.STDEV(C24)</f>
-        <v>0.71452280395362333</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <f ca="1"/>
-        <v>1.5455426281821139</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ref="G24:G26" ca="1" si="0">(D24-E24)/F24</f>
-        <v>8.0985980086250818E-3</v>
+        <v>0</v>
+      </c>
+      <c r="G24" t="e">
+        <f ca="1">(D24-E24)/F24</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="H24">
         <v>-2.9000000000000026</v>
       </c>
       <c r="I24">
-        <v>8.2036955008012603E-3</v>
+        <v>6.2297058931908567E-3</v>
       </c>
       <c r="J24">
         <v>5.7056730701632308E-3</v>
       </c>
       <c r="K24">
-        <v>2.3732532063109467E-3</v>
+        <v>1.9045326811821897E-3</v>
       </c>
       <c r="L24">
-        <v>6.837527541089794E-4</v>
+        <v>4.5127159502306169E-4</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <f ca="1">POWER($C$22,B25)</f>
-        <v>-3.6900220420022132E-3</v>
+        <f ca="1">POWER($C$23,B25)</f>
+        <v>1.2672591446249245E-2</v>
       </c>
       <c r="D25" cm="1">
         <f t="array" ref="D25">_xll.JOHNSON.Esinh_k(Johnson,B25)</f>
-        <v>-0.30943204698606874</v>
+        <v>0.72703953240446417</v>
       </c>
       <c r="E25">
         <f t="array" aca="1" ref="E25:F25" ca="1">_xll.MONTE.STDEV(C25)</f>
-        <v>-0.34298526363508502</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <f ca="1"/>
-        <v>5.8665601633509512</v>
-      </c>
-      <c r="G25">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7194021223249238E-3</v>
+        <v>0</v>
+      </c>
+      <c r="G25" t="e">
+        <f ca="1">(D25-E25)/F25</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="H25">
         <v>-2.8000000000000025</v>
       </c>
       <c r="I25">
-        <v>9.6319237426882517E-3</v>
+        <v>7.3877806466644868E-3</v>
       </c>
       <c r="J25">
         <v>6.5953674494610981E-3</v>
       </c>
       <c r="K25">
-        <v>3.4369482416631019E-3</v>
+        <v>2.7967161827415145E-3</v>
       </c>
       <c r="L25">
-        <v>1.0226305623681764E-3</v>
+        <v>6.837527541089794E-4</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <f ca="1">POWER($C$22,B26)</f>
-        <v>5.7021496878966371E-4</v>
+        <f ca="1">POWER($C$23,B26)</f>
+        <v>1.4265866340059826E-3</v>
       </c>
       <c r="D26" cm="1">
         <f t="array" ref="D26">_xll.JOHNSON.Esinh_k(Johnson,B26)</f>
-        <v>3.6803803743340247</v>
+        <v>-0.30943204698606874</v>
       </c>
       <c r="E26">
         <f t="array" aca="1" ref="E26:F26" ca="1">_xll.MONTE.STDEV(C26)</f>
-        <v>2.8991148201246335</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <f ca="1"/>
-        <v>28.449775935651537</v>
-      </c>
-      <c r="G26">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7461219939885588E-2</v>
+        <v>0</v>
+      </c>
+      <c r="G26" t="e">
+        <f ca="1">(D26-E26)/F26</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="H26">
         <v>-2.7000000000000024</v>
       </c>
       <c r="I26">
-        <v>1.1336043180833468E-2</v>
+        <v>8.7822418540801448E-3</v>
       </c>
       <c r="J26">
         <v>7.6412424937365997E-3</v>
       </c>
       <c r="K26">
-        <v>4.9087493569254593E-3</v>
+        <v>4.0502078501963232E-3</v>
       </c>
       <c r="L26">
-        <v>1.5097936510474752E-3</v>
+        <v>1.0226305623681764E-3</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f ca="1">POWER($C$23,B27)</f>
+        <v>1.6059457396354953E-4</v>
+      </c>
+      <c r="D27" cm="1">
+        <f t="array" ref="D27">_xll.JOHNSON.Esinh_k(Johnson,B27)</f>
+        <v>3.6803803743340247</v>
+      </c>
+      <c r="E27">
+        <f t="array" aca="1" ref="E27:F27" ca="1">_xll.MONTE.STDEV(C27)</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27" t="e">
+        <f ca="1">(D27-E27)/F27</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="H27">
         <v>-2.6000000000000023</v>
       </c>
       <c r="I27">
-        <v>1.3374153962431681E-2</v>
+        <v>1.0465335719336001E-2</v>
       </c>
       <c r="J27">
         <v>8.8736947307866409E-3</v>
       </c>
       <c r="K27">
-        <v>6.9141320948501372E-3</v>
+        <v>5.7846245512400349E-3</v>
       </c>
       <c r="L27">
+        <v>1.5097936510474752E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H28">
+        <v>-2.5000000000000022</v>
+      </c>
+      <c r="I28">
+        <v>1.2501564574641506E-2</v>
+      </c>
+      <c r="J28">
+        <v>1.0329559453804926E-2</v>
+      </c>
+      <c r="K28">
+        <v>8.1478306098394133E-3</v>
+      </c>
+      <c r="L28">
         <v>2.200481002527066E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C28" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">_xll.JOHNSON.X(Johnson,Z)</f>
-        <v>-0.25452887877067093</v>
-      </c>
-      <c r="D28">
+      <c r="C29" t="e" cm="1">
+        <f t="array" aca="1" ref="C29" ca="1">_xll.JOHNSON.X(Johnson,Z)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D29">
         <f>mu</f>
         <v>-0.18331827652210433</v>
       </c>
-      <c r="E28">
-        <f t="array" aca="1" ref="E28:F28" ca="1">_xll.MONTE.STDEV(C28)</f>
-        <v>-0.1973443668159591</v>
-      </c>
-      <c r="F28">
+      <c r="E29" t="e">
+        <f t="array" aca="1" ref="E29:F29" ca="1">_xll.MONTE.STDEV(C29)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F29" t="e">
         <f ca="1"/>
-        <v>0.83969355162122594</v>
-      </c>
-      <c r="G28">
-        <f t="shared" ref="G28" ca="1" si="1">(D28-E28)/F28</f>
-        <v>1.6703820419692515E-2</v>
-      </c>
-      <c r="H28">
-        <v>-2.5000000000000022</v>
-      </c>
-      <c r="I28">
-        <v>1.5817381060070058E-2</v>
-      </c>
-      <c r="J28">
-        <v>1.0329559453804926E-2</v>
-      </c>
-      <c r="K28">
-        <v>9.6044707297148531E-3</v>
-      </c>
-      <c r="L28">
-        <v>3.1662305551806158E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G29" t="e">
+        <f ca="1">(D29-E29)/F29</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="H29">
         <v>-2.4000000000000021</v>
       </c>
       <c r="I29">
-        <v>1.8752865321856195E-2</v>
+        <v>1.4970640122302065E-2</v>
       </c>
       <c r="J29">
         <v>1.2053557774557189E-2</v>
       </c>
       <c r="K29">
-        <v>1.3157644610931496E-2</v>
+        <v>1.1318210229330824E-2</v>
       </c>
       <c r="L29">
-        <v>4.4979827366486425E-3</v>
+        <v>3.1662305551806158E-3</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
@@ -4912,16 +4960,16 @@
         <v>-2.300000000000002</v>
       </c>
       <c r="I30">
-        <v>2.2287403328615518E-2</v>
+        <v>1.7971120372145401E-2</v>
       </c>
       <c r="J30">
         <v>1.4100074371410087E-2</v>
       </c>
       <c r="K30">
-        <v>1.7776727540917244E-2</v>
+        <v>1.5505382026789284E-2</v>
       </c>
       <c r="L30">
-        <v>6.3091485395969649E-3</v>
+        <v>4.4979827366486425E-3</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
@@ -4929,16 +4977,16 @@
         <v>-2.200000000000002</v>
       </c>
       <c r="I31">
-        <v>2.6551835924275985E-2</v>
+        <v>2.162485386135931E-2</v>
       </c>
       <c r="J31">
         <v>1.6535335860321854E-2</v>
       </c>
       <c r="K31">
-        <v>2.3686147538921953E-2</v>
+        <v>2.0948654554711729E-2</v>
       </c>
       <c r="L31">
-        <v>8.738379999018886E-3</v>
+        <v>6.3091485395969649E-3</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
@@ -4946,16 +4994,16 @@
         <v>-2.1000000000000019</v>
       </c>
       <c r="I32">
-        <v>3.1706268651791748E-2</v>
+        <v>2.6082349222530603E-2</v>
       </c>
       <c r="J32">
         <v>1.9440069055922549E-2</v>
       </c>
       <c r="K32">
-        <v>3.1124758746852912E-2</v>
+        <v>2.7912500845991409E-2</v>
       </c>
       <c r="L32">
-        <v>1.1951711127894171E-2</v>
+        <v>8.738379999018886E-3</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.35">
@@ -4963,16 +5011,16 @@
         <v>-2.0000000000000018</v>
       </c>
       <c r="I33">
-        <v>3.7946160369435343E-2</v>
+        <v>3.1529156554821171E-2</v>
       </c>
       <c r="J33">
         <v>2.2912724696017739E-2</v>
       </c>
       <c r="K33">
-        <v>4.0335412919497708E-2</v>
+        <v>3.667839412995362E-2</v>
       </c>
       <c r="L33">
-        <v>1.6143679195266492E-2</v>
+        <v>1.1951711127894171E-2</v>
       </c>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.35">
@@ -4980,16 +5028,16 @@
         <v>-1.9000000000000017</v>
       </c>
       <c r="I34">
-        <v>4.5509216377232126E-2</v>
+        <v>3.8193267748764997E-2</v>
       </c>
       <c r="J34">
         <v>2.7073351399755086E-2</v>
       </c>
       <c r="K34">
-        <v>5.1550866592650089E-2</v>
+        <v>4.7532518548608807E-2</v>
       </c>
       <c r="L34">
-        <v>2.1537001230033159E-2</v>
+        <v>1.6143679195266492E-2</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.35">
@@ -4997,16 +5045,16 @@
         <v>-1.8000000000000016</v>
       </c>
       <c r="I35">
-        <v>5.4682833672723648E-2</v>
+        <v>4.635338095207199E-2</v>
       </c>
       <c r="J35">
         <v>3.2068189760577293E-2</v>
       </c>
       <c r="K35">
-        <v>6.4976211112027962E-2</v>
+        <v>6.0749161720556701E-2</v>
       </c>
       <c r="L35">
-        <v>2.8380381049400383E-2</v>
+        <v>2.1537001230033159E-2</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.35">
@@ -5014,16 +5062,16 @@
         <v>-1.7000000000000015</v>
       </c>
       <c r="I36">
-        <v>6.5811514016871256E-2</v>
+        <v>5.6347575173483537E-2</v>
       </c>
       <c r="J36">
         <v>3.8075016121317418E-2</v>
       </c>
       <c r="K36">
-        <v>8.0768449477460272E-2</v>
+        <v>7.6570009734742317E-2</v>
       </c>
       <c r="L36">
-        <v>3.6944069202113072E-2</v>
+        <v>2.8380381049400383E-2</v>
       </c>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.35">
@@ -5031,16 +5079,16 @@
         <v>-1.6000000000000014</v>
       </c>
       <c r="I37">
-        <v>7.9303106330023757E-2</v>
+        <v>6.8581423232842151E-2</v>
       </c>
       <c r="J37">
         <v>4.5309181693160505E-2</v>
       </c>
       <c r="K37">
-        <v>9.9014331126980507E-2</v>
+        <v>9.518007986163346E-2</v>
       </c>
       <c r="L37">
-        <v>4.7512900186882034E-2</v>
+        <v>3.6944069202113072E-2</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.35">
@@ -5048,16 +5096,16 @@
         <v>-1.5000000000000013</v>
       </c>
       <c r="I38">
-        <v>9.5631856999947168E-2</v>
+        <v>8.3533721173020117E-2</v>
       </c>
       <c r="J38">
         <v>5.4030137936078082E-2</v>
       </c>
       <c r="K38">
-        <v>0.11970803997794603</v>
+        <v>0.11668160036602157</v>
       </c>
       <c r="L38">
-        <v>6.0376691115162584E-2</v>
+        <v>4.7512900186882034E-2</v>
       </c>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.35">
@@ -5065,16 +5113,16 @@
         <v>-1.4000000000000012</v>
       </c>
       <c r="I39">
-        <v>0.11533490846887444</v>
+        <v>0.10175668714524692</v>
       </c>
       <c r="J39">
         <v>6.4547974393468432E-2</v>
       </c>
       <c r="K39">
-        <v>0.14273074468823588</v>
+        <v>0.14106771739328908</v>
       </c>
       <c r="L39">
-        <v>7.5818099411116724E-2</v>
+        <v>6.0376691115162584E-2</v>
       </c>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.35">
@@ -5082,16 +5130,16 @@
         <v>-1.3000000000000012</v>
       </c>
       <c r="I40">
-        <v>0.13899698174264619</v>
+        <v>0.12386553954620814</v>
       </c>
       <c r="J40">
         <v>7.7229068980227855E-2</v>
       </c>
       <c r="K40">
-        <v>0.16783428900627631</v>
+        <v>0.16819839635435682</v>
       </c>
       <c r="L40">
-        <v>9.4098291512360543E-2</v>
+        <v>7.5818099411116724E-2</v>
       </c>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.35">
@@ -5099,16 +5147,16 @@
         <v>-1.2000000000000011</v>
       </c>
       <c r="I41">
-        <v>0.16721550635297847</v>
+        <v>0.1505097457110279</v>
       </c>
       <c r="J41">
         <v>9.2499304803588034E-2</v>
       </c>
       <c r="K41">
-        <v>0.1946313541389823</v>
+        <v>0.19778120212145192</v>
       </c>
       <c r="L41">
-        <v>0.11544104856560938</v>
+        <v>9.4098291512360543E-2</v>
       </c>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.35">
@@ -5116,16 +5164,16 @@
         <v>-1.100000000000001</v>
       </c>
       <c r="I42">
-        <v>0.20053573830560054</v>
+        <v>0.18231516708719597</v>
       </c>
       <c r="J42">
         <v>0.11084239711217125</v>
       </c>
       <c r="K42">
-        <v>0.22259421080404848</v>
+        <v>0.2293597060532393</v>
       </c>
       <c r="L42">
-        <v>0.1400162001061811</v>
+        <v>0.11544104856560938</v>
       </c>
     </row>
     <row r="43" spans="8:12" x14ac:dyDescent="0.35">
@@ -5133,16 +5181,16 @@
         <v>-1.0000000000000009</v>
       </c>
       <c r="I43">
-        <v>0.23934344697746879</v>
+        <v>0.21978371233224786</v>
       </c>
       <c r="J43">
         <v>0.1327897166111156</v>
       </c>
       <c r="K43">
-        <v>0.25106367154362719</v>
+        <v>0.26231201537401122</v>
       </c>
       <c r="L43">
-        <v>0.1679234992663976</v>
+        <v>0.1400162001061811</v>
       </c>
     </row>
     <row r="44" spans="8:12" x14ac:dyDescent="0.35">
@@ -5150,16 +5198,16 @@
         <v>-0.90000000000000091</v>
       </c>
       <c r="I44">
-        <v>0.28370383266135807</v>
+        <v>0.26313711634201442</v>
       </c>
       <c r="J44">
         <v>0.15889676819044174</v>
       </c>
       <c r="K44">
-        <v>0.27926906815860497</v>
+        <v>0.29586132286154604</v>
       </c>
       <c r="L44">
-        <v>0.19917819908999618</v>
+        <v>0.1679234992663976</v>
       </c>
     </row>
     <row r="45" spans="8:12" x14ac:dyDescent="0.35">
@@ -5167,16 +5215,16 @@
         <v>-0.80000000000000093</v>
       </c>
       <c r="I45">
-        <v>0.33314353279466052</v>
+        <v>0.31209818271004786</v>
       </c>
       <c r="J45">
         <v>0.18970067882141106</v>
       </c>
       <c r="K45">
-        <v>0.30635907240424409</v>
+        <v>0.32909944888366083</v>
       </c>
       <c r="L45">
-        <v>0.23369962916910997</v>
+        <v>0.19917819908999618</v>
       </c>
     </row>
     <row r="46" spans="8:12" x14ac:dyDescent="0.35">
@@ -5184,16 +5232,16 @@
         <v>-0.70000000000000095</v>
       </c>
       <c r="I46">
-        <v>0.38639348936483231</v>
+        <v>0.36562223394466031</v>
       </c>
       <c r="J46">
         <v>0.22565364994386311</v>
       </c>
       <c r="K46">
-        <v>0.33144204934714083</v>
+        <v>0.361023161474819</v>
       </c>
       <c r="L46">
-        <v>0.27130398448337512</v>
+        <v>0.23369962916910997</v>
       </c>
     </row>
     <row r="47" spans="8:12" x14ac:dyDescent="0.35">
@@ -5201,16 +5249,16 @@
         <v>-0.60000000000000098</v>
       </c>
       <c r="I47">
-        <v>0.44114844502398848</v>
+        <v>0.42162902038545386</v>
       </c>
       <c r="J47">
         <v>0.26703086079299182</v>
       </c>
       <c r="K47">
-        <v>0.35363351273308435</v>
+        <v>0.39058173000049884</v>
       </c>
       <c r="L47">
-        <v>0.31170231708788843</v>
+        <v>0.27130398448337512</v>
       </c>
     </row>
     <row r="48" spans="8:12" x14ac:dyDescent="0.35">
@@ -5218,16 +5266,16 @@
         <v>-0.500000000000001</v>
       </c>
       <c r="I48">
-        <v>0.49394968253813593</v>
+        <v>0.47683859327233863</v>
       </c>
       <c r="J48">
         <v>0.31381938239430635</v>
       </c>
       <c r="K48">
-        <v>0.37210728633127754</v>
+        <v>0.41673284805446192</v>
       </c>
       <c r="L48">
-        <v>0.35450437574156468</v>
+        <v>0.31170231708788843</v>
       </c>
     </row>
     <row r="49" spans="8:12" x14ac:dyDescent="0.35">
@@ -5235,16 +5283,16 @@
         <v>-0.40000000000000102</v>
       </c>
       <c r="I49">
-        <v>0.54033731014439135</v>
+        <v>0.52686165134711072</v>
       </c>
       <c r="J49">
         <v>0.36560757076051598</v>
       </c>
       <c r="K49">
-        <v>0.38614630456966198</v>
+        <v>0.43850292359506593</v>
       </c>
       <c r="L49">
-        <v>0.39922849533890892</v>
+        <v>0.35450437574156468</v>
       </c>
     </row>
     <row r="50" spans="8:12" x14ac:dyDescent="0.35">
@@ -5252,16 +5300,16 @@
         <v>-0.30000000000000104</v>
       </c>
       <c r="I50">
-        <v>0.57539832144528535</v>
+        <v>0.56668689277319728</v>
       </c>
       <c r="J50">
         <v>0.42150877521786989</v>
       </c>
       <c r="K50">
-        <v>0.39518872151042966</v>
+        <v>0.45504694401087509</v>
       </c>
       <c r="L50">
-        <v>0.4453172388022601</v>
+        <v>0.39922849533890892</v>
       </c>
     </row>
     <row r="51" spans="8:12" x14ac:dyDescent="0.35">
@@ -5269,16 +5317,16 @@
         <v>-0.20000000000000104</v>
       </c>
       <c r="I51">
-        <v>0.59470715122605933</v>
+        <v>0.59158980722526067</v>
       </c>
       <c r="J51">
         <v>0.48016036015686281</v>
       </c>
       <c r="K51">
-        <v>0.39886520272982412</v>
+        <v>0.46570281238686317</v>
       </c>
       <c r="L51">
-        <v>0.49215799108738634</v>
+        <v>0.4453172388022601</v>
       </c>
     </row>
     <row r="52" spans="8:12" x14ac:dyDescent="0.35">
@@ -5286,16 +5334,16 @@
         <v>-0.10000000000000103</v>
       </c>
       <c r="I52">
-        <v>0.59542882121551766</v>
+        <v>0.59826048564870093</v>
       </c>
       <c r="J52">
         <v>0.53982783727702832</v>
       </c>
       <c r="K52">
-        <v>0.39702395178508854</v>
+        <v>0.47003529342785944</v>
       </c>
       <c r="L52">
-        <v>0.5391072542633486</v>
+        <v>0.49215799108738634</v>
       </c>
     </row>
     <row r="53" spans="8:12" x14ac:dyDescent="0.35">
@@ -5303,16 +5351,16 @@
         <v>-1.0269562977782698E-15</v>
       </c>
       <c r="I53">
-        <v>0.57715962684987532</v>
+        <v>0.58573254518205409</v>
       </c>
       <c r="J53">
         <v>0.59861008809060445</v>
       </c>
       <c r="K53">
-        <v>0.38974110802513773</v>
+        <v>0.46786550543392069</v>
       </c>
       <c r="L53">
-        <v>0.58551704670180216</v>
+        <v>0.5391072542633486</v>
       </c>
     </row>
     <row r="54" spans="8:12" x14ac:dyDescent="0.35">
@@ -5320,16 +5368,16 @@
         <v>9.9999999999998979E-2</v>
       </c>
       <c r="I54">
-        <v>0.54210271839214386</v>
+        <v>0.55568406301801265</v>
       </c>
       <c r="J54">
         <v>0.65469786778660533</v>
       </c>
       <c r="K54">
-        <v>0.37731552318190265</v>
+        <v>0.45928317340728742</v>
       </c>
       <c r="L54">
-        <v>0.6307616096276677</v>
+        <v>0.58551704670180216</v>
       </c>
     </row>
     <row r="55" spans="8:12" x14ac:dyDescent="0.35">
@@ -5337,16 +5385,16 @@
         <v>0.19999999999999898</v>
       </c>
       <c r="I55">
-        <v>0.49447256967407777</v>
+        <v>0.51195466625293107</v>
       </c>
       <c r="J55">
         <v>0.70661049867299153</v>
       </c>
       <c r="K55">
-        <v>0.36024841612372832</v>
+        <v>0.44464047362342363</v>
       </c>
       <c r="L55">
-        <v>0.67426259492032903</v>
+        <v>0.6307616096276677</v>
       </c>
     </row>
     <row r="56" spans="8:12" x14ac:dyDescent="0.35">
@@ -5354,16 +5402,16 @@
         <v>0.29999999999999899</v>
       </c>
       <c r="I56">
-        <v>0.43940566781679591</v>
+        <v>0.45951310375493226</v>
       </c>
       <c r="J56">
         <v>0.75334475505344645</v>
       </c>
       <c r="K56">
-        <v>0.33920983599314536</v>
+        <v>0.42452805815285793</v>
       </c>
       <c r="L56">
-        <v>0.71551105270225679</v>
+        <v>0.67426259492032903</v>
       </c>
     </row>
     <row r="57" spans="8:12" x14ac:dyDescent="0.35">
@@ -5371,16 +5419,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="I57">
-        <v>0.38184618915061219</v>
+        <v>0.40333290231099084</v>
       </c>
       <c r="J57">
         <v>0.79440968148262048</v>
       </c>
       <c r="K57">
-        <v>0.31499506041750763</v>
+        <v>0.39973553396848466</v>
       </c>
       <c r="L57">
-        <v>0.75408483827835626</v>
+        <v>0.71551105270225679</v>
       </c>
     </row>
     <row r="58" spans="8:12" x14ac:dyDescent="0.35">
@@ -5388,16 +5436,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="I58">
-        <v>0.32577559423885932</v>
+        <v>0.34756551619886417</v>
       </c>
       <c r="J58">
         <v>0.82976508640009961</v>
       </c>
       <c r="K58">
-        <v>0.28847487892577062</v>
+        <v>0.37120008122633552</v>
       </c>
       <c r="L58">
-        <v>0.78966047915550108</v>
+        <v>0.75408483827835626</v>
       </c>
     </row>
     <row r="59" spans="8:12" x14ac:dyDescent="0.35">
@@ -5405,16 +5453,16 @@
         <v>0.59999999999999898</v>
       </c>
       <c r="I59">
-        <v>0.27390284321552266</v>
+        <v>0.29516008101077751</v>
       </c>
       <c r="J59">
         <v>0.85970610254397384</v>
       </c>
       <c r="K59">
-        <v>0.26054407761647447</v>
+        <v>0.33994786568104446</v>
       </c>
       <c r="L59">
-        <v>0.82201903463938053</v>
+        <v>0.78966047915550108</v>
       </c>
     </row>
     <row r="60" spans="8:12" x14ac:dyDescent="0.35">
@@ -5422,16 +5470,16 @@
         <v>0.69999999999999896</v>
       </c>
       <c r="I60">
-        <v>0.22772309026885401</v>
+        <v>0.24786265305354699</v>
       </c>
       <c r="J60">
         <v>0.88473649070521498</v>
       </c>
       <c r="K60">
-        <v>0.23207232939372091</v>
+        <v>0.30703333139918837</v>
       </c>
       <c r="L60">
-        <v>0.8510459871231203</v>
+        <v>0.82201903463938053</v>
       </c>
     </row>
     <row r="61" spans="8:12" x14ac:dyDescent="0.35">
@@ -5439,16 +5487,16 @@
         <v>0.79999999999999893</v>
       </c>
       <c r="I61">
-        <v>0.18777406465475951</v>
+        <v>0.20643464151232535</v>
       </c>
       <c r="J61">
         <v>0.90545912867964717</v>
       </c>
       <c r="K61">
-        <v>0.20386114863355567</v>
+        <v>0.27348132826957205</v>
       </c>
       <c r="L61">
-        <v>0.87672567135600432</v>
+        <v>0.8510459871231203</v>
       </c>
     </row>
     <row r="62" spans="8:12" x14ac:dyDescent="0.35">
@@ -5456,16 +5504,16 @@
         <v>0.89999999999999891</v>
       </c>
       <c r="I62">
-        <v>0.15394269159729695</v>
+        <v>0.17094208255481272</v>
       </c>
       <c r="J62">
         <v>0.92249563844821658</v>
       </c>
       <c r="K62">
-        <v>0.17660968747111744</v>
+        <v>0.2402363860289409</v>
       </c>
       <c r="L62">
-        <v>0.89913112989631394</v>
+        <v>0.87672567135600432</v>
       </c>
     </row>
     <row r="63" spans="8:12" x14ac:dyDescent="0.35">
@@ -5473,16 +5521,16 @@
         <v>0.99999999999999889</v>
       </c>
       <c r="I63">
-        <v>0.12573535723614146</v>
+        <v>0.14102310732675341</v>
       </c>
       <c r="J63">
         <v>0.93643532470665591</v>
       </c>
       <c r="K63">
-        <v>0.15089106605067718</v>
+        <v>0.20812240753154615</v>
       </c>
       <c r="L63">
-        <v>0.91841054758371254</v>
+        <v>0.89913112989631394</v>
       </c>
     </row>
     <row r="64" spans="8:12" x14ac:dyDescent="0.35">
@@ -5490,16 +5538,16 @@
         <v>1.099999999999999</v>
       </c>
       <c r="I64">
-        <v>0.10247924379988503</v>
+        <v>0.11609451902596506</v>
       </c>
       <c r="J64">
         <v>0.9478077952472802</v>
       </c>
       <c r="K64">
-        <v>0.1271397875585551</v>
+        <v>0.17781477557172073</v>
       </c>
       <c r="L64">
-        <v>0.93477154988264299</v>
+        <v>0.91841054758371254</v>
       </c>
     </row>
     <row r="65" spans="8:12" x14ac:dyDescent="0.35">
@@ -5507,16 +5555,16 @@
         <v>1.1999999999999991</v>
       </c>
       <c r="I65">
-        <v>8.3454771452459969E-2</v>
+        <v>9.5492644712746544E-2</v>
       </c>
       <c r="J65">
         <v>0.95707218903654212</v>
       </c>
       <c r="K65">
-        <v>0.10564972858903163</v>
+        <v>0.14982552236305358</v>
       </c>
       <c r="L65">
-        <v>0.9484646509808301</v>
+        <v>0.93477154988264299</v>
       </c>
     </row>
     <row r="66" spans="8:12" x14ac:dyDescent="0.35">
@@ -5524,16 +5572,16 @@
         <v>1.2999999999999992</v>
       </c>
       <c r="I66">
-        <v>6.7973055423371204E-2</v>
+        <v>7.8559459413378926E-2</v>
       </c>
       <c r="J66">
         <v>0.96461676084963277</v>
       </c>
       <c r="K66">
-        <v>8.6581327377994829E-2</v>
+        <v>0.12450096132240532</v>
       </c>
       <c r="L66">
-        <v>0.95976702402819636</v>
+        <v>0.9484646509808301</v>
       </c>
     </row>
     <row r="67" spans="8:12" x14ac:dyDescent="0.35">
@@ -5541,16 +5589,16 @@
         <v>1.3999999999999992</v>
       </c>
       <c r="I67">
-        <v>5.5414890241784878E-2</v>
+        <v>6.4689101103908325E-2</v>
       </c>
       <c r="J67">
         <v>0.97076415638537239</v>
       </c>
       <c r="K67">
-        <v>6.9975988703070452E-2</v>
+        <v>0.10203015791040425</v>
       </c>
       <c r="L67">
-        <v>0.96896756518996463</v>
+        <v>0.95976702402819636</v>
       </c>
     </row>
     <row r="68" spans="8:12" x14ac:dyDescent="0.35">
@@ -5558,16 +5606,16 @@
         <v>1.4999999999999993</v>
       </c>
       <c r="I68">
-        <v>4.5245345804669039E-2</v>
+        <v>5.3348411896260793E-2</v>
       </c>
       <c r="J68">
         <v>0.97577926447744701</v>
       </c>
       <c r="K68">
-        <v>5.5775413262316602E-2</v>
+        <v>8.2461904818584827E-2</v>
       </c>
       <c r="L68">
-        <v>0.97635396851130229</v>
+        <v>0.96896756518996463</v>
       </c>
     </row>
     <row r="69" spans="8:12" x14ac:dyDescent="0.35">
@@ -5575,16 +5623,16 @@
         <v>1.5999999999999994</v>
       </c>
       <c r="I69">
-        <v>3.7014277081999572E-2</v>
+        <v>4.4081848771799527E-2</v>
       </c>
       <c r="J69">
         <v>0.97987775432362723</v>
       </c>
       <c r="K69">
-        <v>4.3843528634727978E-2</v>
+        <v>6.5727500316870441E-2</v>
       </c>
       <c r="L69">
-        <v>0.98220225408289652</v>
+        <v>0.97635396851130229</v>
       </c>
     </row>
     <row r="70" spans="8:12" x14ac:dyDescent="0.35">
@@ -5592,16 +5640,16 @@
         <v>1.6999999999999995</v>
       </c>
       <c r="I70">
-        <v>3.0349578854128156E-2</v>
+        <v>3.6507840328979774E-2</v>
       </c>
       <c r="J70">
         <v>0.98323425636184081</v>
       </c>
       <c r="K70">
-        <v>3.3988903389060465E-2</v>
+        <v>5.16665923868425E-2</v>
       </c>
       <c r="L70">
-        <v>0.9867689282952028</v>
+        <v>0.98220225408289652</v>
       </c>
     </row>
     <row r="71" spans="8:12" x14ac:dyDescent="0.35">
@@ -5609,16 +5657,16 @@
         <v>1.7999999999999996</v>
       </c>
       <c r="I71">
-        <v>2.4947380161910032E-2</v>
+        <v>3.0311076692013831E-2</v>
       </c>
       <c r="J71">
         <v>0.98598968932458764</v>
       </c>
       <c r="K71">
-        <v>2.5985899553835238E-2</v>
+        <v>4.0053592212178295E-2</v>
       </c>
       <c r="L71">
-        <v>0.9902857260411948</v>
+        <v>0.9867689282952028</v>
       </c>
     </row>
     <row r="72" spans="8:12" x14ac:dyDescent="0.35">
@@ -5626,16 +5674,16 @@
         <v>1.8999999999999997</v>
       </c>
       <c r="I72">
-        <v>2.0561569352483568E-2</v>
+        <v>2.5233391274780408E-2</v>
       </c>
       <c r="J72">
         <v>0.98825755897140199</v>
       </c>
       <c r="K72">
-        <v>1.9593287345387095E-2</v>
+        <v>3.0622600914242487E-2</v>
       </c>
       <c r="L72">
-        <v>0.99295670616128739</v>
+        <v>0.9902857260411948</v>
       </c>
     </row>
     <row r="73" spans="8:12" x14ac:dyDescent="0.35">
@@ -5643,16 +5691,16 @@
         <v>1.9999999999999998</v>
       </c>
       <c r="I73">
-        <v>1.6993892996149909E-2</v>
+        <v>2.1064695581679397E-2</v>
       </c>
       <c r="J73">
         <v>0.99012923108926487</v>
       </c>
       <c r="K73">
-        <v>1.4569538978236743E-2</v>
+        <v>2.3089345732782745E-2</v>
       </c>
       <c r="L73">
-        <v>0.99495735016618658</v>
+        <v>0.99295670616128739</v>
       </c>
     </row>
     <row r="74" spans="8:12" x14ac:dyDescent="0.35">
@@ -5660,16 +5708,16 @@
         <v>2.0999999999999996</v>
       </c>
       <c r="I74">
-        <v>1.4085184456303192E-2</v>
+        <v>1.7634688453057518E-2</v>
       </c>
       <c r="J74">
         <v>0.99167826820763394</v>
       </c>
       <c r="K74">
-        <v>1.0684476824571722E-2</v>
+        <v>1.7169202732841192E-2</v>
       </c>
       <c r="L74">
-        <v>0.99643524956985763</v>
+        <v>0.99495735016618658</v>
       </c>
     </row>
     <row r="75" spans="8:12" x14ac:dyDescent="0.35">
@@ -5677,16 +5725,16 @@
         <v>2.1999999999999997</v>
       </c>
       <c r="I75">
-        <v>1.1707890250092369E-2</v>
+        <v>1.4805628237730175E-2</v>
       </c>
       <c r="J75">
         <v>0.99296395371698609</v>
       </c>
       <c r="K75">
-        <v>7.7273336186864392E-3</v>
+        <v>1.2590923362052458E-2</v>
       </c>
       <c r="L75">
-        <v>0.99751195232230505</v>
+        <v>0.99643524956985763</v>
       </c>
     </row>
     <row r="76" spans="8:12" x14ac:dyDescent="0.35">
@@ -5694,16 +5742,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I76">
-        <v>9.7598597336093773E-3</v>
+        <v>1.2466218036361576E-2</v>
       </c>
       <c r="J76">
         <v>0.99403413258985318</v>
       </c>
       <c r="K76">
-        <v>5.5115660199926931E-3</v>
+        <v>9.106132848932677E-3</v>
       </c>
       <c r="L76">
-        <v>0.99828556336816709</v>
+        <v>0.99751195232230505</v>
       </c>
     </row>
     <row r="77" spans="8:12" x14ac:dyDescent="0.35">
@@ -5711,16 +5759,16 @@
         <v>2.4</v>
       </c>
       <c r="I77">
-        <v>8.1592698982939811E-3</v>
+        <v>1.0526533731672923E-2</v>
       </c>
       <c r="J77">
         <v>0.99492748909742335</v>
       </c>
       <c r="K77">
-        <v>3.8769420973590535E-3</v>
+        <v>6.4950026568476515E-3</v>
       </c>
       <c r="L77">
-        <v>0.9988337461459853</v>
+        <v>0.99828556336816709</v>
       </c>
     </row>
     <row r="78" spans="8:12" x14ac:dyDescent="0.35">
@@ -5728,16 +5776,16 @@
         <v>2.5</v>
       </c>
       <c r="I78">
-        <v>6.8405242152831357E-3</v>
+        <v>8.9138724753217869E-3</v>
       </c>
       <c r="J78">
         <v>0.99567536708715021</v>
       </c>
       <c r="K78">
-        <v>2.6895062966261762E-3</v>
+        <v>4.568710441179645E-3</v>
       </c>
       <c r="L78">
-        <v>0.99921683895094049</v>
+        <v>0.9988337461459853</v>
       </c>
     </row>
     <row r="79" spans="8:12" x14ac:dyDescent="0.35">
@@ -5745,16 +5793,16 @@
         <v>2.6</v>
       </c>
       <c r="I79">
-        <v>5.7509635581052959E-3</v>
+        <v>7.5693849518498517E-3</v>
       </c>
       <c r="J79">
         <v>0.99630322205337885</v>
       </c>
       <c r="K79">
-        <v>1.8400294145894814E-3</v>
+        <v>3.1693987659461372E-3</v>
       </c>
       <c r="L79">
-        <v>0.99948087211676628</v>
+        <v>0.99921683895094049</v>
       </c>
     </row>
     <row r="80" spans="8:12" x14ac:dyDescent="0.35">
@@ -5762,16 +5810,16 @@
         <v>2.7</v>
       </c>
       <c r="I80">
-        <v>4.8482414581218526E-3</v>
+        <v>6.4453597493496573E-3</v>
       </c>
       <c r="J80">
         <v>0.99683177866878769</v>
       </c>
       <c r="K80">
-        <v>1.241497689572178E-3</v>
+        <v>2.168348504415149E-3</v>
       </c>
       <c r="L80">
-        <v>0.99966034087037814</v>
+        <v>0.99948087211676628</v>
       </c>
     </row>
     <row r="81" spans="8:12" x14ac:dyDescent="0.35">
@@ -5779,16 +5827,16 @@
         <v>2.8000000000000003</v>
       </c>
       <c r="I81">
-        <v>4.0982359455794416E-3</v>
+        <v>5.5030419650537775E-3</v>
       </c>
       <c r="J81">
         <v>0.99727795364724292</v>
       </c>
       <c r="K81">
-        <v>8.2610645449592067E-4</v>
+        <v>1.463019904504783E-3</v>
       </c>
       <c r="L81">
-        <v>0.9997806490298029</v>
+        <v>0.99966034087037814</v>
       </c>
     </row>
     <row r="82" spans="8:12" x14ac:dyDescent="0.35">
@@ -5796,16 +5844,16 @@
         <v>2.9000000000000004</v>
       </c>
       <c r="I82">
-        <v>3.4733910783840906E-3</v>
+        <v>4.7108849258413223E-3</v>
       </c>
       <c r="J82">
         <v>0.9976555920820569</v>
       </c>
       <c r="K82">
-        <v>5.4211954457831233E-4</v>
+        <v>9.7350981505563302E-4</v>
       </c>
       <c r="L82">
-        <v>0.99986018749144967</v>
+        <v>0.9997806490298029</v>
       </c>
     </row>
     <row r="83" spans="8:12" x14ac:dyDescent="0.35">
@@ -5813,16 +5861,16 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="I83">
-        <v>2.9514005876051532E-3</v>
+        <v>4.043150573963262E-3</v>
       </c>
       <c r="J83">
         <v>0.99797605569841419</v>
       </c>
       <c r="K83">
-        <v>3.5085127892498511E-4</v>
+        <v>6.3885071313540126E-4</v>
       </c>
       <c r="L83">
-        <v>0.99991204780711773</v>
+        <v>0.99986018749144967</v>
       </c>
     </row>
     <row r="84" spans="8:12" x14ac:dyDescent="0.35">
@@ -5830,16 +5878,16 @@
         <v>3.1000000000000005</v>
       </c>
       <c r="I84">
-        <v>2.5141629147183366E-3</v>
+        <v>3.4787892306154138E-3</v>
       </c>
       <c r="J84">
         <v>0.99824869356626755</v>
       </c>
       <c r="K84">
-        <v>2.2393398716512202E-4</v>
+        <v>4.1345417627405937E-4</v>
       </c>
       <c r="L84">
-        <v>0.9999453957451081</v>
+        <v>0.99991204780711773</v>
       </c>
     </row>
     <row r="85" spans="8:12" x14ac:dyDescent="0.35">
@@ -5847,16 +5895,16 @@
         <v>3.2000000000000006</v>
       </c>
       <c r="I85">
-        <v>2.1469510690586085E-3</v>
+        <v>3.0005425676843875E-3</v>
       </c>
       <c r="J85">
         <v>0.99848121947733492</v>
       </c>
       <c r="K85">
-        <v>1.4095676091077988E-4</v>
+        <v>2.6389084995445336E-4</v>
       </c>
       <c r="L85">
-        <v>0.99996654420133968</v>
+        <v>0.9999453957451081</v>
       </c>
     </row>
     <row r="86" spans="8:12" x14ac:dyDescent="0.35">
@@ -5864,16 +5912,16 @@
         <v>3.3000000000000007</v>
       </c>
       <c r="I86">
-        <v>1.8377523482641029E-3</v>
+        <v>2.5942246219057556E-3</v>
       </c>
       <c r="J86">
         <v>0.99868001513339677</v>
       </c>
       <c r="K86">
-        <v>8.7502560127317714E-5</v>
+        <v>1.6610787810491804E-4</v>
       </c>
       <c r="L86">
-        <v>0.99997977128828142</v>
+        <v>0.99996654420133968</v>
       </c>
     </row>
     <row r="87" spans="8:12" x14ac:dyDescent="0.35">
@@ -5881,16 +5929,16 @@
         <v>3.4000000000000008</v>
       </c>
       <c r="I87">
-        <v>1.5767423466555525E-3</v>
+        <v>2.2481447322403158E-3</v>
       </c>
       <c r="J87">
         <v>0.99885037428363677</v>
       </c>
       <c r="K87">
-        <v>5.3570359110430774E-5</v>
+        <v>1.0311576754162756E-4</v>
       </c>
       <c r="L87">
-        <v>0.99998793007523878</v>
+        <v>0.99997977128828142</v>
       </c>
     </row>
     <row r="88" spans="8:12" x14ac:dyDescent="0.35">
@@ -5898,16 +5946,16 @@
         <v>3.5000000000000009</v>
       </c>
       <c r="I88">
-        <v>1.3558651751259989E-3</v>
+        <v>1.9526436183371142E-3</v>
       </c>
       <c r="J88">
         <v>0.99899669978044936</v>
       </c>
       <c r="K88">
-        <v>3.2344266403547226E-5</v>
+        <v>6.3128995187286524E-5</v>
       </c>
       <c r="L88">
-        <v>0.99999289328717444</v>
+        <v>0.99998793007523878</v>
       </c>
     </row>
     <row r="89" spans="8:12" x14ac:dyDescent="0.35">
@@ -5915,16 +5963,16 @@
         <v>3.600000000000001</v>
       </c>
       <c r="I89">
-        <v>1.1684977660526561E-3</v>
+        <v>1.6997197136385473E-3</v>
       </c>
       <c r="J89">
         <v>0.99912266302459396</v>
       </c>
       <c r="K89">
-        <v>1.92592336877485E-5</v>
+        <v>3.8115500288447229E-5</v>
       </c>
       <c r="L89">
-        <v>0.99999587095251719</v>
+        <v>0.99999289328717444</v>
       </c>
     </row>
     <row r="90" spans="8:12" x14ac:dyDescent="0.35">
@@ -5932,16 +5980,16 @@
         <v>3.7000000000000011</v>
       </c>
       <c r="I90">
-        <v>1.0091808349999151E-3</v>
+        <v>1.4827275743613338E-3</v>
       </c>
       <c r="J90">
         <v>0.99923133330214875</v>
       </c>
       <c r="K90">
-        <v>1.1309662629486974E-5</v>
+        <v>2.2695686401474357E-5</v>
       </c>
       <c r="L90">
-        <v>0.99999763278569898</v>
+        <v>0.99999587095251719</v>
       </c>
     </row>
     <row r="91" spans="8:12" x14ac:dyDescent="0.35">
@@ -5949,16 +5997,16 @@
         <v>3.8000000000000012</v>
       </c>
       <c r="I91">
-        <v>8.7340276935282755E-4</v>
+        <v>1.2961339288959828E-3</v>
       </c>
       <c r="J91">
         <v>0.99932528296521794</v>
       </c>
       <c r="K91">
-        <v>6.5498182178739744E-6</v>
+        <v>1.3327661967599159E-5</v>
       </c>
       <c r="L91">
-        <v>0.99999866087185763</v>
+        <v>0.99999763278569898</v>
       </c>
     </row>
     <row r="92" spans="8:12" x14ac:dyDescent="0.35">
@@ -5966,16 +6014,16 @@
         <v>3.9000000000000012</v>
       </c>
       <c r="I92">
-        <v>7.574256199980884E-4</v>
+        <v>1.1353199007592327E-3</v>
       </c>
       <c r="J92">
         <v>0.99940667318650722</v>
       </c>
       <c r="K92">
-        <v>3.7409145954420133E-6</v>
+        <v>7.7185116848182121E-6</v>
       </c>
       <c r="L92">
-        <v>0.99999925252893296</v>
+        <v>0.99999866087185763</v>
       </c>
     </row>
     <row r="93" spans="8:12" x14ac:dyDescent="0.35">
@@ -5983,16 +6031,16 @@
         <v>4.0000000000000009</v>
       </c>
       <c r="I93">
-        <v>6.5814465358202286E-4</v>
+        <v>9.9642028890174761E-4</v>
       </c>
       <c r="J93">
         <v>0.99947732405415812</v>
       </c>
       <c r="K93">
-        <v>2.1071492103023972E-6</v>
+        <v>4.4084113568267356E-6</v>
       </c>
       <c r="L93">
-        <v>0.99999958833337033</v>
+        <v>0.99999925252893296</v>
       </c>
     </row>
     <row r="94" spans="8:12" x14ac:dyDescent="0.35">
@@ -6000,16 +6048,16 @@
         <v>4.1000000000000005</v>
       </c>
       <c r="I94">
-        <v>5.7297471375401332E-4</v>
+        <v>8.7619264935989358E-4</v>
       </c>
       <c r="J94">
         <v>0.99953877201214625</v>
       </c>
       <c r="K94">
-        <v>1.1705278083347855E-6</v>
+        <v>2.4831308687302349E-6</v>
       </c>
       <c r="L94">
-        <v>0.99999977629907244</v>
+        <v>0.99999958833337033</v>
       </c>
     </row>
     <row r="95" spans="8:12" x14ac:dyDescent="0.35">
@@ -6017,16 +6065,16 @@
         <v>4.2</v>
       </c>
       <c r="I95">
-        <v>4.9975804626297467E-4</v>
+        <v>7.7191039433856864E-4</v>
       </c>
       <c r="J95">
         <v>0.99959231704952622</v>
       </c>
       <c r="K95">
-        <v>6.4126440127278319E-7</v>
+        <v>1.3793867654802345E-6</v>
       </c>
       <c r="L95">
-        <v>0.99999988006304719</v>
+        <v>0.99999977629907244</v>
       </c>
     </row>
     <row r="96" spans="8:12" x14ac:dyDescent="0.35">
@@ -6034,16 +6082,16 @@
         <v>4.3</v>
       </c>
       <c r="I96">
-        <v>4.3668934832442088E-4</v>
+        <v>6.8127529043126569E-4</v>
       </c>
       <c r="J96">
         <v>0.99963906156478877</v>
       </c>
       <c r="K96">
-        <v>3.4646668191963948E-7</v>
+        <v>7.5568612893329128E-7</v>
       </c>
       <c r="L96">
-        <v>0.99999993655549446</v>
+        <v>0.99999988006304719</v>
       </c>
     </row>
     <row r="97" spans="8:12" x14ac:dyDescent="0.35">
@@ -6051,16 +6099,16 @@
         <v>4.3999999999999995</v>
       </c>
       <c r="I97">
-        <v>3.8225467277555944E-4</v>
+        <v>6.0234566151115142E-4</v>
       </c>
       <c r="J97">
         <v>0.99967994245286662</v>
       </c>
       <c r="K97">
-        <v>1.8460980860359997E-7</v>
+        <v>4.0828722933091742E-7</v>
       </c>
       <c r="L97">
-        <v>0.99999996688811787</v>
+        <v>0.99999993655549446</v>
       </c>
     </row>
     <row r="98" spans="8:12" x14ac:dyDescent="0.35">
@@ -6068,16 +6116,16 @@
         <v>4.4999999999999991</v>
       </c>
       <c r="I98">
-        <v>3.3518150336470754E-4</v>
+        <v>5.3347733494850847E-4</v>
       </c>
       <c r="J98">
         <v>0.99971575766102583</v>
       </c>
       <c r="K98">
-        <v>9.7010114438558822E-8</v>
+        <v>2.1755000176195073E-7</v>
       </c>
       <c r="L98">
-        <v>0.99999998295032966</v>
+        <v>0.99999996688811787</v>
       </c>
     </row>
     <row r="99" spans="8:12" x14ac:dyDescent="0.35">
@@ -6085,16 +6133,16 @@
         <v>4.5999999999999988</v>
       </c>
       <c r="I99">
-        <v>2.943978590340524E-4</v>
+        <v>4.7327495247416327E-4</v>
       </c>
       <c r="J99">
         <v>0.9997471882196507</v>
       </c>
       <c r="K99">
-        <v>5.0274552257759479E-8</v>
+        <v>1.1431976841681189E-7</v>
       </c>
       <c r="L99">
-        <v>0.99999999133867901</v>
+        <v>0.99999998295032966</v>
       </c>
     </row>
     <row r="100" spans="8:12" x14ac:dyDescent="0.35">
@@ -6102,16 +6150,16 @@
         <v>4.6999999999999984</v>
       </c>
       <c r="I100">
-        <v>2.5899871342338073E-4</v>
+        <v>4.2055173088343908E-4</v>
       </c>
       <c r="J100">
         <v>0.99977481656196399</v>
       </c>
       <c r="K100">
-        <v>2.5694984247864265E-8</v>
+        <v>5.9245112786729675E-8</v>
       </c>
       <c r="L100">
-        <v>0.99999999565907394</v>
+        <v>0.99999999133867901</v>
       </c>
     </row>
     <row r="101" spans="8:12" x14ac:dyDescent="0.35">
@@ -6119,16 +6167,16 @@
         <v>4.799999999999998</v>
       </c>
       <c r="I101">
-        <v>2.2821835536683484E-4</v>
+        <v>3.7429612776366692E-4</v>
       </c>
       <c r="J101">
         <v>0.99979914179298124</v>
       </c>
       <c r="K101">
-        <v>1.2951421863969333E-8</v>
+        <v>3.0279777172615305E-8</v>
       </c>
       <c r="L101">
-        <v>0.99999999785362736</v>
+        <v>0.99999999565907394</v>
       </c>
     </row>
     <row r="102" spans="8:12" x14ac:dyDescent="0.35">
@@ -6136,16 +6184,16 @@
         <v>4.8999999999999977</v>
       </c>
       <c r="I102">
-        <v>2.0140758585771506E-4</v>
+        <v>3.3364416311326613E-4</v>
       </c>
       <c r="J102">
         <v>0.99982059244457355</v>
       </c>
       <c r="K102">
-        <v>6.4380670222978091E-9</v>
+        <v>1.5262362659051862E-8</v>
       </c>
       <c r="L102">
-        <v>0.99999999895299929</v>
+        <v>0.99999999785362736</v>
       </c>
     </row>
     <row r="103" spans="8:12" x14ac:dyDescent="0.35">
@@ -6153,20 +6201,157 @@
         <v>4.9999999999999973</v>
       </c>
       <c r="I103">
-        <v>1.7801486164813004E-4</v>
+        <v>2.9785638450960893E-4</v>
       </c>
       <c r="J103">
         <v>0.99983953715420237</v>
       </c>
       <c r="K103">
-        <v>3.1561852577758855E-9</v>
+        <v>7.5868205629954428E-9</v>
       </c>
       <c r="L103">
-        <v>0.99999999949614815</v>
+        <v>0.99999999895299929</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71F1E49-69B3-41E4-B5F7-85CA4F6581D0}">
+  <dimension ref="B2:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" cm="1">
+        <f t="array" ref="C6">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
+        <v>1463763757296</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" cm="1">
+        <f t="array" ref="C7">_xll.JOHNSON.MOMENT(Johnson,1)</f>
+        <v>99.916681723477893</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" cm="1">
+        <f t="array" ref="C8">_xll.JOHNSON.MOMENT(Johnson,2) - C7*C7</f>
+        <v>0.72009759720276634</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" cm="1">
+        <f t="array" ref="C12">_xll.NORMAL.PUT.VALUE(f, s, k)</f>
+        <v>11.923538474048499</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" cm="1">
+        <f t="array" ref="C13">_xll.NORMAL.PUT.DELTA(f, s, k)</f>
+        <v>-0.4403823076297575</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" cm="1">
+        <f t="array" ref="C14">_xll.NORMAL.PUT.IMPLIED(f, value, k)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" cm="1">
+        <f t="array" ref="C15">_xll.JOHNSON.PUT.VALUE(Johnson,k)</f>
+        <v>0.35277488780918986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Do not divide share measure by mean.
</commit_message>
<xml_diff>
--- a/xll_johnson/johnson.xlsx
+++ b/xll_johnson/johnson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\keithalewis\fms_johnson\xll_johnson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A91A57-C8E4-47A1-948B-93ACF0E2630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F765FB4F-5DB0-4F86-993B-153AA4357C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{04679C06-6483-44F4-8D12-E76B362C6884}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{04679C06-6483-44F4-8D12-E76B362C6884}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,30 +19,32 @@
   <definedNames>
     <definedName name="cdf">_xlfn.ANCHORARRAY(Sheet1!$J$3)</definedName>
     <definedName name="delta" localSheetId="1">Sheet2!$C$3</definedName>
-    <definedName name="delta">Sheet1!$C$4</definedName>
+    <definedName name="delta">Sheet1!$C$6</definedName>
     <definedName name="f">Sheet2!$C$9</definedName>
     <definedName name="gamma" localSheetId="1">Sheet2!$C$2</definedName>
-    <definedName name="gamma">Sheet1!$C$3</definedName>
+    <definedName name="gamma">Sheet1!$C$5</definedName>
     <definedName name="implied">Sheet2!$C$14</definedName>
     <definedName name="Johnson" localSheetId="1">Sheet2!$C$6</definedName>
-    <definedName name="Johnson">Sheet1!$C$7</definedName>
+    <definedName name="Johnson">Sheet1!$C$9</definedName>
     <definedName name="k">Sheet2!$C$11</definedName>
     <definedName name="lambda" localSheetId="1">Sheet2!$C$5</definedName>
-    <definedName name="lambda">Sheet1!$C$6</definedName>
+    <definedName name="lambda">Sheet1!$C$4</definedName>
+    <definedName name="mean" localSheetId="0">Sheet1!$C$15</definedName>
     <definedName name="mean">Sheet2!$C$7</definedName>
-    <definedName name="mu">Sheet1!$C$13</definedName>
+    <definedName name="mu">Sheet1!$C$7</definedName>
     <definedName name="ncdf">_xlfn.ANCHORARRAY(Sheet1!$L$3)</definedName>
-    <definedName name="Normal">Sheet1!$C$15</definedName>
+    <definedName name="Normal">Sheet1!$C$17</definedName>
     <definedName name="npdf">_xlfn.ANCHORARRAY(Sheet1!$K$3)</definedName>
     <definedName name="pdf">_xlfn.ANCHORARRAY(Sheet1!$I$3)</definedName>
     <definedName name="s" localSheetId="1">Sheet2!$C$10</definedName>
     <definedName name="s">Sheet1!$C$2</definedName>
-    <definedName name="sigma">Sheet1!$C$14</definedName>
+    <definedName name="sigma">Sheet1!$C$8</definedName>
     <definedName name="value">Sheet2!$C$12</definedName>
+    <definedName name="variance" localSheetId="0">Sheet1!$C$16</definedName>
     <definedName name="variance">Sheet2!$C$8</definedName>
     <definedName name="x">_xlfn.ANCHORARRAY(Sheet1!$H$3)</definedName>
     <definedName name="xi" localSheetId="1">Sheet2!$C$4</definedName>
-    <definedName name="xi">Sheet1!$C$5</definedName>
+    <definedName name="xi">Sheet1!$C$3</definedName>
     <definedName name="Z">Sheet1!$C$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -88,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>xi</t>
   </si>
@@ -773,307 +775,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.5399836433269091E-4</c:v>
+                  <c:v>8.1325471509349561E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1211821774760813E-4</c:v>
+                  <c:v>8.3747258629299302E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7852629168763541E-4</c:v>
+                  <c:v>8.6254232474303633E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5452935795671087E-4</c:v>
+                  <c:v>8.8849868006336312E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4166034456623633E-4</c:v>
+                  <c:v>9.1537802129834696E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4172099301256791E-4</c:v>
+                  <c:v>9.4321842207431393E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5683322055249427E-4</c:v>
+                  <c:v>9.7205975075748729E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0895010941344631E-3</c:v>
+                  <c:v>1.0019437659376204E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2426857667214234E-3</c:v>
+                  <c:v>1.0329142175855919E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4198962794959649E-3</c:v>
+                  <c:v>1.065016954258232E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.625299822335634E-3</c:v>
+                  <c:v>1.0983000367506436E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8638559044121114E-3</c:v>
+                  <c:v>1.1328138586254344E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1414799598519774E-3</c:v>
+                  <c:v>1.1686112740796172E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4652432537375711E-3</c:v>
+                  <c:v>1.2057477336439642E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.843617627810908E-3</c:v>
+                  <c:v>1.2442814282461969E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2867757148734374E-3</c:v>
+                  <c:v>1.284273442209066E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.8069598556386285E-3</c:v>
+                  <c:v>1.3257879157972124E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.418936191114802E-3</c:v>
+                  <c:v>1.368892217973088E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1405544175295729E-3</c:v>
+                  <c:v>1.4136571300723934E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9934386381301956E-3</c:v>
+                  <c:v>1.4601570411638913E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.0038407971688699E-3</c:v>
+                  <c:v>1.5084701559173164E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.2036955008012603E-3</c:v>
+                  <c:v>1.5586787158670251E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.6319237426882517E-3</c:v>
+                  <c:v>1.6108692350282403E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1336043180833468E-2</c:v>
+                  <c:v>1.6651327508980198E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3374153962431681E-2</c:v>
+                  <c:v>1.721565091954598E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5817381060070058E-2</c:v>
+                  <c:v>1.7802671628575889E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.8752865321856195E-2</c:v>
+                  <c:v>1.8413452486478035E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2287403328615518E-2</c:v>
+                  <c:v>1.9049113393504295E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.6551835924275985E-2</c:v>
+                  <c:v>1.9710834764993337E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1706268651791748E-2</c:v>
+                  <c:v>2.0399861232245941E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.7946160369435343E-2</c:v>
+                  <c:v>2.1117505596806582E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.5509216377232126E-2</c:v>
+                  <c:v>2.1865153057401952E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.4682833672723648E-2</c:v>
+                  <c:v>2.2644265730395862E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.5811514016871256E-2</c:v>
+                  <c:v>2.3456387486377482E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.9303106330023757E-2</c:v>
+                  <c:v>2.4303149127418637E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.5631856999947168E-2</c:v>
+                  <c:v>2.5186273931632137E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.11533490846887444</c:v>
+                  <c:v>2.6107583593956138E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.13899698174264619</c:v>
+                  <c:v>2.7069004594597394E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.16721550635297847</c:v>
+                  <c:v>2.8072575029314045E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.20053573830560054</c:v>
+                  <c:v>2.9120451938725427E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.23934344697746879</c:v>
+                  <c:v>3.0214919177136917E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.28370383266135807</c:v>
+                  <c:v>3.1358395864985425E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.33314353279466052</c:v>
+                  <c:v>3.2553445472984291E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.38639348936483231</c:v>
+                  <c:v>3.3802785590409312E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.44114844502398848</c:v>
+                  <c:v>3.5109298434767423E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.49394968253813593</c:v>
+                  <c:v>3.6476042165363838E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.54033731014439135</c:v>
+                  <c:v>3.790626306909701E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.57539832144528535</c:v>
+                  <c:v>3.9403408693210326E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.59470715122605933</c:v>
+                  <c:v>4.0971142006786758E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.59542882121551766</c:v>
+                  <c:v>4.2613356680561013E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.57715962684987532</c:v>
+                  <c:v>4.4334193583221102E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.54210271839214386</c:v>
+                  <c:v>4.6138058601875501E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.49447256967407777</c:v>
+                  <c:v>4.8029641904868324E-4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.43940566781679591</c:v>
+                  <c:v>5.0013938776761015E-4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.38184618915061219</c:v>
+                  <c:v>5.2096272168181709E-4</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.32577559423885932</c:v>
+                  <c:v>5.4282317117530158E-4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.27390284321552266</c:v>
+                  <c:v>5.6578127217381724E-4</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.22772309026885401</c:v>
+                  <c:v>5.8990163316033795E-4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.18777406465475951</c:v>
+                  <c:v>6.1525324664212812E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.15394269159729695</c:v>
+                  <c:v>6.4190982738727758E-4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.12573535723614146</c:v>
+                  <c:v>6.6995017999100018E-4</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.10247924379988503</c:v>
+                  <c:v>6.9945859860222055E-4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.3454771452459969E-2</c:v>
+                  <c:v>7.3052530194237528E-4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.7973055423371204E-2</c:v>
+                  <c:v>7.6324690708499672E-4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.5414890241784878E-2</c:v>
+                  <c:v>7.9772694584083915E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.5245345804669039E-2</c:v>
+                  <c:v>8.3407642801426054E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.7014277081999572E-2</c:v>
+                  <c:v>8.7241445626796076E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.0349578854128156E-2</c:v>
+                  <c:v>9.128688978616771E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.4947380161910032E-2</c:v>
+                  <c:v>9.5557711912347377E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.0561569352483568E-2</c:v>
+                  <c:v>1.0006867891784866E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.6993892996149909E-2</c:v>
+                  <c:v>1.0483567602092266E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.4085184456303192E-2</c:v>
+                  <c:v>1.0987580323649731E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.1707890250092369E-2</c:v>
+                  <c:v>1.1520748123883687E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.7598597336093773E-3</c:v>
+                  <c:v>1.2085056760998375E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>8.1592698982939811E-3</c:v>
+                  <c:v>1.2682648460918813E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.8405242152831357E-3</c:v>
+                  <c:v>1.3315835973552292E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.7509635581052959E-3</c:v>
+                  <c:v>1.3987118051098106E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.8482414581218526E-3</c:v>
+                  <c:v>1.4699196508715442E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.0982359455794416E-3</c:v>
+                  <c:v>1.5454995047810504E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3.4733910783840906E-3</c:v>
+                  <c:v>1.6257680044873617E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2.9514005876051532E-3</c:v>
+                  <c:v>1.7110683534587493E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.5141629147183366E-3</c:v>
+                  <c:v>1.8017728645304777E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.1469510690586085E-3</c:v>
+                  <c:v>1.8982857778500318E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.8377523482641029E-3</c:v>
+                  <c:v>2.001046386206776E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.5767423466555525E-3</c:v>
+                  <c:v>2.1105325051088749E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.3558651751259989E-3</c:v>
+                  <c:v>2.2272643299805282E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.1684977660526561E-3</c:v>
+                  <c:v>2.3518087285976808E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.0091808349999151E-3</c:v>
+                  <c:v>2.4847840234761783E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>8.7340276935282755E-4</c:v>
+                  <c:v>2.6268653265101582E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>7.574256199980884E-4</c:v>
+                  <c:v>2.7787904968896416E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6.5814465358202286E-4</c:v>
+                  <c:v>2.9413668033931731E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.7297471375401332E-4</c:v>
+                  <c:v>3.11547838377419E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.9975804626297467E-4</c:v>
+                  <c:v>3.3020946073983762E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.3668934832442088E-4</c:v>
+                  <c:v>3.5022794628494416E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>3.8225467277555944E-4</c:v>
+                  <c:v>3.7172021102631963E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.3518150336470754E-4</c:v>
+                  <c:v>3.9481487591000912E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.943978590340524E-4</c:v>
+                  <c:v>4.1965360564283453E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.5899871342338073E-4</c:v>
+                  <c:v>4.4639261991581856E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.2821835536683484E-4</c:v>
+                  <c:v>4.7520440167479238E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0140758585771506E-4</c:v>
+                  <c:v>5.0627963095296429E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.7801486164813004E-4</c:v>
+                  <c:v>5.3982937729660481E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,307 +1432,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.2047300610986715E-4</c:v>
+                  <c:v>3.3409809180207084E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6871468417442053E-4</c:v>
+                  <c:v>3.4235103248658749E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2317271261348441E-4</c:v>
+                  <c:v>3.5085038291449155E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8473952524562556E-4</c:v>
+                  <c:v>3.5960483419117395E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.5444921734547634E-4</c:v>
+                  <c:v>3.6862343294619127E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3350222853063585E-4</c:v>
+                  <c:v>3.7791559794958518E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2329471234382501E-4</c:v>
+                  <c:v>3.8749113760405685E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.2545355505402327E-4</c:v>
+                  <c:v>3.9736026836517668E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0418782182627373E-3</c:v>
+                  <c:v>4.0753363414458565E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1747908416026576E-3</c:v>
+                  <c:v>4.1802232675458573E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3267963653426085E-3</c:v>
+                  <c:v>4.2883790745673611E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5009548333401734E-3</c:v>
+                  <c:v>4.3999242968095764E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7008685336363238E-3</c:v>
+                  <c:v>4.5149846298614404E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9307872510138657E-3</c:v>
+                  <c:v>4.6336911833849692E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1957356729779831E-3</c:v>
+                  <c:v>4.7561807478779805E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5016679451859702E-3</c:v>
+                  <c:v>4.8825960762854947E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.8556555607303635E-3</c:v>
+                  <c:v>5.0130861813879601E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.266116247183648E-3</c:v>
+                  <c:v>5.1478066499416331E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.7430933562233037E-3</c:v>
+                  <c:v>5.2869199746397033E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.2985975482454086E-3</c:v>
+                  <c:v>5.4305959050177099E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.9470254004463921E-3</c:v>
+                  <c:v>5.5790118185111703E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.7056730701632308E-3</c:v>
+                  <c:v>5.7323531129627181E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.5953674494610981E-3</c:v>
+                  <c:v>5.8908136219676388E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.6412424937365997E-3</c:v>
+                  <c:v>6.0545960545377309E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.8736947307866409E-3</c:v>
+                  <c:v>6.2239124606822127E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.0329559453804926E-2</c:v>
+                  <c:v>6.3989847246143094E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.2053557774557189E-2</c:v>
+                  <c:v>6.5800450874142768E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4100074371410087E-2</c:v>
+                  <c:v>6.7673367011206187E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.6535335860321854E-2</c:v>
+                  <c:v>6.9611142163672479E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.9440069055922549E-2</c:v>
+                  <c:v>7.1616444058353323E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2912724696017739E-2</c:v>
+                  <c:v>7.3692068259628707E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.7073351399755086E-2</c:v>
+                  <c:v>7.5840945195493337E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2068189760577293E-2</c:v>
+                  <c:v>7.8066147620731163E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.8075016121317418E-2</c:v>
+                  <c:v>8.0370898547799108E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.5309181693160505E-2</c:v>
+                  <c:v>8.2758579678143818E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.4030137936078082E-2</c:v>
+                  <c:v>8.5232740369423077E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.4547974393468432E-2</c:v>
+                  <c:v>8.7797107176706968E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7.7229068980227855E-2</c:v>
+                  <c:v>9.0455594008875817E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.2499304803588034E-2</c:v>
+                  <c:v>9.3212312944673803E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.11084239711217125</c:v>
+                  <c:v>9.6071585756402067E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.1327897166111156</c:v>
+                  <c:v>9.9037956193170906E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.15889676819044174</c:v>
+                  <c:v>1.0211620307984393E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.18970067882141106</c:v>
+                  <c:v>1.0531135429236449E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.22565364994386311</c:v>
+                  <c:v>1.0862870167527294E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.26703086079299182</c:v>
+                  <c:v>1.1207381697263541E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.31381938239430635</c:v>
+                  <c:v>1.1565256884952801E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.36560757076051598</c:v>
+                  <c:v>1.1937114108799274E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.42150877521786989</c:v>
+                  <c:v>1.2323605204815347E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.48016036015686281</c:v>
+                  <c:v>1.2725417549344087E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.53982783727702832</c:v>
+                  <c:v>1.3143276288702377E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.59861008809060445</c:v>
+                  <c:v>1.3577946727624246E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.65469786778660533</c:v>
+                  <c:v>1.4030236889187586E-3</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.70661049867299153</c:v>
+                  <c:v>1.4501000260063734E-3</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.75334475505344645</c:v>
+                  <c:v>1.4991138736132337E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.79440968148262048</c:v>
+                  <c:v>1.5501605784903338E-3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.82976508640009961</c:v>
+                  <c:v>1.6033409842656776E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.85970610254397384</c:v>
+                  <c:v>1.6587617965870827E-3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.88473649070521498</c:v>
+                  <c:v>1.7165359758324339E-3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.90545912867964717</c:v>
+                  <c:v>1.7767831597259032E-3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.92249563844821658</c:v>
+                  <c:v>1.8396301184185337E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.93643532470665591</c:v>
+                  <c:v>1.9052112448371128E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.9478077952472802</c:v>
+                  <c:v>1.9736690833725423E-3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.95707218903654212</c:v>
+                  <c:v>2.0451549002782343E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.96461676084963277</c:v>
+                  <c:v>2.1198292994776269E-3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.97076415638537239</c:v>
+                  <c:v>2.197862887846902E-3</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.97577926447744701</c:v>
+                  <c:v>2.2794369944418302E-3</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.97987775432362723</c:v>
+                  <c:v>2.3647444485889735E-3</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.98323425636184081</c:v>
+                  <c:v>2.453990422261354E-3</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.98598968932458764</c:v>
+                  <c:v>2.547393342712756E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.98825755897140199</c:v>
+                  <c:v>2.6451858819647178E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.99012923108926487</c:v>
+                  <c:v>2.7476160304289454E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.99167826820763394</c:v>
+                  <c:v>2.8549482627171496E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.99296395371698609</c:v>
+                  <c:v>2.9674648045471264E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.99403413258985318</c:v>
+                  <c:v>3.085467010615961E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.99492748909742335</c:v>
+                  <c:v>3.2092768643814384E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.99567536708715021</c:v>
+                  <c:v>3.3392386118973882E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99630322205337885</c:v>
+                  <c:v>3.4757205431962257E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.99683177866878769</c:v>
+                  <c:v>3.6191169362248532E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.99727795364724292</c:v>
+                  <c:v>3.7698501800405571E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.9976555920820569</c:v>
+                  <c:v>3.9283730958890595E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99797605569841419</c:v>
+                  <c:v>4.0951714769393299E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.99824869356626755</c:v>
+                  <c:v>4.2707668698832579E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.99848121947733492</c:v>
+                  <c:v>4.4557196243518171E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.99868001513339677</c:v>
+                  <c:v>4.6506322392025901E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.99885037428363677</c:v>
+                  <c:v>4.8561530382466578E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.99899669978044936</c:v>
+                  <c:v>5.0729802119631739E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.99912266302459396</c:v>
+                  <c:v>5.3018662662685512E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.99923133330214875</c:v>
+                  <c:v>5.5436229245410251E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.99932528296521794</c:v>
+                  <c:v>5.799126534942689E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.99940667318650722</c:v>
+                  <c:v>6.069324041737989E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.99947732405415812</c:v>
+                  <c:v>6.3552395869005962E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.99953877201214625</c:v>
+                  <c:v>6.6579818169792415E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.99959231704952622</c:v>
+                  <c:v>6.9787519801180475E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.99963906156478877</c:v>
+                  <c:v>7.31885290950407E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.99967994245286662</c:v>
+                  <c:v>7.6796990025644885E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.99971575766102583</c:v>
+                  <c:v>8.0628273202341671E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.9997471882196507</c:v>
+                  <c:v>8.4699099478720008E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.99977481656196399</c:v>
+                  <c:v>8.9027677792944959E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.99979914179298124</c:v>
+                  <c:v>9.3633859083501192E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.99982059244457355</c:v>
+                  <c:v>9.8539308389918312E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.99983953715420237</c:v>
+                  <c:v>1.0376769755518545E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2087,307 +2089,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>2.4129955889966093E-8</c:v>
+                  <c:v>5.8980677169218135E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7431684654640798E-8</c:v>
+                  <c:v>6.0492681129785834E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1949531688809475E-8</c:v>
+                  <c:v>6.2004681152684267E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7579213595838451E-7</c:v>
+                  <c:v>6.3514764117297243E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3145022194775128E-7</c:v>
+                  <c:v>6.50209733424989E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1631982102863674E-7</c:v>
+                  <c:v>6.6521312474688676E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1302197849724961E-6</c:v>
+                  <c:v>6.8013749594635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0440364018191555E-6</c:v>
+                  <c:v>6.9496221532749078E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6457198742106871E-6</c:v>
+                  <c:v>7.0966638381221789E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4127884815149315E-6</c:v>
+                  <c:v>7.2422888190370627E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1124473987528957E-5</c:v>
+                  <c:v>7.3862841835390672E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9031849904549581E-5</c:v>
+                  <c:v>7.5284358038701038E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2110825670618461E-5</c:v>
+                  <c:v>7.6685288532059942E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.3430703369420841E-5</c:v>
+                  <c:v>7.8063483341690262E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7679741268153059E-5</c:v>
+                  <c:v>7.9416796178787011E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.4189809909383787E-4</c:v>
+                  <c:v>8.0743089916978511E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2647634381399296E-4</c:v>
+                  <c:v>8.2040242137593714E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5648237506747424E-4</c:v>
+                  <c:v>8.3306150722949876E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.5337843369258552E-4</c:v>
+                  <c:v>8.4538739477327804E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.4717932134422715E-4</c:v>
+                  <c:v>8.5735963754845934E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2790791308723813E-3</c:v>
+                  <c:v>8.6895816073086982E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9045326811821897E-3</c:v>
+                  <c:v>8.8016331691074839E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.7967161827415145E-3</c:v>
+                  <c:v>8.909559413004578E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.0502078501963232E-3</c:v>
+                  <c:v>9.0131740615411945E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.7846245512400349E-3</c:v>
+                  <c:v>9.1122967418376583E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.1478306098394133E-3</c:v>
+                  <c:v>9.2067535075830792E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.1318210229330824E-2</c:v>
+                  <c:v>9.2963773467442182E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.5505382026789284E-2</c:v>
+                  <c:v>9.3810086729234451E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.0948654554711729E-2</c:v>
+                  <c:v>9.4604957983454835E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.7912500845991409E-2</c:v>
+                  <c:v>9.5346953865130993E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.667839412995362E-2</c:v>
+                  <c:v>9.6034728826426163E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.7532518548608807E-2</c:v>
+                  <c:v>9.6667029200712296E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.0749161720556701E-2</c:v>
+                  <c:v>9.7242697009187348E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.6570009734742317E-2</c:v>
+                  <c:v>9.7760673493863956E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.518007986163346E-2</c:v>
+                  <c:v>9.8220002361844805E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.11668160036602157</c:v>
+                  <c:v>9.8619832726972223E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.14106771739328908</c:v>
+                  <c:v>9.8959421736187367E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.16819839635435682</c:v>
+                  <c:v>9.9238136869252938E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.19778120212145192</c:v>
+                  <c:v>9.9455457901874281E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.2293597060532393</c:v>
+                  <c:v>9.9610978523690982E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.26231201537401122</c:v>
+                  <c:v>9.9704407604095449E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.29586132286154604</c:v>
+                  <c:v>9.9735570100358162E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.32909944888366083</c:v>
+                  <c:v>9.9704407604095449E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.361023161474819</c:v>
+                  <c:v>9.9610978523690996E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.39058173000049884</c:v>
+                  <c:v>9.9455457901874281E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.41673284805446192</c:v>
+                  <c:v>9.9238136869252938E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.43850292359506593</c:v>
+                  <c:v>9.8959421736187367E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.45504694401087509</c:v>
+                  <c:v>9.8619832726972223E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.46570281238686317</c:v>
+                  <c:v>9.8220002361844805E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.47003529342785944</c:v>
+                  <c:v>9.7760673493863956E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.46786550543392069</c:v>
+                  <c:v>9.7242697009187362E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.45928317340728742</c:v>
+                  <c:v>9.6667029200712296E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.44464047362342363</c:v>
+                  <c:v>9.6034728826426205E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.42452805815285793</c:v>
+                  <c:v>9.5346953865131007E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.39973553396848466</c:v>
+                  <c:v>9.4604957983454849E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.37120008122633552</c:v>
+                  <c:v>9.3810086729234465E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.33994786568104446</c:v>
+                  <c:v>9.2963773467442223E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.30703333139918837</c:v>
+                  <c:v>9.2067535075830834E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27348132826957205</c:v>
+                  <c:v>9.1122967418376624E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.2402363860289409</c:v>
+                  <c:v>9.0131740615411987E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.20812240753154615</c:v>
+                  <c:v>8.9095594130045822E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.17781477557172073</c:v>
+                  <c:v>8.8016331691074867E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.14982552236305358</c:v>
+                  <c:v>8.6895816073087023E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.12450096132240532</c:v>
+                  <c:v>8.5735963754845962E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.10203015791040425</c:v>
+                  <c:v>8.4538739477327859E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8.2461904818584827E-2</c:v>
+                  <c:v>8.3306150722949904E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>6.5727500316870441E-2</c:v>
+                  <c:v>8.2040242137593769E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.16665923868425E-2</c:v>
+                  <c:v>8.0743089916978567E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.0053592212178295E-2</c:v>
+                  <c:v>7.9416796178787052E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.0622600914242487E-2</c:v>
+                  <c:v>7.8063483341690304E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.3089345732782745E-2</c:v>
+                  <c:v>7.6685288532059998E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.7169202732841192E-2</c:v>
+                  <c:v>7.5284358038701094E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.2590923362052458E-2</c:v>
+                  <c:v>7.3862841835390741E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.106132848932677E-3</c:v>
+                  <c:v>7.2422888190370682E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6.4950026568476515E-3</c:v>
+                  <c:v>7.0966638381221817E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.568710441179645E-3</c:v>
+                  <c:v>6.9496221532749106E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>3.1693987659461372E-3</c:v>
+                  <c:v>6.8013749594635867E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2.168348504415149E-3</c:v>
+                  <c:v>6.6521312474688704E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.463019904504783E-3</c:v>
+                  <c:v>6.5020973342498914E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>9.7350981505563302E-4</c:v>
+                  <c:v>6.3514764117297243E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6.3885071313540126E-4</c:v>
+                  <c:v>6.2004681152684267E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.1345417627405937E-4</c:v>
+                  <c:v>6.0492681129785834E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.6389084995445336E-4</c:v>
+                  <c:v>5.8980677169218128E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.6610787810491804E-4</c:v>
+                  <c:v>5.7470535171058233E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.0311576754162756E-4</c:v>
+                  <c:v>5.5964070390809847E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6.3128995187286524E-5</c:v>
+                  <c:v>5.4463044258137625E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>3.8115500288447229E-5</c:v>
+                  <c:v>5.2969161443924849E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.2695686401474357E-5</c:v>
+                  <c:v>5.148406717999366E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.3327661967599159E-5</c:v>
+                  <c:v>5.0009344834621924E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>7.7185116848182121E-6</c:v>
+                  <c:v>4.8546513745803224E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.4084113568267356E-6</c:v>
+                  <c:v>4.7097027313031573E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.4831308687302349E-6</c:v>
+                  <c:v>4.5662271347255458E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.3793867654802345E-6</c:v>
+                  <c:v>4.4243562677544909E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>7.5568612893329128E-7</c:v>
+                  <c:v>4.2842148011951832E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.0828722933091742E-7</c:v>
+                  <c:v>4.1459203049026172E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2.1755000176195073E-7</c:v>
+                  <c:v>4.0095831835479899E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.1431976841681189E-7</c:v>
+                  <c:v>3.8753066364573305E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>5.9245112786729675E-8</c:v>
+                  <c:v>3.7431866408936226E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.0279777172615305E-8</c:v>
+                  <c:v>3.6133119580733238E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.5262362659051862E-8</c:v>
+                  <c:v>3.4857641611340084E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.5868205629954428E-9</c:v>
+                  <c:v>3.3606176842019796E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,307 +2746,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>3.437040041465167E-9</c:v>
+                  <c:v>0.15268159383311036</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8888383886189786E-9</c:v>
+                  <c:v>0.15865525393145713</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3621834660249021E-8</c:v>
+                  <c:v>0.16478012998031044</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6574140887802855E-8</c:v>
+                  <c:v>0.17105612630848172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1147335033974173E-8</c:v>
+                  <c:v>0.1774829537232322</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7125529341379746E-8</c:v>
+                  <c:v>0.18406012534675942</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8196891743427202E-7</c:v>
+                  <c:v>0.19078695285251052</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3637339674763567E-7</c:v>
+                  <c:v>0.19766254312269227</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1349960017720306E-7</c:v>
+                  <c:v>0.20468579534725251</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1040358424141417E-6</c:v>
+                  <c:v>0.21185539858339653</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.9603643926502379E-6</c:v>
+                  <c:v>0.21916982979337724</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4346633864257292E-6</c:v>
+                  <c:v>0.22662735237686799</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9379267369208399E-6</c:v>
+                  <c:v>0.23422601521269465</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0129753677645681E-5</c:v>
+                  <c:v>0.24196365222307276</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7052461216082726E-5</c:v>
+                  <c:v>0.24983788247177674</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.8327666707850252E-5</c:v>
+                  <c:v>0.2578461108058645</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.6438932026160451E-5</c:v>
+                  <c:v>0.26598552904870032</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.5130149028268534E-5</c:v>
+                  <c:v>0.27425311775007333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.199556345671815E-4</c:v>
+                  <c:v>0.28264564849720042</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8902363669015543E-4</c:v>
+                  <c:v>0.29115968678834614</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9397900284716671E-4</c:v>
+                  <c:v>0.29979159546869572</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5127159502306169E-4</c:v>
+                  <c:v>0.30853753872598666</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.837527541089794E-4</c:v>
+                  <c:v>0.31739348664125883</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0226305623681764E-3</c:v>
+                  <c:v>0.32635522028791986</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5097936510474752E-3</c:v>
+                  <c:v>0.33541833737016929</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.200481002527066E-3</c:v>
+                  <c:v>0.34457825838967565</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.1662305551806158E-3</c:v>
+                  <c:v>0.35383023332727603</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.4979827366486425E-3</c:v>
+                  <c:v>0.36316934882438068</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.3091485395969649E-3</c:v>
+                  <c:v>0.37259053584671581</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.738379999018886E-3</c:v>
+                  <c:v>0.38208857781104716</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.1951711127894171E-2</c:v>
+                  <c:v>0.39165811915360504</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6143679195266492E-2</c:v>
+                  <c:v>0.40129367431707608</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.1537001230033159E-2</c:v>
+                  <c:v>0.41098963713127024</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.8380381049400383E-2</c:v>
+                  <c:v>0.42074029056089679</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.6944069202113072E-2</c:v>
+                  <c:v>0.43053981679232617</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.7512900186882034E-2</c:v>
+                  <c:v>0.44038230762975733</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.0376691115162584E-2</c:v>
+                  <c:v>0.45026177516988697</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7.5818099411116724E-2</c:v>
+                  <c:v>0.4601721627229709</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.4098291512360543E-2</c:v>
+                  <c:v>0.47010735594710512</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.11544104856560938</c:v>
+                  <c:v>0.4800611941616274</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.1400162001061811</c:v>
+                  <c:v>0.49002748180476186</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.1679234992663976</c:v>
+                  <c:v>0.49999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.19917819908999618</c:v>
+                  <c:v>0.50997251819523792</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.23369962916910997</c:v>
+                  <c:v>0.51993880583837238</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.27130398448337512</c:v>
+                  <c:v>0.52989264405289471</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.31170231708788843</c:v>
+                  <c:v>0.53982783727702888</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.35450437574156468</c:v>
+                  <c:v>0.54973822483011281</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.39922849533890892</c:v>
+                  <c:v>0.55961769237024239</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.4453172388022601</c:v>
+                  <c:v>0.56946018320767355</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.49215799108738634</c:v>
+                  <c:v>0.57925970943910288</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.5391072542633486</c:v>
+                  <c:v>0.58901036286872954</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.58551704670180216</c:v>
+                  <c:v>0.5987063256829237</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.6307616096276677</c:v>
+                  <c:v>0.60834188084639473</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.67426259492032903</c:v>
+                  <c:v>0.61791142218895256</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.71551105270225679</c:v>
+                  <c:v>0.62740946415328391</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.75408483827835626</c:v>
+                  <c:v>0.63683065117561899</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.78966047915550108</c:v>
+                  <c:v>0.64616976667272374</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.82201903463938053</c:v>
+                  <c:v>0.65542174161032407</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.8510459871231203</c:v>
+                  <c:v>0.66458166262983043</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.87672567135600432</c:v>
+                  <c:v>0.67364477971207992</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.89913112989631394</c:v>
+                  <c:v>0.6826065133587409</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.91841054758371254</c:v>
+                  <c:v>0.69146246127401301</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.93477154988264299</c:v>
+                  <c:v>0.70020840453130395</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.9484646509808301</c:v>
+                  <c:v>0.70884031321165353</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.95976702402819636</c:v>
+                  <c:v>0.71735435150279925</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.96896756518996463</c:v>
+                  <c:v>0.72574688224992634</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.97635396851130229</c:v>
+                  <c:v>0.73401447095129935</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.98220225408289652</c:v>
+                  <c:v>0.74215388919413527</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.9867689282952028</c:v>
+                  <c:v>0.75016211752822293</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.9902857260411948</c:v>
+                  <c:v>0.75803634777692697</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.99295670616128739</c:v>
+                  <c:v>0.76577398478730496</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.99495735016618658</c:v>
+                  <c:v>0.77337264762313174</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.99643524956985763</c:v>
+                  <c:v>0.78083017020662249</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.99751195232230505</c:v>
+                  <c:v>0.78814460141660314</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.99828556336816709</c:v>
+                  <c:v>0.79531420465274738</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.9988337461459853</c:v>
+                  <c:v>0.80233745687730762</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99921683895094049</c:v>
+                  <c:v>0.80921304714748943</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.99948087211676628</c:v>
+                  <c:v>0.81593987465324047</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.99966034087037814</c:v>
+                  <c:v>0.82251704627676769</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.9997806490298029</c:v>
+                  <c:v>0.82894387369151823</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99986018749144967</c:v>
+                  <c:v>0.83521987001968956</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.99991204780711773</c:v>
+                  <c:v>0.84134474606854281</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.9999453957451081</c:v>
+                  <c:v>0.84731840616688969</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.99996654420133968</c:v>
+                  <c:v>0.85314094362410409</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.99997977128828142</c:v>
+                  <c:v>0.85881263583487111</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.99998793007523878</c:v>
+                  <c:v>0.86433393905361733</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.99999289328717444</c:v>
+                  <c:v>0.86970548286319116</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.99999587095251719</c:v>
+                  <c:v>0.87492806436284987</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.99999763278569898</c:v>
+                  <c:v>0.88000264210098744</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.99999866087185763</c:v>
+                  <c:v>0.88493032977829178</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.99999925252893296</c:v>
+                  <c:v>0.88971238974714872</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.99999958833337033</c:v>
+                  <c:v>0.89435022633314476</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.99999977629907244</c:v>
+                  <c:v>0.89884537900441408</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.99999988006304719</c:v>
+                  <c:v>0.9031995154143897</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.99999993655549446</c:v>
+                  <c:v>0.90741442434320507</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.99999996688811787</c:v>
+                  <c:v>0.91149200856259793</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.99999998295032966</c:v>
+                  <c:v>0.91543427764866436</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.99999999133867901</c:v>
+                  <c:v>0.91924334076622882</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.99999999565907394</c:v>
+                  <c:v>0.92292139944792806</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.99999999785362736</c:v>
+                  <c:v>0.9264707403903516</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.99999999895299929</c:v>
+                  <c:v>0.9298937282887767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4190,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F0A76B-08E5-40E0-BCFA-A9D795A3DB2C}">
   <dimension ref="B1:L103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -4205,12 +4207,12 @@
   <sheetData>
     <row r="1" spans="2:12" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I1" s="3">
-        <f>1-SUM(pdf)*D17</f>
-        <v>5.4997005830159651E-4</v>
+        <f>1-SUM(pdf)*D19</f>
+        <v>0.98968046230571172</v>
       </c>
       <c r="K1" s="3">
-        <f>1-SUM(npdf)*D17</f>
-        <v>3.0788288585270607E-9</v>
+        <f>1-SUM(npdf)*D19</f>
+        <v>0.2181814449184053</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
@@ -4238,81 +4240,81 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="H3" cm="1">
-        <f t="array" ref="H3:H103">_xlfn.SEQUENCE(1+(C17-B17)/D17,1,B17,D17)</f>
+        <f t="array" ref="H3:H103">_xlfn.SEQUENCE(1+(C19-B19)/D19,1,B19,D19)</f>
         <v>-5</v>
       </c>
       <c r="I3" cm="1">
         <f t="array" ref="I3:I103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Johnson,_xlpm.x,s)))</f>
-        <v>4.5399836433269091E-4</v>
+        <v>8.1325471509349561E-5</v>
       </c>
       <c r="J3" cm="1">
         <f t="array" ref="J3:J103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Johnson,_xlpm.x,s)))</f>
-        <v>4.2047300610986715E-4</v>
+        <v>3.3409809180207084E-4</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" ref="K3:K103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.PDF(Normal,_xlpm.x,s)))</f>
-        <v>2.4129955889966093E-8</v>
+        <v>5.8980677169218135E-2</v>
       </c>
       <c r="L3" cm="1">
         <f t="array" ref="L3:L103">_xlfn.MAP(x,_xlfn.LAMBDA(_xlpm.x,_xll.VARIATE.CDF(Normal,_xlpm.x,s)))</f>
-        <v>3.437040041465167E-9</v>
+        <v>0.15268159383311036</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>-4.9000000000000004</v>
       </c>
       <c r="I4">
-        <v>5.1211821774760813E-4</v>
+        <v>8.3747258629299302E-5</v>
       </c>
       <c r="J4">
-        <v>4.6871468417442053E-4</v>
+        <v>3.4235103248658749E-4</v>
       </c>
       <c r="K4">
-        <v>4.7431684654640798E-8</v>
+        <v>6.0492681129785834E-2</v>
       </c>
       <c r="L4">
-        <v>6.8888383886189786E-9</v>
+        <v>0.15865525393145713</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>0</v>
-      </c>
-      <c r="C5">
-        <v>-0.1</v>
       </c>
       <c r="H5">
         <v>-4.8000000000000007</v>
       </c>
       <c r="I5">
-        <v>5.7852629168763541E-4</v>
+        <v>8.6254232474303633E-5</v>
       </c>
       <c r="J5">
-        <v>5.2317271261348441E-4</v>
+        <v>3.5085038291449155E-4</v>
       </c>
       <c r="K5">
-        <v>9.1949531688809475E-8</v>
+        <v>6.2004681152684267E-2</v>
       </c>
       <c r="L5">
-        <v>1.3621834660249021E-8</v>
+        <v>0.16478012998031044</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4321,275 +4323,278 @@
         <v>-4.7000000000000011</v>
       </c>
       <c r="I6">
-        <v>6.5452935795671087E-4</v>
+        <v>8.8849868006336312E-5</v>
       </c>
       <c r="J6">
-        <v>5.8473952524562556E-4</v>
+        <v>3.5960483419117395E-4</v>
       </c>
       <c r="K6">
-        <v>1.7579213595838451E-7</v>
+        <v>6.3514764117297243E-2</v>
       </c>
       <c r="L6">
-        <v>2.6574140887802855E-8</v>
+        <v>0.17105612630848172</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" cm="1">
-        <f t="array" ref="C7">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
-        <v>2046863984336</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="H7">
         <v>-4.6000000000000014</v>
       </c>
       <c r="I7">
-        <v>7.4166034456623633E-4</v>
+        <v>9.1537802129834696E-5</v>
       </c>
       <c r="J7">
-        <v>6.5444921734547634E-4</v>
+        <v>3.6862343294619127E-4</v>
       </c>
       <c r="K7">
-        <v>3.3145022194775128E-7</v>
+        <v>6.50209733424989E-2</v>
       </c>
       <c r="L7">
-        <v>5.1147335033974173E-8</v>
+        <v>0.1774829537232322</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
-        <v>8</v>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
       </c>
       <c r="H8">
         <v>-4.5000000000000018</v>
       </c>
       <c r="I8">
-        <v>8.4172099301256791E-4</v>
+        <v>9.4321842207431393E-5</v>
       </c>
       <c r="J8">
-        <v>7.3350222853063585E-4</v>
+        <v>3.7791559794958518E-4</v>
       </c>
       <c r="K8">
-        <v>6.1631982102863674E-7</v>
+        <v>6.6521312474688676E-2</v>
       </c>
       <c r="L8">
-        <v>9.7125529341379746E-8</v>
+        <v>0.18406012534675942</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" cm="1">
-        <f t="array" ref="C9">_xll.JOHNSON.MOMENT(Johnson,B9)</f>
-        <v>-0.18331827652210433</v>
-      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" cm="1">
+        <f t="array" ref="C9">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
+        <v>2540972209616</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="H9">
         <v>-4.4000000000000021</v>
       </c>
       <c r="I9">
-        <v>9.5683322055249427E-4</v>
+        <v>9.7205975075748729E-5</v>
       </c>
       <c r="J9">
-        <v>8.2329471234382501E-4</v>
+        <v>3.8749113760405685E-4</v>
       </c>
       <c r="K9">
-        <v>1.1302197849724961E-6</v>
+        <v>6.8013749594635853E-2</v>
       </c>
       <c r="L9">
-        <v>1.8196891743427202E-7</v>
+        <v>0.19078695285251052</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" cm="1">
-        <f t="array" ref="C10">_xll.JOHNSON.MOMENT(Johnson,B10)</f>
-        <v>0.753703187708885</v>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="H10">
         <v>-4.3000000000000025</v>
       </c>
       <c r="I10">
-        <v>1.0895010941344631E-3</v>
+        <v>1.0019437659376204E-4</v>
       </c>
       <c r="J10">
-        <v>9.2545355505402327E-4</v>
+        <v>3.9736026836517668E-4</v>
       </c>
       <c r="K10">
-        <v>2.0440364018191555E-6</v>
+        <v>6.9496221532749078E-2</v>
       </c>
       <c r="L10">
-        <v>3.3637339674763567E-7</v>
+        <v>0.19766254312269227</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" cm="1">
         <f t="array" ref="C11">_xll.JOHNSON.MOMENT(Johnson,B11)</f>
-        <v>-0.53104345500307115</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>-4.2000000000000028</v>
       </c>
       <c r="I11">
-        <v>1.2426857667214234E-3</v>
+        <v>1.0329142175855919E-4</v>
       </c>
       <c r="J11">
-        <v>1.0418782182627373E-3</v>
+        <v>4.0753363414458565E-4</v>
       </c>
       <c r="K11">
-        <v>3.6457198742106871E-6</v>
+        <v>7.0966638381221789E-2</v>
       </c>
       <c r="L11">
-        <v>6.1349960017720306E-7</v>
+        <v>0.20468579534725251</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" cm="1">
         <f t="array" ref="C12">_xll.JOHNSON.MOMENT(Johnson,B12)</f>
-        <v>3.8482088381788087</v>
+        <v>103.19452804946532</v>
       </c>
       <c r="H12">
         <v>-4.1000000000000032</v>
       </c>
       <c r="I12">
-        <v>1.4198962794959649E-3</v>
+        <v>1.065016954258232E-4</v>
       </c>
       <c r="J12">
-        <v>1.1747908416026576E-3</v>
+        <v>4.1802232675458573E-4</v>
       </c>
       <c r="K12">
-        <v>6.4127884815149315E-6</v>
+        <v>7.2422888190370627E-2</v>
       </c>
       <c r="L12">
-        <v>1.1040358424141417E-6</v>
+        <v>0.21185539858339653</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <f>C9</f>
-        <v>-0.18331827652210433</v>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" cm="1">
+        <f t="array" ref="C13">_xll.JOHNSON.MOMENT(Johnson,B13)</f>
+        <v>1095.8358414839597</v>
       </c>
       <c r="H13">
         <v>-4.0000000000000036</v>
       </c>
       <c r="I13">
-        <v>1.625299822335634E-3</v>
+        <v>1.0983000367506436E-4</v>
       </c>
       <c r="J13">
-        <v>1.3267963653426085E-3</v>
+        <v>4.2883790745673611E-4</v>
       </c>
       <c r="K13">
-        <v>1.1124473987528957E-5</v>
+        <v>7.3862841835390672E-2</v>
       </c>
       <c r="L13">
-        <v>1.9603643926502379E-6</v>
+        <v>0.21916982979337724</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <f>SQRT(C10-C9^2)</f>
-        <v>0.84858564517781598</v>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" cm="1">
+        <f t="array" ref="C14">_xll.JOHNSON.MOMENT(Johnson,B14)</f>
+        <v>12286.017050009947</v>
       </c>
       <c r="H14">
         <v>-3.9000000000000035</v>
       </c>
       <c r="I14">
-        <v>1.8638559044121114E-3</v>
+        <v>1.1328138586254344E-4</v>
       </c>
       <c r="J14">
-        <v>1.5009548333401734E-3</v>
+        <v>4.3999242968095764E-4</v>
       </c>
       <c r="K14">
-        <v>1.9031849904549581E-5</v>
+        <v>7.5284358038701038E-2</v>
       </c>
       <c r="L14">
-        <v>3.4346633864257292E-6</v>
+        <v>0.22662735237686799</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" cm="1">
-        <f t="array" ref="C15">_xll.\VARIATE.NORMAL(mu, sigma)</f>
-        <v>2047804073264</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <f>C11</f>
+        <v>10</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="H15">
         <v>-3.8000000000000034</v>
       </c>
       <c r="I15">
-        <v>2.1414799598519774E-3</v>
+        <v>1.1686112740796172E-4</v>
       </c>
       <c r="J15">
-        <v>1.7008685336363238E-3</v>
+        <v>4.5149846298614404E-4</v>
       </c>
       <c r="K15">
-        <v>3.2110825670618461E-5</v>
+        <v>7.6685288532059942E-2</v>
       </c>
       <c r="L15">
-        <v>5.9379267369208399E-6</v>
+        <v>0.23422601521269465</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <f>SQRT(C12-C11^2)</f>
+        <v>1.787324270932759</v>
+      </c>
       <c r="H16">
         <v>-3.7000000000000033</v>
       </c>
       <c r="I16">
-        <v>2.4652432537375711E-3</v>
+        <v>1.2057477336439642E-4</v>
       </c>
       <c r="J16">
-        <v>1.9307872510138657E-3</v>
+        <v>4.6336911833849692E-4</v>
       </c>
       <c r="K16">
-        <v>5.3430703369420841E-5</v>
+        <v>7.8063483341690262E-2</v>
       </c>
       <c r="L16">
-        <v>1.0129753677645681E-5</v>
+        <v>0.24196365222307276</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17">
-        <v>-5</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>0.1</v>
-      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" cm="1">
+        <f t="array" ref="C17">_xll.\VARIATE.NORMAL(mu, sigma)</f>
+        <v>2541180997344</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="H17">
         <v>-3.6000000000000032</v>
       </c>
       <c r="I17">
-        <v>2.843617627810908E-3</v>
+        <v>1.2442814282461969E-4</v>
       </c>
       <c r="J17">
-        <v>2.1957356729779831E-3</v>
+        <v>4.7561807478779805E-4</v>
       </c>
       <c r="K17">
-        <v>8.7679741268153059E-5</v>
+        <v>7.9416796178787011E-2</v>
       </c>
       <c r="L17">
-        <v>1.7052461216082726E-5</v>
+        <v>0.24983788247177674</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
@@ -4597,33 +4602,42 @@
         <v>-3.5000000000000031</v>
       </c>
       <c r="I18">
-        <v>3.2867757148734374E-3</v>
+        <v>1.284273442209066E-4</v>
       </c>
       <c r="J18">
-        <v>2.5016679451859702E-3</v>
+        <v>4.8825960762854947E-4</v>
       </c>
       <c r="K18">
-        <v>1.4189809909383787E-4</v>
+        <v>8.0743089916978511E-2</v>
       </c>
       <c r="L18">
-        <v>2.8327666707850252E-5</v>
+        <v>0.2578461108058645</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>-5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
       <c r="H19">
         <v>-3.400000000000003</v>
       </c>
       <c r="I19">
-        <v>3.8069598556386285E-3</v>
+        <v>1.3257879157972124E-4</v>
       </c>
       <c r="J19">
-        <v>2.8556555607303635E-3</v>
+        <v>5.0130861813879601E-4</v>
       </c>
       <c r="K19">
-        <v>2.2647634381399296E-4</v>
+        <v>8.2040242137593714E-2</v>
       </c>
       <c r="L19">
-        <v>4.6438932026160451E-5</v>
+        <v>0.26598552904870032</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
@@ -4631,16 +4645,16 @@
         <v>-3.3000000000000029</v>
       </c>
       <c r="I20">
-        <v>4.418936191114802E-3</v>
+        <v>1.368892217973088E-4</v>
       </c>
       <c r="J20">
-        <v>3.266116247183648E-3</v>
+        <v>5.1478066499416331E-4</v>
       </c>
       <c r="K20">
-        <v>3.5648237506747424E-4</v>
+        <v>8.3306150722949876E-2</v>
       </c>
       <c r="L20">
-        <v>7.5130149028268534E-5</v>
+        <v>0.27425311775007333</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
@@ -4649,30 +4663,30 @@
       </c>
       <c r="C21">
         <f ca="1">_xlfn.NORM.S.INV(RAND())</f>
-        <v>-0.71470218777855732</v>
-      </c>
-      <c r="E21">
+        <v>0.79626444700830856</v>
+      </c>
+      <c r="E21" t="e">
         <f t="array" aca="1" ref="E21:F21" ca="1">_xll.MONTE.STDEV(Z)</f>
-        <v>0</v>
-      </c>
-      <c r="F21">
+        <v>#NAME?</v>
+      </c>
+      <c r="F21" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="H21">
         <v>-3.2000000000000028</v>
       </c>
       <c r="I21">
-        <v>5.1405544175295729E-3</v>
+        <v>1.4136571300723934E-4</v>
       </c>
       <c r="J21">
-        <v>3.7430933562233037E-3</v>
+        <v>5.2869199746397033E-4</v>
       </c>
       <c r="K21">
-        <v>5.5337843369258552E-4</v>
+        <v>8.4538739477327804E-2</v>
       </c>
       <c r="L21">
-        <v>1.199556345671815E-4</v>
+        <v>0.28264564849720042</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
@@ -4681,30 +4695,30 @@
       </c>
       <c r="C22">
         <f ca="1">(Z-gamma)/delta</f>
-        <v>-0.54313479185237157</v>
-      </c>
-      <c r="E22">
+        <v>0.79626444700830856</v>
+      </c>
+      <c r="E22" t="e">
         <f t="array" aca="1" ref="E22:F22" ca="1">_xll.MONTE.STDEV(C22)</f>
-        <v>0</v>
-      </c>
-      <c r="F22">
+        <v>#NAME?</v>
+      </c>
+      <c r="F22" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="H22">
         <v>-3.1000000000000028</v>
       </c>
       <c r="I22">
-        <v>5.9934386381301956E-3</v>
+        <v>1.4601570411638913E-4</v>
       </c>
       <c r="J22">
-        <v>4.2985975482454086E-3</v>
+        <v>5.4305959050177099E-4</v>
       </c>
       <c r="K22">
-        <v>8.4717932134422715E-4</v>
+        <v>8.5735963754845934E-2</v>
       </c>
       <c r="L22">
-        <v>1.8902363669015543E-4</v>
+        <v>0.29115968678834614</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
@@ -4713,30 +4727,30 @@
       </c>
       <c r="C23">
         <f ca="1">SINH(C22)</f>
-        <v>-0.57023515432115079</v>
-      </c>
-      <c r="E23">
+        <v>0.88311610793408302</v>
+      </c>
+      <c r="E23" t="e">
         <f t="array" aca="1" ref="E23:F23" ca="1">_xll.MONTE.STDEV(C23)</f>
-        <v>0</v>
-      </c>
-      <c r="F23">
+        <v>#NAME?</v>
+      </c>
+      <c r="F23" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="H23">
         <v>-3.0000000000000027</v>
       </c>
       <c r="I23">
-        <v>7.0038407971688699E-3</v>
+        <v>1.5084701559173164E-4</v>
       </c>
       <c r="J23">
-        <v>4.9470254004463921E-3</v>
+        <v>5.5790118185111703E-4</v>
       </c>
       <c r="K23">
-        <v>1.2790791308723813E-3</v>
+        <v>8.6895816073086982E-2</v>
       </c>
       <c r="L23">
-        <v>2.9397900284716671E-4</v>
+        <v>0.29979159546869572</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
@@ -4745,38 +4759,38 @@
       </c>
       <c r="C24">
         <f ca="1">POWER($C$23,B24)</f>
-        <v>-0.57023515432115079</v>
+        <v>0.88311610793408302</v>
       </c>
       <c r="D24" cm="1">
         <f t="array" ref="D24">_xll.JOHNSON.Esinh_k(Johnson,B24)</f>
-        <v>-8.3318276522104329E-2</v>
-      </c>
-      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="e">
         <f t="array" aca="1" ref="E24:F24" ca="1">_xll.MONTE.STDEV(C24)</f>
-        <v>0</v>
-      </c>
-      <c r="F24">
+        <v>#NAME?</v>
+      </c>
+      <c r="F24" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="G24" t="e">
         <f ca="1">(D24-E24)/F24</f>
-        <v>#DIV/0!</v>
+        <v>#NAME?</v>
       </c>
       <c r="H24">
         <v>-2.9000000000000026</v>
       </c>
       <c r="I24">
-        <v>8.2036955008012603E-3</v>
+        <v>1.5586787158670251E-4</v>
       </c>
       <c r="J24">
-        <v>5.7056730701632308E-3</v>
+        <v>5.7323531129627181E-4</v>
       </c>
       <c r="K24">
-        <v>1.9045326811821897E-3</v>
+        <v>8.8016331691074839E-2</v>
       </c>
       <c r="L24">
-        <v>4.5127159502306169E-4</v>
+        <v>0.30853753872598666</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
@@ -4785,38 +4799,38 @@
       </c>
       <c r="C25">
         <f ca="1">POWER($C$23,B25)</f>
-        <v>0.32516813122366667</v>
+        <v>0.77989406009264295</v>
       </c>
       <c r="D25" cm="1">
         <f t="array" ref="D25">_xll.JOHNSON.Esinh_k(Johnson,B25)</f>
-        <v>0.72703953240446417</v>
-      </c>
-      <c r="E25">
+        <v>3.1945280494653252</v>
+      </c>
+      <c r="E25" t="e">
         <f t="array" aca="1" ref="E25:F25" ca="1">_xll.MONTE.STDEV(C25)</f>
-        <v>0</v>
-      </c>
-      <c r="F25">
+        <v>#NAME?</v>
+      </c>
+      <c r="F25" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="G25" t="e">
         <f ca="1">(D25-E25)/F25</f>
-        <v>#DIV/0!</v>
+        <v>#NAME?</v>
       </c>
       <c r="H25">
         <v>-2.8000000000000025</v>
       </c>
       <c r="I25">
-        <v>9.6319237426882517E-3</v>
+        <v>1.6108692350282403E-4</v>
       </c>
       <c r="J25">
-        <v>6.5953674494610981E-3</v>
+        <v>5.8908136219676388E-4</v>
       </c>
       <c r="K25">
-        <v>2.7967161827415145E-3</v>
+        <v>8.909559413004578E-2</v>
       </c>
       <c r="L25">
-        <v>6.837527541089794E-4</v>
+        <v>0.31739348664125883</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
@@ -4825,38 +4839,38 @@
       </c>
       <c r="C26">
         <f ca="1">POWER($C$23,B26)</f>
-        <v>-0.18542229948864777</v>
+        <v>0.68873700694992468</v>
       </c>
       <c r="D26" cm="1">
         <f t="array" ref="D26">_xll.JOHNSON.Esinh_k(Johnson,B26)</f>
-        <v>-0.30943204698606874</v>
-      </c>
-      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="e">
         <f t="array" aca="1" ref="E26:F26" ca="1">_xll.MONTE.STDEV(C26)</f>
-        <v>0</v>
-      </c>
-      <c r="F26">
+        <v>#NAME?</v>
+      </c>
+      <c r="F26" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="G26" t="e">
         <f ca="1">(D26-E26)/F26</f>
-        <v>#DIV/0!</v>
+        <v>#NAME?</v>
       </c>
       <c r="H26">
         <v>-2.7000000000000024</v>
       </c>
       <c r="I26">
-        <v>1.1336043180833468E-2</v>
+        <v>1.6651327508980198E-4</v>
       </c>
       <c r="J26">
-        <v>7.6412424937365997E-3</v>
+        <v>6.0545960545377309E-4</v>
       </c>
       <c r="K26">
-        <v>4.0502078501963232E-3</v>
+        <v>9.0131740615411945E-2</v>
       </c>
       <c r="L26">
-        <v>1.0226305623681764E-3</v>
+        <v>0.32635522028791986</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
@@ -4865,38 +4879,38 @@
       </c>
       <c r="C27">
         <f ca="1">POWER($C$23,B27)</f>
-        <v>0.10573431356349171</v>
+        <v>0.60823474496778696</v>
       </c>
       <c r="D27" cm="1">
         <f t="array" ref="D27">_xll.JOHNSON.Esinh_k(Johnson,B27)</f>
-        <v>3.6803803743340247</v>
-      </c>
-      <c r="E27">
+        <v>369.30022033075073</v>
+      </c>
+      <c r="E27" t="e">
         <f t="array" aca="1" ref="E27:F27" ca="1">_xll.MONTE.STDEV(C27)</f>
-        <v>0</v>
-      </c>
-      <c r="F27">
+        <v>#NAME?</v>
+      </c>
+      <c r="F27" t="e">
         <f ca="1"/>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="G27" t="e">
         <f ca="1">(D27-E27)/F27</f>
-        <v>#DIV/0!</v>
+        <v>#NAME?</v>
       </c>
       <c r="H27">
         <v>-2.6000000000000023</v>
       </c>
       <c r="I27">
-        <v>1.3374153962431681E-2</v>
+        <v>1.721565091954598E-4</v>
       </c>
       <c r="J27">
-        <v>8.8736947307866409E-3</v>
+        <v>6.2239124606822127E-4</v>
       </c>
       <c r="K27">
-        <v>5.7846245512400349E-3</v>
+        <v>9.1122967418376583E-2</v>
       </c>
       <c r="L27">
-        <v>1.5097936510474752E-3</v>
+        <v>0.33541833737016929</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
@@ -4904,16 +4918,16 @@
         <v>-2.5000000000000022</v>
       </c>
       <c r="I28">
-        <v>1.5817381060070058E-2</v>
+        <v>1.7802671628575889E-4</v>
       </c>
       <c r="J28">
-        <v>1.0329559453804926E-2</v>
+        <v>6.3989847246143094E-4</v>
       </c>
       <c r="K28">
-        <v>8.1478306098394133E-3</v>
+        <v>9.2067535075830792E-2</v>
       </c>
       <c r="L28">
-        <v>2.200481002527066E-3</v>
+        <v>0.34457825838967565</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
@@ -4922,38 +4936,38 @@
       </c>
       <c r="C29" cm="1">
         <f t="array" aca="1" ref="C29" ca="1">_xll.JOHNSON.X(Johnson,Z)</f>
-        <v>-0.67023515432115066</v>
+        <v>10.883116107934082</v>
       </c>
       <c r="D29">
         <f>mu</f>
-        <v>-0.18331827652210433</v>
+        <v>-1</v>
       </c>
       <c r="E29" t="e">
         <f t="array" aca="1" ref="E29:F29" ca="1">_xll.MONTE.STDEV(C29)</f>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="F29" t="e">
         <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="G29" t="e">
         <f ca="1">(D29-E29)/F29</f>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="H29">
         <v>-2.4000000000000021</v>
       </c>
       <c r="I29">
-        <v>1.8752865321856195E-2</v>
+        <v>1.8413452486478035E-4</v>
       </c>
       <c r="J29">
-        <v>1.2053557774557189E-2</v>
+        <v>6.5800450874142768E-4</v>
       </c>
       <c r="K29">
-        <v>1.1318210229330824E-2</v>
+        <v>9.2963773467442182E-2</v>
       </c>
       <c r="L29">
-        <v>3.1662305551806158E-3</v>
+        <v>0.35383023332727603</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
@@ -4961,16 +4975,16 @@
         <v>-2.300000000000002</v>
       </c>
       <c r="I30">
-        <v>2.2287403328615518E-2</v>
+        <v>1.9049113393504295E-4</v>
       </c>
       <c r="J30">
-        <v>1.4100074371410087E-2</v>
+        <v>6.7673367011206187E-4</v>
       </c>
       <c r="K30">
-        <v>1.5505382026789284E-2</v>
+        <v>9.3810086729234451E-2</v>
       </c>
       <c r="L30">
-        <v>4.4979827366486425E-3</v>
+        <v>0.36316934882438068</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
@@ -4978,16 +4992,16 @@
         <v>-2.200000000000002</v>
       </c>
       <c r="I31">
-        <v>2.6551835924275985E-2</v>
+        <v>1.9710834764993337E-4</v>
       </c>
       <c r="J31">
-        <v>1.6535335860321854E-2</v>
+        <v>6.9611142163672479E-4</v>
       </c>
       <c r="K31">
-        <v>2.0948654554711729E-2</v>
+        <v>9.4604957983454835E-2</v>
       </c>
       <c r="L31">
-        <v>6.3091485395969649E-3</v>
+        <v>0.37259053584671581</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
@@ -4995,16 +5009,16 @@
         <v>-2.1000000000000019</v>
       </c>
       <c r="I32">
-        <v>3.1706268651791748E-2</v>
+        <v>2.0399861232245941E-4</v>
       </c>
       <c r="J32">
-        <v>1.9440069055922549E-2</v>
+        <v>7.1616444058353323E-4</v>
       </c>
       <c r="K32">
-        <v>2.7912500845991409E-2</v>
+        <v>9.5346953865130993E-2</v>
       </c>
       <c r="L32">
-        <v>8.738379999018886E-3</v>
+        <v>0.38208857781104716</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.35">
@@ -5012,16 +5026,16 @@
         <v>-2.0000000000000018</v>
       </c>
       <c r="I33">
-        <v>3.7946160369435343E-2</v>
+        <v>2.1117505596806582E-4</v>
       </c>
       <c r="J33">
-        <v>2.2912724696017739E-2</v>
+        <v>7.3692068259628707E-4</v>
       </c>
       <c r="K33">
-        <v>3.667839412995362E-2</v>
+        <v>9.6034728826426163E-2</v>
       </c>
       <c r="L33">
-        <v>1.1951711127894171E-2</v>
+        <v>0.39165811915360504</v>
       </c>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.35">
@@ -5029,16 +5043,16 @@
         <v>-1.9000000000000017</v>
       </c>
       <c r="I34">
-        <v>4.5509216377232126E-2</v>
+        <v>2.1865153057401952E-4</v>
       </c>
       <c r="J34">
-        <v>2.7073351399755086E-2</v>
+        <v>7.5840945195493337E-4</v>
       </c>
       <c r="K34">
-        <v>4.7532518548608807E-2</v>
+        <v>9.6667029200712296E-2</v>
       </c>
       <c r="L34">
-        <v>1.6143679195266492E-2</v>
+        <v>0.40129367431707608</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.35">
@@ -5046,16 +5060,16 @@
         <v>-1.8000000000000016</v>
       </c>
       <c r="I35">
-        <v>5.4682833672723648E-2</v>
+        <v>2.2644265730395862E-4</v>
       </c>
       <c r="J35">
-        <v>3.2068189760577293E-2</v>
+        <v>7.8066147620731163E-4</v>
       </c>
       <c r="K35">
-        <v>6.0749161720556701E-2</v>
+        <v>9.7242697009187348E-2</v>
       </c>
       <c r="L35">
-        <v>2.1537001230033159E-2</v>
+        <v>0.41098963713127024</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.35">
@@ -5063,16 +5077,16 @@
         <v>-1.7000000000000015</v>
       </c>
       <c r="I36">
-        <v>6.5811514016871256E-2</v>
+        <v>2.3456387486377482E-4</v>
       </c>
       <c r="J36">
-        <v>3.8075016121317418E-2</v>
+        <v>8.0370898547799108E-4</v>
       </c>
       <c r="K36">
-        <v>7.6570009734742317E-2</v>
+        <v>9.7760673493863956E-2</v>
       </c>
       <c r="L36">
-        <v>2.8380381049400383E-2</v>
+        <v>0.42074029056089679</v>
       </c>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.35">
@@ -5080,16 +5094,16 @@
         <v>-1.6000000000000014</v>
       </c>
       <c r="I37">
-        <v>7.9303106330023757E-2</v>
+        <v>2.4303149127418637E-4</v>
       </c>
       <c r="J37">
-        <v>4.5309181693160505E-2</v>
+        <v>8.2758579678143818E-4</v>
       </c>
       <c r="K37">
-        <v>9.518007986163346E-2</v>
+        <v>9.8220002361844805E-2</v>
       </c>
       <c r="L37">
-        <v>3.6944069202113072E-2</v>
+        <v>0.43053981679232617</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.35">
@@ -5097,16 +5111,16 @@
         <v>-1.5000000000000013</v>
       </c>
       <c r="I38">
-        <v>9.5631856999947168E-2</v>
+        <v>2.5186273931632137E-4</v>
       </c>
       <c r="J38">
-        <v>5.4030137936078082E-2</v>
+        <v>8.5232740369423077E-4</v>
       </c>
       <c r="K38">
-        <v>0.11668160036602157</v>
+        <v>9.8619832726972223E-2</v>
       </c>
       <c r="L38">
-        <v>4.7512900186882034E-2</v>
+        <v>0.44038230762975733</v>
       </c>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.35">
@@ -5114,16 +5128,16 @@
         <v>-1.4000000000000012</v>
       </c>
       <c r="I39">
-        <v>0.11533490846887444</v>
+        <v>2.6107583593956138E-4</v>
       </c>
       <c r="J39">
-        <v>6.4547974393468432E-2</v>
+        <v>8.7797107176706968E-4</v>
       </c>
       <c r="K39">
-        <v>0.14106771739328908</v>
+        <v>9.8959421736187367E-2</v>
       </c>
       <c r="L39">
-        <v>6.0376691115162584E-2</v>
+        <v>0.45026177516988697</v>
       </c>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.35">
@@ -5131,16 +5145,16 @@
         <v>-1.3000000000000012</v>
       </c>
       <c r="I40">
-        <v>0.13899698174264619</v>
+        <v>2.7069004594597394E-4</v>
       </c>
       <c r="J40">
-        <v>7.7229068980227855E-2</v>
+        <v>9.0455594008875817E-4</v>
       </c>
       <c r="K40">
-        <v>0.16819839635435682</v>
+        <v>9.9238136869252938E-2</v>
       </c>
       <c r="L40">
-        <v>7.5818099411116724E-2</v>
+        <v>0.4601721627229709</v>
       </c>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.35">
@@ -5148,16 +5162,16 @@
         <v>-1.2000000000000011</v>
       </c>
       <c r="I41">
-        <v>0.16721550635297847</v>
+        <v>2.8072575029314045E-4</v>
       </c>
       <c r="J41">
-        <v>9.2499304803588034E-2</v>
+        <v>9.3212312944673803E-4</v>
       </c>
       <c r="K41">
-        <v>0.19778120212145192</v>
+        <v>9.9455457901874281E-2</v>
       </c>
       <c r="L41">
-        <v>9.4098291512360543E-2</v>
+        <v>0.47010735594710512</v>
       </c>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.35">
@@ -5165,16 +5179,16 @@
         <v>-1.100000000000001</v>
       </c>
       <c r="I42">
-        <v>0.20053573830560054</v>
+        <v>2.9120451938725427E-4</v>
       </c>
       <c r="J42">
-        <v>0.11084239711217125</v>
+        <v>9.6071585756402067E-4</v>
       </c>
       <c r="K42">
-        <v>0.2293597060532393</v>
+        <v>9.9610978523690982E-2</v>
       </c>
       <c r="L42">
-        <v>0.11544104856560938</v>
+        <v>0.4800611941616274</v>
       </c>
     </row>
     <row r="43" spans="8:12" x14ac:dyDescent="0.35">
@@ -5182,16 +5196,16 @@
         <v>-1.0000000000000009</v>
       </c>
       <c r="I43">
-        <v>0.23934344697746879</v>
+        <v>3.0214919177136917E-4</v>
       </c>
       <c r="J43">
-        <v>0.1327897166111156</v>
+        <v>9.9037956193170906E-4</v>
       </c>
       <c r="K43">
-        <v>0.26231201537401122</v>
+        <v>9.9704407604095449E-2</v>
       </c>
       <c r="L43">
-        <v>0.1400162001061811</v>
+        <v>0.49002748180476186</v>
       </c>
     </row>
     <row r="44" spans="8:12" x14ac:dyDescent="0.35">
@@ -5199,16 +5213,16 @@
         <v>-0.90000000000000091</v>
       </c>
       <c r="I44">
-        <v>0.28370383266135807</v>
+        <v>3.1358395864985425E-4</v>
       </c>
       <c r="J44">
-        <v>0.15889676819044174</v>
+        <v>1.0211620307984393E-3</v>
       </c>
       <c r="K44">
-        <v>0.29586132286154604</v>
+        <v>9.9735570100358162E-2</v>
       </c>
       <c r="L44">
-        <v>0.1679234992663976</v>
+        <v>0.49999999999999989</v>
       </c>
     </row>
     <row r="45" spans="8:12" x14ac:dyDescent="0.35">
@@ -5216,16 +5230,16 @@
         <v>-0.80000000000000093</v>
       </c>
       <c r="I45">
-        <v>0.33314353279466052</v>
+        <v>3.2553445472984291E-4</v>
       </c>
       <c r="J45">
-        <v>0.18970067882141106</v>
+        <v>1.0531135429236449E-3</v>
       </c>
       <c r="K45">
-        <v>0.32909944888366083</v>
+        <v>9.9704407604095449E-2</v>
       </c>
       <c r="L45">
-        <v>0.19917819908999618</v>
+        <v>0.50997251819523792</v>
       </c>
     </row>
     <row r="46" spans="8:12" x14ac:dyDescent="0.35">
@@ -5233,16 +5247,16 @@
         <v>-0.70000000000000095</v>
       </c>
       <c r="I46">
-        <v>0.38639348936483231</v>
+        <v>3.3802785590409312E-4</v>
       </c>
       <c r="J46">
-        <v>0.22565364994386311</v>
+        <v>1.0862870167527294E-3</v>
       </c>
       <c r="K46">
-        <v>0.361023161474819</v>
+        <v>9.9610978523690996E-2</v>
       </c>
       <c r="L46">
-        <v>0.23369962916910997</v>
+        <v>0.51993880583837238</v>
       </c>
     </row>
     <row r="47" spans="8:12" x14ac:dyDescent="0.35">
@@ -5250,16 +5264,16 @@
         <v>-0.60000000000000098</v>
       </c>
       <c r="I47">
-        <v>0.44114844502398848</v>
+        <v>3.5109298434767423E-4</v>
       </c>
       <c r="J47">
-        <v>0.26703086079299182</v>
+        <v>1.1207381697263541E-3</v>
       </c>
       <c r="K47">
-        <v>0.39058173000049884</v>
+        <v>9.9455457901874281E-2</v>
       </c>
       <c r="L47">
-        <v>0.27130398448337512</v>
+        <v>0.52989264405289471</v>
       </c>
     </row>
     <row r="48" spans="8:12" x14ac:dyDescent="0.35">
@@ -5267,16 +5281,16 @@
         <v>-0.500000000000001</v>
       </c>
       <c r="I48">
-        <v>0.49394968253813593</v>
+        <v>3.6476042165363838E-4</v>
       </c>
       <c r="J48">
-        <v>0.31381938239430635</v>
+        <v>1.1565256884952801E-3</v>
       </c>
       <c r="K48">
-        <v>0.41673284805446192</v>
+        <v>9.9238136869252938E-2</v>
       </c>
       <c r="L48">
-        <v>0.31170231708788843</v>
+        <v>0.53982783727702888</v>
       </c>
     </row>
     <row r="49" spans="8:12" x14ac:dyDescent="0.35">
@@ -5284,16 +5298,16 @@
         <v>-0.40000000000000102</v>
       </c>
       <c r="I49">
-        <v>0.54033731014439135</v>
+        <v>3.790626306909701E-4</v>
       </c>
       <c r="J49">
-        <v>0.36560757076051598</v>
+        <v>1.1937114108799274E-3</v>
       </c>
       <c r="K49">
-        <v>0.43850292359506593</v>
+        <v>9.8959421736187367E-2</v>
       </c>
       <c r="L49">
-        <v>0.35450437574156468</v>
+        <v>0.54973822483011281</v>
       </c>
     </row>
     <row r="50" spans="8:12" x14ac:dyDescent="0.35">
@@ -5301,16 +5315,16 @@
         <v>-0.30000000000000104</v>
       </c>
       <c r="I50">
-        <v>0.57539832144528535</v>
+        <v>3.9403408693210326E-4</v>
       </c>
       <c r="J50">
-        <v>0.42150877521786989</v>
+        <v>1.2323605204815347E-3</v>
       </c>
       <c r="K50">
-        <v>0.45504694401087509</v>
+        <v>9.8619832726972223E-2</v>
       </c>
       <c r="L50">
-        <v>0.39922849533890892</v>
+        <v>0.55961769237024239</v>
       </c>
     </row>
     <row r="51" spans="8:12" x14ac:dyDescent="0.35">
@@ -5318,16 +5332,16 @@
         <v>-0.20000000000000104</v>
       </c>
       <c r="I51">
-        <v>0.59470715122605933</v>
+        <v>4.0971142006786758E-4</v>
       </c>
       <c r="J51">
-        <v>0.48016036015686281</v>
+        <v>1.2725417549344087E-3</v>
       </c>
       <c r="K51">
-        <v>0.46570281238686317</v>
+        <v>9.8220002361844805E-2</v>
       </c>
       <c r="L51">
-        <v>0.4453172388022601</v>
+        <v>0.56946018320767355</v>
       </c>
     </row>
     <row r="52" spans="8:12" x14ac:dyDescent="0.35">
@@ -5335,16 +5349,16 @@
         <v>-0.10000000000000103</v>
       </c>
       <c r="I52">
-        <v>0.59542882121551766</v>
+        <v>4.2613356680561013E-4</v>
       </c>
       <c r="J52">
-        <v>0.53982783727702832</v>
+        <v>1.3143276288702377E-3</v>
       </c>
       <c r="K52">
-        <v>0.47003529342785944</v>
+        <v>9.7760673493863956E-2</v>
       </c>
       <c r="L52">
-        <v>0.49215799108738634</v>
+        <v>0.57925970943910288</v>
       </c>
     </row>
     <row r="53" spans="8:12" x14ac:dyDescent="0.35">
@@ -5352,16 +5366,16 @@
         <v>-1.0269562977782698E-15</v>
       </c>
       <c r="I53">
-        <v>0.57715962684987532</v>
+        <v>4.4334193583221102E-4</v>
       </c>
       <c r="J53">
-        <v>0.59861008809060445</v>
+        <v>1.3577946727624246E-3</v>
       </c>
       <c r="K53">
-        <v>0.46786550543392069</v>
+        <v>9.7242697009187362E-2</v>
       </c>
       <c r="L53">
-        <v>0.5391072542633486</v>
+        <v>0.58901036286872954</v>
       </c>
     </row>
     <row r="54" spans="8:12" x14ac:dyDescent="0.35">
@@ -5369,16 +5383,16 @@
         <v>9.9999999999998979E-2</v>
       </c>
       <c r="I54">
-        <v>0.54210271839214386</v>
+        <v>4.6138058601875501E-4</v>
       </c>
       <c r="J54">
-        <v>0.65469786778660533</v>
+        <v>1.4030236889187586E-3</v>
       </c>
       <c r="K54">
-        <v>0.45928317340728742</v>
+        <v>9.6667029200712296E-2</v>
       </c>
       <c r="L54">
-        <v>0.58551704670180216</v>
+        <v>0.5987063256829237</v>
       </c>
     </row>
     <row r="55" spans="8:12" x14ac:dyDescent="0.35">
@@ -5386,16 +5400,16 @@
         <v>0.19999999999999898</v>
       </c>
       <c r="I55">
-        <v>0.49447256967407777</v>
+        <v>4.8029641904868324E-4</v>
       </c>
       <c r="J55">
-        <v>0.70661049867299153</v>
+        <v>1.4501000260063734E-3</v>
       </c>
       <c r="K55">
-        <v>0.44464047362342363</v>
+        <v>9.6034728826426205E-2</v>
       </c>
       <c r="L55">
-        <v>0.6307616096276677</v>
+        <v>0.60834188084639473</v>
       </c>
     </row>
     <row r="56" spans="8:12" x14ac:dyDescent="0.35">
@@ -5403,16 +5417,16 @@
         <v>0.29999999999999899</v>
       </c>
       <c r="I56">
-        <v>0.43940566781679591</v>
+        <v>5.0013938776761015E-4</v>
       </c>
       <c r="J56">
-        <v>0.75334475505344645</v>
+        <v>1.4991138736132337E-3</v>
       </c>
       <c r="K56">
-        <v>0.42452805815285793</v>
+        <v>9.5346953865131007E-2</v>
       </c>
       <c r="L56">
-        <v>0.67426259492032903</v>
+        <v>0.61791142218895256</v>
       </c>
     </row>
     <row r="57" spans="8:12" x14ac:dyDescent="0.35">
@@ -5420,16 +5434,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="I57">
-        <v>0.38184618915061219</v>
+        <v>5.2096272168181709E-4</v>
       </c>
       <c r="J57">
-        <v>0.79440968148262048</v>
+        <v>1.5501605784903338E-3</v>
       </c>
       <c r="K57">
-        <v>0.39973553396848466</v>
+        <v>9.4604957983454849E-2</v>
       </c>
       <c r="L57">
-        <v>0.71551105270225679</v>
+        <v>0.62740946415328391</v>
       </c>
     </row>
     <row r="58" spans="8:12" x14ac:dyDescent="0.35">
@@ -5437,16 +5451,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="I58">
-        <v>0.32577559423885932</v>
+        <v>5.4282317117530158E-4</v>
       </c>
       <c r="J58">
-        <v>0.82976508640009961</v>
+        <v>1.6033409842656776E-3</v>
       </c>
       <c r="K58">
-        <v>0.37120008122633552</v>
+        <v>9.3810086729234465E-2</v>
       </c>
       <c r="L58">
-        <v>0.75408483827835626</v>
+        <v>0.63683065117561899</v>
       </c>
     </row>
     <row r="59" spans="8:12" x14ac:dyDescent="0.35">
@@ -5454,16 +5468,16 @@
         <v>0.59999999999999898</v>
       </c>
       <c r="I59">
-        <v>0.27390284321552266</v>
+        <v>5.6578127217381724E-4</v>
       </c>
       <c r="J59">
-        <v>0.85970610254397384</v>
+        <v>1.6587617965870827E-3</v>
       </c>
       <c r="K59">
-        <v>0.33994786568104446</v>
+        <v>9.2963773467442223E-2</v>
       </c>
       <c r="L59">
-        <v>0.78966047915550108</v>
+        <v>0.64616976667272374</v>
       </c>
     </row>
     <row r="60" spans="8:12" x14ac:dyDescent="0.35">
@@ -5471,16 +5485,16 @@
         <v>0.69999999999999896</v>
       </c>
       <c r="I60">
-        <v>0.22772309026885401</v>
+        <v>5.8990163316033795E-4</v>
       </c>
       <c r="J60">
-        <v>0.88473649070521498</v>
+        <v>1.7165359758324339E-3</v>
       </c>
       <c r="K60">
-        <v>0.30703333139918837</v>
+        <v>9.2067535075830834E-2</v>
       </c>
       <c r="L60">
-        <v>0.82201903463938053</v>
+        <v>0.65542174161032407</v>
       </c>
     </row>
     <row r="61" spans="8:12" x14ac:dyDescent="0.35">
@@ -5488,16 +5502,16 @@
         <v>0.79999999999999893</v>
       </c>
       <c r="I61">
-        <v>0.18777406465475951</v>
+        <v>6.1525324664212812E-4</v>
       </c>
       <c r="J61">
-        <v>0.90545912867964717</v>
+        <v>1.7767831597259032E-3</v>
       </c>
       <c r="K61">
-        <v>0.27348132826957205</v>
+        <v>9.1122967418376624E-2</v>
       </c>
       <c r="L61">
-        <v>0.8510459871231203</v>
+        <v>0.66458166262983043</v>
       </c>
     </row>
     <row r="62" spans="8:12" x14ac:dyDescent="0.35">
@@ -5505,16 +5519,16 @@
         <v>0.89999999999999891</v>
       </c>
       <c r="I62">
-        <v>0.15394269159729695</v>
+        <v>6.4190982738727758E-4</v>
       </c>
       <c r="J62">
-        <v>0.92249563844821658</v>
+        <v>1.8396301184185337E-3</v>
       </c>
       <c r="K62">
-        <v>0.2402363860289409</v>
+        <v>9.0131740615411987E-2</v>
       </c>
       <c r="L62">
-        <v>0.87672567135600432</v>
+        <v>0.67364477971207992</v>
       </c>
     </row>
     <row r="63" spans="8:12" x14ac:dyDescent="0.35">
@@ -5522,16 +5536,16 @@
         <v>0.99999999999999889</v>
       </c>
       <c r="I63">
-        <v>0.12573535723614146</v>
+        <v>6.6995017999100018E-4</v>
       </c>
       <c r="J63">
-        <v>0.93643532470665591</v>
+        <v>1.9052112448371128E-3</v>
       </c>
       <c r="K63">
-        <v>0.20812240753154615</v>
+        <v>8.9095594130045822E-2</v>
       </c>
       <c r="L63">
-        <v>0.89913112989631394</v>
+        <v>0.6826065133587409</v>
       </c>
     </row>
     <row r="64" spans="8:12" x14ac:dyDescent="0.35">
@@ -5539,16 +5553,16 @@
         <v>1.099999999999999</v>
       </c>
       <c r="I64">
-        <v>0.10247924379988503</v>
+        <v>6.9945859860222055E-4</v>
       </c>
       <c r="J64">
-        <v>0.9478077952472802</v>
+        <v>1.9736690833725423E-3</v>
       </c>
       <c r="K64">
-        <v>0.17781477557172073</v>
+        <v>8.8016331691074867E-2</v>
       </c>
       <c r="L64">
-        <v>0.91841054758371254</v>
+        <v>0.69146246127401301</v>
       </c>
     </row>
     <row r="65" spans="8:12" x14ac:dyDescent="0.35">
@@ -5556,16 +5570,16 @@
         <v>1.1999999999999991</v>
       </c>
       <c r="I65">
-        <v>8.3454771452459969E-2</v>
+        <v>7.3052530194237528E-4</v>
       </c>
       <c r="J65">
-        <v>0.95707218903654212</v>
+        <v>2.0451549002782343E-3</v>
       </c>
       <c r="K65">
-        <v>0.14982552236305358</v>
+        <v>8.6895816073087023E-2</v>
       </c>
       <c r="L65">
-        <v>0.93477154988264299</v>
+        <v>0.70020840453130395</v>
       </c>
     </row>
     <row r="66" spans="8:12" x14ac:dyDescent="0.35">
@@ -5573,16 +5587,16 @@
         <v>1.2999999999999992</v>
       </c>
       <c r="I66">
-        <v>6.7973055423371204E-2</v>
+        <v>7.6324690708499672E-4</v>
       </c>
       <c r="J66">
-        <v>0.96461676084963277</v>
+        <v>2.1198292994776269E-3</v>
       </c>
       <c r="K66">
-        <v>0.12450096132240532</v>
+        <v>8.5735963754845962E-2</v>
       </c>
       <c r="L66">
-        <v>0.9484646509808301</v>
+        <v>0.70884031321165353</v>
       </c>
     </row>
     <row r="67" spans="8:12" x14ac:dyDescent="0.35">
@@ -5590,16 +5604,16 @@
         <v>1.3999999999999992</v>
       </c>
       <c r="I67">
-        <v>5.5414890241784878E-2</v>
+        <v>7.9772694584083915E-4</v>
       </c>
       <c r="J67">
-        <v>0.97076415638537239</v>
+        <v>2.197862887846902E-3</v>
       </c>
       <c r="K67">
-        <v>0.10203015791040425</v>
+        <v>8.4538739477327859E-2</v>
       </c>
       <c r="L67">
-        <v>0.95976702402819636</v>
+        <v>0.71735435150279925</v>
       </c>
     </row>
     <row r="68" spans="8:12" x14ac:dyDescent="0.35">
@@ -5607,16 +5621,16 @@
         <v>1.4999999999999993</v>
       </c>
       <c r="I68">
-        <v>4.5245345804669039E-2</v>
+        <v>8.3407642801426054E-4</v>
       </c>
       <c r="J68">
-        <v>0.97577926447744701</v>
+        <v>2.2794369944418302E-3</v>
       </c>
       <c r="K68">
-        <v>8.2461904818584827E-2</v>
+        <v>8.3306150722949904E-2</v>
       </c>
       <c r="L68">
-        <v>0.96896756518996463</v>
+        <v>0.72574688224992634</v>
       </c>
     </row>
     <row r="69" spans="8:12" x14ac:dyDescent="0.35">
@@ -5624,16 +5638,16 @@
         <v>1.5999999999999994</v>
       </c>
       <c r="I69">
-        <v>3.7014277081999572E-2</v>
+        <v>8.7241445626796076E-4</v>
       </c>
       <c r="J69">
-        <v>0.97987775432362723</v>
+        <v>2.3647444485889735E-3</v>
       </c>
       <c r="K69">
-        <v>6.5727500316870441E-2</v>
+        <v>8.2040242137593769E-2</v>
       </c>
       <c r="L69">
-        <v>0.97635396851130229</v>
+        <v>0.73401447095129935</v>
       </c>
     </row>
     <row r="70" spans="8:12" x14ac:dyDescent="0.35">
@@ -5641,16 +5655,16 @@
         <v>1.6999999999999995</v>
       </c>
       <c r="I70">
-        <v>3.0349578854128156E-2</v>
+        <v>9.128688978616771E-4</v>
       </c>
       <c r="J70">
-        <v>0.98323425636184081</v>
+        <v>2.453990422261354E-3</v>
       </c>
       <c r="K70">
-        <v>5.16665923868425E-2</v>
+        <v>8.0743089916978567E-2</v>
       </c>
       <c r="L70">
-        <v>0.98220225408289652</v>
+        <v>0.74215388919413527</v>
       </c>
     </row>
     <row r="71" spans="8:12" x14ac:dyDescent="0.35">
@@ -5658,16 +5672,16 @@
         <v>1.7999999999999996</v>
       </c>
       <c r="I71">
-        <v>2.4947380161910032E-2</v>
+        <v>9.5557711912347377E-4</v>
       </c>
       <c r="J71">
-        <v>0.98598968932458764</v>
+        <v>2.547393342712756E-3</v>
       </c>
       <c r="K71">
-        <v>4.0053592212178295E-2</v>
+        <v>7.9416796178787052E-2</v>
       </c>
       <c r="L71">
-        <v>0.9867689282952028</v>
+        <v>0.75016211752822293</v>
       </c>
     </row>
     <row r="72" spans="8:12" x14ac:dyDescent="0.35">
@@ -5675,16 +5689,16 @@
         <v>1.8999999999999997</v>
       </c>
       <c r="I72">
-        <v>2.0561569352483568E-2</v>
+        <v>1.0006867891784866E-3</v>
       </c>
       <c r="J72">
-        <v>0.98825755897140199</v>
+        <v>2.6451858819647178E-3</v>
       </c>
       <c r="K72">
-        <v>3.0622600914242487E-2</v>
+        <v>7.8063483341690304E-2</v>
       </c>
       <c r="L72">
-        <v>0.9902857260411948</v>
+        <v>0.75803634777692697</v>
       </c>
     </row>
     <row r="73" spans="8:12" x14ac:dyDescent="0.35">
@@ -5692,16 +5706,16 @@
         <v>1.9999999999999998</v>
       </c>
       <c r="I73">
-        <v>1.6993892996149909E-2</v>
+        <v>1.0483567602092266E-3</v>
       </c>
       <c r="J73">
-        <v>0.99012923108926487</v>
+        <v>2.7476160304289454E-3</v>
       </c>
       <c r="K73">
-        <v>2.3089345732782745E-2</v>
+        <v>7.6685288532059998E-2</v>
       </c>
       <c r="L73">
-        <v>0.99295670616128739</v>
+        <v>0.76577398478730496</v>
       </c>
     </row>
     <row r="74" spans="8:12" x14ac:dyDescent="0.35">
@@ -5709,16 +5723,16 @@
         <v>2.0999999999999996</v>
       </c>
       <c r="I74">
-        <v>1.4085184456303192E-2</v>
+        <v>1.0987580323649731E-3</v>
       </c>
       <c r="J74">
-        <v>0.99167826820763394</v>
+        <v>2.8549482627171496E-3</v>
       </c>
       <c r="K74">
-        <v>1.7169202732841192E-2</v>
+        <v>7.5284358038701094E-2</v>
       </c>
       <c r="L74">
-        <v>0.99495735016618658</v>
+        <v>0.77337264762313174</v>
       </c>
     </row>
     <row r="75" spans="8:12" x14ac:dyDescent="0.35">
@@ -5726,16 +5740,16 @@
         <v>2.1999999999999997</v>
       </c>
       <c r="I75">
-        <v>1.1707890250092369E-2</v>
+        <v>1.1520748123883687E-3</v>
       </c>
       <c r="J75">
-        <v>0.99296395371698609</v>
+        <v>2.9674648045471264E-3</v>
       </c>
       <c r="K75">
-        <v>1.2590923362052458E-2</v>
+        <v>7.3862841835390741E-2</v>
       </c>
       <c r="L75">
-        <v>0.99643524956985763</v>
+        <v>0.78083017020662249</v>
       </c>
     </row>
     <row r="76" spans="8:12" x14ac:dyDescent="0.35">
@@ -5743,16 +5757,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I76">
-        <v>9.7598597336093773E-3</v>
+        <v>1.2085056760998375E-3</v>
       </c>
       <c r="J76">
-        <v>0.99403413258985318</v>
+        <v>3.085467010615961E-3</v>
       </c>
       <c r="K76">
-        <v>9.106132848932677E-3</v>
+        <v>7.2422888190370682E-2</v>
       </c>
       <c r="L76">
-        <v>0.99751195232230505</v>
+        <v>0.78814460141660314</v>
       </c>
     </row>
     <row r="77" spans="8:12" x14ac:dyDescent="0.35">
@@ -5760,16 +5774,16 @@
         <v>2.4</v>
       </c>
       <c r="I77">
-        <v>8.1592698982939811E-3</v>
+        <v>1.2682648460918813E-3</v>
       </c>
       <c r="J77">
-        <v>0.99492748909742335</v>
+        <v>3.2092768643814384E-3</v>
       </c>
       <c r="K77">
-        <v>6.4950026568476515E-3</v>
+        <v>7.0966638381221817E-2</v>
       </c>
       <c r="L77">
-        <v>0.99828556336816709</v>
+        <v>0.79531420465274738</v>
       </c>
     </row>
     <row r="78" spans="8:12" x14ac:dyDescent="0.35">
@@ -5777,16 +5791,16 @@
         <v>2.5</v>
       </c>
       <c r="I78">
-        <v>6.8405242152831357E-3</v>
+        <v>1.3315835973552292E-3</v>
       </c>
       <c r="J78">
-        <v>0.99567536708715021</v>
+        <v>3.3392386118973882E-3</v>
       </c>
       <c r="K78">
-        <v>4.568710441179645E-3</v>
+        <v>6.9496221532749106E-2</v>
       </c>
       <c r="L78">
-        <v>0.9988337461459853</v>
+        <v>0.80233745687730762</v>
       </c>
     </row>
     <row r="79" spans="8:12" x14ac:dyDescent="0.35">
@@ -5794,16 +5808,16 @@
         <v>2.6</v>
       </c>
       <c r="I79">
-        <v>5.7509635581052959E-3</v>
+        <v>1.3987118051098106E-3</v>
       </c>
       <c r="J79">
-        <v>0.99630322205337885</v>
+        <v>3.4757205431962257E-3</v>
       </c>
       <c r="K79">
-        <v>3.1693987659461372E-3</v>
+        <v>6.8013749594635867E-2</v>
       </c>
       <c r="L79">
-        <v>0.99921683895094049</v>
+        <v>0.80921304714748943</v>
       </c>
     </row>
     <row r="80" spans="8:12" x14ac:dyDescent="0.35">
@@ -5811,16 +5825,16 @@
         <v>2.7</v>
       </c>
       <c r="I80">
-        <v>4.8482414581218526E-3</v>
+        <v>1.4699196508715442E-3</v>
       </c>
       <c r="J80">
-        <v>0.99683177866878769</v>
+        <v>3.6191169362248532E-3</v>
       </c>
       <c r="K80">
-        <v>2.168348504415149E-3</v>
+        <v>6.6521312474688704E-2</v>
       </c>
       <c r="L80">
-        <v>0.99948087211676628</v>
+        <v>0.81593987465324047</v>
       </c>
     </row>
     <row r="81" spans="8:12" x14ac:dyDescent="0.35">
@@ -5828,16 +5842,16 @@
         <v>2.8000000000000003</v>
       </c>
       <c r="I81">
-        <v>4.0982359455794416E-3</v>
+        <v>1.5454995047810504E-3</v>
       </c>
       <c r="J81">
-        <v>0.99727795364724292</v>
+        <v>3.7698501800405571E-3</v>
       </c>
       <c r="K81">
-        <v>1.463019904504783E-3</v>
+        <v>6.5020973342498914E-2</v>
       </c>
       <c r="L81">
-        <v>0.99966034087037814</v>
+        <v>0.82251704627676769</v>
       </c>
     </row>
     <row r="82" spans="8:12" x14ac:dyDescent="0.35">
@@ -5845,16 +5859,16 @@
         <v>2.9000000000000004</v>
       </c>
       <c r="I82">
-        <v>3.4733910783840906E-3</v>
+        <v>1.6257680044873617E-3</v>
       </c>
       <c r="J82">
-        <v>0.9976555920820569</v>
+        <v>3.9283730958890595E-3</v>
       </c>
       <c r="K82">
-        <v>9.7350981505563302E-4</v>
+        <v>6.3514764117297243E-2</v>
       </c>
       <c r="L82">
-        <v>0.9997806490298029</v>
+        <v>0.82894387369151823</v>
       </c>
     </row>
     <row r="83" spans="8:12" x14ac:dyDescent="0.35">
@@ -5862,16 +5876,16 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="I83">
-        <v>2.9514005876051532E-3</v>
+        <v>1.7110683534587493E-3</v>
       </c>
       <c r="J83">
-        <v>0.99797605569841419</v>
+        <v>4.0951714769393299E-3</v>
       </c>
       <c r="K83">
-        <v>6.3885071313540126E-4</v>
+        <v>6.2004681152684267E-2</v>
       </c>
       <c r="L83">
-        <v>0.99986018749144967</v>
+        <v>0.83521987001968956</v>
       </c>
     </row>
     <row r="84" spans="8:12" x14ac:dyDescent="0.35">
@@ -5879,16 +5893,16 @@
         <v>3.1000000000000005</v>
       </c>
       <c r="I84">
-        <v>2.5141629147183366E-3</v>
+        <v>1.8017728645304777E-3</v>
       </c>
       <c r="J84">
-        <v>0.99824869356626755</v>
+        <v>4.2707668698832579E-3</v>
       </c>
       <c r="K84">
-        <v>4.1345417627405937E-4</v>
+        <v>6.0492681129785834E-2</v>
       </c>
       <c r="L84">
-        <v>0.99991204780711773</v>
+        <v>0.84134474606854281</v>
       </c>
     </row>
     <row r="85" spans="8:12" x14ac:dyDescent="0.35">
@@ -5896,16 +5910,16 @@
         <v>3.2000000000000006</v>
       </c>
       <c r="I85">
-        <v>2.1469510690586085E-3</v>
+        <v>1.8982857778500318E-3</v>
       </c>
       <c r="J85">
-        <v>0.99848121947733492</v>
+        <v>4.4557196243518171E-3</v>
       </c>
       <c r="K85">
-        <v>2.6389084995445336E-4</v>
+        <v>5.8980677169218128E-2</v>
       </c>
       <c r="L85">
-        <v>0.9999453957451081</v>
+        <v>0.84731840616688969</v>
       </c>
     </row>
     <row r="86" spans="8:12" x14ac:dyDescent="0.35">
@@ -5913,16 +5927,16 @@
         <v>3.3000000000000007</v>
       </c>
       <c r="I86">
-        <v>1.8377523482641029E-3</v>
+        <v>2.001046386206776E-3</v>
       </c>
       <c r="J86">
-        <v>0.99868001513339677</v>
+        <v>4.6506322392025901E-3</v>
       </c>
       <c r="K86">
-        <v>1.6610787810491804E-4</v>
+        <v>5.7470535171058233E-2</v>
       </c>
       <c r="L86">
-        <v>0.99996654420133968</v>
+        <v>0.85314094362410409</v>
       </c>
     </row>
     <row r="87" spans="8:12" x14ac:dyDescent="0.35">
@@ -5930,16 +5944,16 @@
         <v>3.4000000000000008</v>
       </c>
       <c r="I87">
-        <v>1.5767423466555525E-3</v>
+        <v>2.1105325051088749E-3</v>
       </c>
       <c r="J87">
-        <v>0.99885037428363677</v>
+        <v>4.8561530382466578E-3</v>
       </c>
       <c r="K87">
-        <v>1.0311576754162756E-4</v>
+        <v>5.5964070390809847E-2</v>
       </c>
       <c r="L87">
-        <v>0.99997977128828142</v>
+        <v>0.85881263583487111</v>
       </c>
     </row>
     <row r="88" spans="8:12" x14ac:dyDescent="0.35">
@@ -5947,16 +5961,16 @@
         <v>3.5000000000000009</v>
       </c>
       <c r="I88">
-        <v>1.3558651751259989E-3</v>
+        <v>2.2272643299805282E-3</v>
       </c>
       <c r="J88">
-        <v>0.99899669978044936</v>
+        <v>5.0729802119631739E-3</v>
       </c>
       <c r="K88">
-        <v>6.3128995187286524E-5</v>
+        <v>5.4463044258137625E-2</v>
       </c>
       <c r="L88">
-        <v>0.99998793007523878</v>
+        <v>0.86433393905361733</v>
       </c>
     </row>
     <row r="89" spans="8:12" x14ac:dyDescent="0.35">
@@ -5964,16 +5978,16 @@
         <v>3.600000000000001</v>
       </c>
       <c r="I89">
-        <v>1.1684977660526561E-3</v>
+        <v>2.3518087285976808E-3</v>
       </c>
       <c r="J89">
-        <v>0.99912266302459396</v>
+        <v>5.3018662662685512E-3</v>
       </c>
       <c r="K89">
-        <v>3.8115500288447229E-5</v>
+        <v>5.2969161443924849E-2</v>
       </c>
       <c r="L89">
-        <v>0.99999289328717444</v>
+        <v>0.86970548286319116</v>
       </c>
     </row>
     <row r="90" spans="8:12" x14ac:dyDescent="0.35">
@@ -5981,16 +5995,16 @@
         <v>3.7000000000000011</v>
       </c>
       <c r="I90">
-        <v>1.0091808349999151E-3</v>
+        <v>2.4847840234761783E-3</v>
       </c>
       <c r="J90">
-        <v>0.99923133330214875</v>
+        <v>5.5436229245410251E-3</v>
       </c>
       <c r="K90">
-        <v>2.2695686401474357E-5</v>
+        <v>5.148406717999366E-2</v>
       </c>
       <c r="L90">
-        <v>0.99999587095251719</v>
+        <v>0.87492806436284987</v>
       </c>
     </row>
     <row r="91" spans="8:12" x14ac:dyDescent="0.35">
@@ -5998,16 +6012,16 @@
         <v>3.8000000000000012</v>
       </c>
       <c r="I91">
-        <v>8.7340276935282755E-4</v>
+        <v>2.6268653265101582E-3</v>
       </c>
       <c r="J91">
-        <v>0.99932528296521794</v>
+        <v>5.799126534942689E-3</v>
       </c>
       <c r="K91">
-        <v>1.3327661967599159E-5</v>
+        <v>5.0009344834621924E-2</v>
       </c>
       <c r="L91">
-        <v>0.99999763278569898</v>
+        <v>0.88000264210098744</v>
       </c>
     </row>
     <row r="92" spans="8:12" x14ac:dyDescent="0.35">
@@ -6015,16 +6029,16 @@
         <v>3.9000000000000012</v>
       </c>
       <c r="I92">
-        <v>7.574256199980884E-4</v>
+        <v>2.7787904968896416E-3</v>
       </c>
       <c r="J92">
-        <v>0.99940667318650722</v>
+        <v>6.069324041737989E-3</v>
       </c>
       <c r="K92">
-        <v>7.7185116848182121E-6</v>
+        <v>4.8546513745803224E-2</v>
       </c>
       <c r="L92">
-        <v>0.99999866087185763</v>
+        <v>0.88493032977829178</v>
       </c>
     </row>
     <row r="93" spans="8:12" x14ac:dyDescent="0.35">
@@ -6032,16 +6046,16 @@
         <v>4.0000000000000009</v>
       </c>
       <c r="I93">
-        <v>6.5814465358202286E-4</v>
+        <v>2.9413668033931731E-3</v>
       </c>
       <c r="J93">
-        <v>0.99947732405415812</v>
+        <v>6.3552395869005962E-3</v>
       </c>
       <c r="K93">
-        <v>4.4084113568267356E-6</v>
+        <v>4.7097027313031573E-2</v>
       </c>
       <c r="L93">
-        <v>0.99999925252893296</v>
+        <v>0.88971238974714872</v>
       </c>
     </row>
     <row r="94" spans="8:12" x14ac:dyDescent="0.35">
@@ -6049,16 +6063,16 @@
         <v>4.1000000000000005</v>
       </c>
       <c r="I94">
-        <v>5.7297471375401332E-4</v>
+        <v>3.11547838377419E-3</v>
       </c>
       <c r="J94">
-        <v>0.99953877201214625</v>
+        <v>6.6579818169792415E-3</v>
       </c>
       <c r="K94">
-        <v>2.4831308687302349E-6</v>
+        <v>4.5662271347255458E-2</v>
       </c>
       <c r="L94">
-        <v>0.99999958833337033</v>
+        <v>0.89435022633314476</v>
       </c>
     </row>
     <row r="95" spans="8:12" x14ac:dyDescent="0.35">
@@ -6066,16 +6080,16 @@
         <v>4.2</v>
       </c>
       <c r="I95">
-        <v>4.9975804626297467E-4</v>
+        <v>3.3020946073983762E-3</v>
       </c>
       <c r="J95">
-        <v>0.99959231704952622</v>
+        <v>6.9787519801180475E-3</v>
       </c>
       <c r="K95">
-        <v>1.3793867654802345E-6</v>
+        <v>4.4243562677544909E-2</v>
       </c>
       <c r="L95">
-        <v>0.99999977629907244</v>
+        <v>0.89884537900441408</v>
       </c>
     </row>
     <row r="96" spans="8:12" x14ac:dyDescent="0.35">
@@ -6083,16 +6097,16 @@
         <v>4.3</v>
       </c>
       <c r="I96">
-        <v>4.3668934832442088E-4</v>
+        <v>3.5022794628494416E-3</v>
       </c>
       <c r="J96">
-        <v>0.99963906156478877</v>
+        <v>7.31885290950407E-3</v>
       </c>
       <c r="K96">
-        <v>7.5568612893329128E-7</v>
+        <v>4.2842148011951832E-2</v>
       </c>
       <c r="L96">
-        <v>0.99999988006304719</v>
+        <v>0.9031995154143897</v>
       </c>
     </row>
     <row r="97" spans="8:12" x14ac:dyDescent="0.35">
@@ -6100,16 +6114,16 @@
         <v>4.3999999999999995</v>
       </c>
       <c r="I97">
-        <v>3.8225467277555944E-4</v>
+        <v>3.7172021102631963E-3</v>
       </c>
       <c r="J97">
-        <v>0.99967994245286662</v>
+        <v>7.6796990025644885E-3</v>
       </c>
       <c r="K97">
-        <v>4.0828722933091742E-7</v>
+        <v>4.1459203049026172E-2</v>
       </c>
       <c r="L97">
-        <v>0.99999993655549446</v>
+        <v>0.90741442434320507</v>
       </c>
     </row>
     <row r="98" spans="8:12" x14ac:dyDescent="0.35">
@@ -6117,16 +6131,16 @@
         <v>4.4999999999999991</v>
       </c>
       <c r="I98">
-        <v>3.3518150336470754E-4</v>
+        <v>3.9481487591000912E-3</v>
       </c>
       <c r="J98">
-        <v>0.99971575766102583</v>
+        <v>8.0628273202341671E-3</v>
       </c>
       <c r="K98">
-        <v>2.1755000176195073E-7</v>
+        <v>4.0095831835479899E-2</v>
       </c>
       <c r="L98">
-        <v>0.99999996688811787</v>
+        <v>0.91149200856259793</v>
       </c>
     </row>
     <row r="99" spans="8:12" x14ac:dyDescent="0.35">
@@ -6134,16 +6148,16 @@
         <v>4.5999999999999988</v>
       </c>
       <c r="I99">
-        <v>2.943978590340524E-4</v>
+        <v>4.1965360564283453E-3</v>
       </c>
       <c r="J99">
-        <v>0.9997471882196507</v>
+        <v>8.4699099478720008E-3</v>
       </c>
       <c r="K99">
-        <v>1.1431976841681189E-7</v>
+        <v>3.8753066364573305E-2</v>
       </c>
       <c r="L99">
-        <v>0.99999998295032966</v>
+        <v>0.91543427764866436</v>
       </c>
     </row>
     <row r="100" spans="8:12" x14ac:dyDescent="0.35">
@@ -6151,16 +6165,16 @@
         <v>4.6999999999999984</v>
       </c>
       <c r="I100">
-        <v>2.5899871342338073E-4</v>
+        <v>4.4639261991581856E-3</v>
       </c>
       <c r="J100">
-        <v>0.99977481656196399</v>
+        <v>8.9027677792944959E-3</v>
       </c>
       <c r="K100">
-        <v>5.9245112786729675E-8</v>
+        <v>3.7431866408936226E-2</v>
       </c>
       <c r="L100">
-        <v>0.99999999133867901</v>
+        <v>0.91924334076622882</v>
       </c>
     </row>
     <row r="101" spans="8:12" x14ac:dyDescent="0.35">
@@ -6168,16 +6182,16 @@
         <v>4.799999999999998</v>
       </c>
       <c r="I101">
-        <v>2.2821835536683484E-4</v>
+        <v>4.7520440167479238E-3</v>
       </c>
       <c r="J101">
-        <v>0.99979914179298124</v>
+        <v>9.3633859083501192E-3</v>
       </c>
       <c r="K101">
-        <v>3.0279777172615305E-8</v>
+        <v>3.6133119580733238E-2</v>
       </c>
       <c r="L101">
-        <v>0.99999999565907394</v>
+        <v>0.92292139944792806</v>
       </c>
     </row>
     <row r="102" spans="8:12" x14ac:dyDescent="0.35">
@@ -6185,16 +6199,16 @@
         <v>4.8999999999999977</v>
       </c>
       <c r="I102">
-        <v>2.0140758585771506E-4</v>
+        <v>5.0627963095296429E-3</v>
       </c>
       <c r="J102">
-        <v>0.99982059244457355</v>
+        <v>9.8539308389918312E-3</v>
       </c>
       <c r="K102">
-        <v>1.5262362659051862E-8</v>
+        <v>3.4857641611340084E-2</v>
       </c>
       <c r="L102">
-        <v>0.99999999785362736</v>
+        <v>0.9264707403903516</v>
       </c>
     </row>
     <row r="103" spans="8:12" x14ac:dyDescent="0.35">
@@ -6202,16 +6216,16 @@
         <v>4.9999999999999973</v>
       </c>
       <c r="I103">
-        <v>1.7801486164813004E-4</v>
+        <v>5.3982937729660481E-3</v>
       </c>
       <c r="J103">
-        <v>0.99983953715420237</v>
+        <v>1.0376769755518545E-2</v>
       </c>
       <c r="K103">
-        <v>7.5868205629954428E-9</v>
+        <v>3.3606176842019796E-2</v>
       </c>
       <c r="L103">
-        <v>0.99999999895299929</v>
+        <v>0.9298937282887767</v>
       </c>
     </row>
   </sheetData>
@@ -6224,8 +6238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71F1E49-69B3-41E4-B5F7-85CA4F6581D0}">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -6238,7 +6252,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
@@ -6262,7 +6276,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -6271,7 +6285,7 @@
       </c>
       <c r="C6" s="2" cm="1">
         <f t="array" ref="C6">_xll.\VARIATE.JOHNSON(gamma, delta, lambda, xi)</f>
-        <v>2046863983184</v>
+        <v>2541175990896</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -6280,7 +6294,7 @@
       </c>
       <c r="C7" s="5" cm="1">
         <f t="array" ref="C7">_xll.JOHNSON.MOMENT(Johnson,1)</f>
-        <v>100.03302941027492</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
@@ -6289,7 +6303,7 @@
       </c>
       <c r="C8" s="5" cm="1">
         <f t="array" ref="C8">_xll.JOHNSON.MOMENT(Johnson,2) - mean^2</f>
-        <v>0.12965566769526049</v>
+        <v>3.1945280494255712E-2</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
@@ -6298,7 +6312,7 @@
       </c>
       <c r="C9" s="5">
         <f>mean</f>
-        <v>100.03302941027492</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
@@ -6307,7 +6321,7 @@
       </c>
       <c r="C10" s="5">
         <f>SQRT(variance)</f>
-        <v>0.36007730794269788</v>
+        <v>0.17873242709216397</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
@@ -6316,7 +6330,7 @@
       </c>
       <c r="C11" s="5">
         <f>f</f>
-        <v>100.03302941027492</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
@@ -6325,7 +6339,7 @@
       </c>
       <c r="C12" s="5" cm="1">
         <f t="array" ref="C12">_xll.NORMAL.PUT.VALUE(f, s, k)</f>
-        <v>14.292496918495097</v>
+        <v>7.1209126309667425</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
@@ -6334,7 +6348,7 @@
       </c>
       <c r="C13" s="5" cm="1">
         <f t="array" ref="C13">_xll.NORMAL.PUT.DELTA(f, s, k)</f>
-        <v>-0.42856111125118518</v>
+        <v>-0.46439543684516627</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
@@ -6343,7 +6357,7 @@
       </c>
       <c r="C14" s="5" cm="1">
         <f t="array" ref="C14">_xll.NORMAL.PUT.IMPLIED(f, value, k)</f>
-        <v>0.36007730794269727</v>
+        <v>0.1787324268788342</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
@@ -6352,7 +6366,7 @@
       </c>
       <c r="C15" s="5" cm="1">
         <f t="array" ref="C15">_xll.JOHNSON.PUT.VALUE(Johnson,k)</f>
-        <v>-5205.8183162309806</v>
+        <v>5.6278234348496881E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>